<commit_message>
REalistic data in experiment
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\MIDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095D734D-65B4-4FDA-B031-67B925C38272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7977DF2-854B-4D81-8F93-8825831B6392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="1680" yWindow="45" windowWidth="27120" windowHeight="15600" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$M$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -119,33 +120,126 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+  <si>
+    <t>sam</t>
+  </si>
+  <si>
+    <t>germ_l</t>
+  </si>
+  <si>
+    <t>Dict</t>
+  </si>
+  <si>
+    <t>Key1</t>
+  </si>
+  <si>
+    <t>Key2</t>
+  </si>
+  <si>
+    <t>slice</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>germ</t>
+  </si>
+  <si>
+    <t>pgr</t>
+  </si>
+  <si>
+    <t>pgr_l</t>
+  </si>
+  <si>
+    <t>Germ low</t>
+  </si>
+  <si>
+    <t>Germ high</t>
+  </si>
+  <si>
+    <t>Lmu 0 Germ low</t>
+  </si>
+  <si>
+    <t>Lmu 0 Germ high</t>
+  </si>
+  <si>
+    <t>Lmu 1 Germ low</t>
+  </si>
+  <si>
+    <t>Lmu 1 Germ high</t>
+  </si>
+  <si>
+    <t>Lmu 2 Germ high</t>
+  </si>
+  <si>
+    <t>Lmu 3 Germ low</t>
+  </si>
+  <si>
+    <t>Lmu 3 Germ high</t>
+  </si>
+  <si>
+    <t>Lmu 40 Germ low</t>
+  </si>
+  <si>
+    <t>Lmu 4 Germ high</t>
+  </si>
+  <si>
+    <t>Lmu 2 Germ low</t>
+  </si>
+  <si>
+    <t>PGR low</t>
+  </si>
+  <si>
+    <t>PGR high</t>
+  </si>
+  <si>
+    <t>Lmu 0 PGR low</t>
+  </si>
+  <si>
+    <t>Lmu 0 PGR high</t>
+  </si>
+  <si>
+    <t>Lmu 1 PGR low</t>
+  </si>
+  <si>
+    <t>Lmu 1 PGR high</t>
+  </si>
+  <si>
+    <t>Lmu 2 PGR low</t>
+  </si>
+  <si>
+    <t>Lmu 2 PGR high</t>
+  </si>
+  <si>
+    <t>Lmu 3 PGR low</t>
+  </si>
+  <si>
+    <t>Lmu 3 PGR high</t>
+  </si>
+  <si>
+    <t>Lmu 40 PGR low</t>
+  </si>
+  <si>
+    <t>Lmu 4 PGR high</t>
+  </si>
   <si>
     <t>0:1</t>
   </si>
   <si>
-    <t>sam</t>
-  </si>
-  <si>
-    <t>germ_l</t>
-  </si>
-  <si>
-    <t>Dict</t>
-  </si>
-  <si>
-    <t>Key1</t>
-  </si>
-  <si>
-    <t>Key2</t>
-  </si>
-  <si>
-    <t>slice</t>
-  </si>
-  <si>
-    <t>annual</t>
-  </si>
-  <si>
-    <t>Default</t>
+    <t>1:2</t>
+  </si>
+  <si>
+    <t>2:3</t>
+  </si>
+  <si>
+    <t>3:4</t>
+  </si>
+  <si>
+    <t>4:5</t>
   </si>
 </sst>
 </file>
@@ -200,12 +294,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -214,6 +305,15 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -530,69 +630,1223 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="17.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="B5">
-        <f>IF(B1="sam",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <f>IF(OR(B1="sam",B1="sai"),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:M5" si="0">IF(OR(C1="sam",C1="sai"),1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="B6">
+        <v>0.9</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.9</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.9</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0.9</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0.9</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0.9</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0.9</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0.9</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0.9</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0.9</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>0.9</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A4:M5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add pyomo component deletions so that multiple trials can be done
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B42340-B616-467E-AD0B-CDCF488889D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D02A2A-602C-4701-9E89-079EDBF19AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -325,17 +325,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -662,7 +652,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,7 +881,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
add multiprocessing, fixed up control.py, changes to exp
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D02A2A-602C-4701-9E89-079EDBF19AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EE0E92-2337-4A7C-83C5-30564CD33E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -652,7 +652,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,13 +881,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>1</v>

</xml_diff>

<commit_message>
updated pasture module with linked changes
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\MIDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EE0E92-2337-4A7C-83C5-30564CD33E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B134E351-773D-44A3-BA6C-873FAE1879DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="2436" yWindow="84" windowWidth="15456" windowHeight="11424" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -649,10 +649,10 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A6:A7"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,7 +881,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
@@ -969,7 +969,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>14</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>16</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>22</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>17</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>18</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>19</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>20</v>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>21</v>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>23</v>
@@ -1453,7 +1453,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>24</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
added back updated version of exp.xl and made a few changes to pas pyomo (still more needed) - model now working
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\MIDAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B134E351-773D-44A3-BA6C-873FAE1879DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482FA613-82F6-4ED5-B002-7E00E2EE1599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2436" yWindow="84" windowWidth="15456" windowHeight="11424" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$4:$N$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$O$5</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1" iterateCount="1" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
     <author>Michael Young</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{3BDB7BEB-FC53-4975-ADDB-A81C02A033DC}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{3BDB7BEB-FC53-4975-ADDB-A81C02A033DC}">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{7875E08E-43A6-4F76-BAD2-431E3C040A9B}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{7875E08E-43A6-4F76-BAD2-431E3C040A9B}">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{86423575-3B9D-46A2-9D4D-B5C8EEE47047}">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{86423575-3B9D-46A2-9D4D-B5C8EEE47047}">
       <text>
         <r>
           <rPr>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>sam</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>Run trial</t>
+  </si>
+  <si>
+    <t>full output</t>
   </si>
 </sst>
 </file>
@@ -646,27 +649,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:A20"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
@@ -700,17 +700,17 @@
       <c r="N1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="O1" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -724,10 +724,10 @@
         <v>1</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>10</v>
@@ -741,13 +741,13 @@
       <c r="N2" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+      <c r="O2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>6</v>
@@ -782,64 +782,69 @@
       <c r="N3" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <f>IF(OR(C1="sam",C1="sai"),1,0)</f>
-        <v>1</v>
-      </c>
       <c r="D5">
-        <f t="shared" ref="D5:N5" si="0">IF(OR(D1="sam",D1="sai"),1,0)</f>
+        <f>IF(OR(D1="sam",D1="sai"),1,0)</f>
         <v>1</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E5:O5" si="0">IF(OR(E1="sam",E1="sai"),1,0)</f>
         <v>1</v>
       </c>
       <c r="F5">
@@ -878,19 +883,23 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -922,20 +931,23 @@
       <c r="N6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
       <c r="E7">
         <v>1</v>
       </c>
@@ -966,23 +978,26 @@
       <c r="N7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>0.9</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
       <c r="F8">
         <v>1</v>
       </c>
@@ -1010,23 +1025,26 @@
       <c r="N8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
       <c r="F9">
         <v>1</v>
       </c>
@@ -1054,26 +1072,29 @@
       <c r="N9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>0.9</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
       <c r="G10">
         <v>1</v>
       </c>
@@ -1098,26 +1119,29 @@
       <c r="N10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
-        <v>1</v>
-      </c>
-      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
       <c r="G11">
         <v>1</v>
       </c>
@@ -1142,17 +1166,20 @@
       <c r="N11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="b">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
       <c r="D12">
         <v>1</v>
       </c>
@@ -1160,11 +1187,11 @@
         <v>1</v>
       </c>
       <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
         <v>0.9</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
       <c r="H12">
         <v>1</v>
       </c>
@@ -1186,17 +1213,20 @@
       <c r="N12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="b">
-        <v>1</v>
-      </c>
-      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="D13">
         <v>1</v>
       </c>
@@ -1204,11 +1234,11 @@
         <v>1</v>
       </c>
       <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
       <c r="H13">
         <v>1</v>
       </c>
@@ -1230,17 +1260,20 @@
       <c r="N13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="b">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
       <c r="D14">
         <v>1</v>
       </c>
@@ -1251,11 +1284,11 @@
         <v>1</v>
       </c>
       <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>0.9</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
       <c r="I14">
         <v>1</v>
       </c>
@@ -1274,17 +1307,20 @@
       <c r="N14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="b">
-        <v>1</v>
-      </c>
-      <c r="B15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
       <c r="D15">
         <v>1</v>
       </c>
@@ -1295,11 +1331,11 @@
         <v>1</v>
       </c>
       <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
       <c r="I15">
         <v>1</v>
       </c>
@@ -1318,17 +1354,20 @@
       <c r="N15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
       <c r="D16">
         <v>1</v>
       </c>
@@ -1342,11 +1381,11 @@
         <v>1</v>
       </c>
       <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <v>0.9</v>
       </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
       <c r="J16">
         <v>1</v>
       </c>
@@ -1362,17 +1401,20 @@
       <c r="N16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
-        <v>1</v>
-      </c>
-      <c r="B17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
       <c r="D17">
         <v>1</v>
       </c>
@@ -1386,11 +1428,11 @@
         <v>1</v>
       </c>
       <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
       <c r="J17">
         <v>1</v>
       </c>
@@ -1406,17 +1448,20 @@
       <c r="N17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
       <c r="D18">
         <v>1</v>
       </c>
@@ -1433,11 +1478,11 @@
         <v>1</v>
       </c>
       <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
         <v>0.9</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
       <c r="K18">
         <v>1</v>
       </c>
@@ -1450,17 +1495,20 @@
       <c r="N18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
-        <v>1</v>
-      </c>
-      <c r="B19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
       <c r="D19">
         <v>1</v>
       </c>
@@ -1477,11 +1525,11 @@
         <v>1</v>
       </c>
       <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
       <c r="K19">
         <v>1</v>
       </c>
@@ -1494,17 +1542,20 @@
       <c r="N19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="b">
-        <v>1</v>
-      </c>
-      <c r="B20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
       <c r="D20">
         <v>1</v>
       </c>
@@ -1524,11 +1575,11 @@
         <v>1</v>
       </c>
       <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
         <v>0.9</v>
       </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
       <c r="L20">
         <v>1</v>
       </c>
@@ -1538,17 +1589,20 @@
       <c r="N20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="b">
         <v>0</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
       <c r="D21">
         <v>1</v>
       </c>
@@ -1568,11 +1622,11 @@
         <v>1</v>
       </c>
       <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
       <c r="L21">
         <v>1</v>
       </c>
@@ -1582,17 +1636,20 @@
       <c r="N21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="b">
         <v>0</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
       <c r="D22">
         <v>1</v>
       </c>
@@ -1615,28 +1672,31 @@
         <v>1</v>
       </c>
       <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
         <v>0.9</v>
       </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
       <c r="M22">
         <v>1</v>
       </c>
       <c r="N22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="b">
         <v>0</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
       <c r="D23">
         <v>1</v>
       </c>
@@ -1659,28 +1719,31 @@
         <v>1</v>
       </c>
       <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
       <c r="M23">
         <v>1</v>
       </c>
       <c r="N23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="b">
         <v>0</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
       <c r="D24">
         <v>1</v>
       </c>
@@ -1706,25 +1769,28 @@
         <v>1</v>
       </c>
       <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
         <v>0.9</v>
       </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
       <c r="N24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="b">
         <v>0</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
       <c r="D25">
         <v>1</v>
       </c>
@@ -1750,25 +1816,28 @@
         <v>1</v>
       </c>
       <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
       <c r="N25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="b">
         <v>0</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
       <c r="D26">
         <v>1</v>
       </c>
@@ -1797,22 +1866,25 @@
         <v>1</v>
       </c>
       <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
         <v>0.9</v>
       </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="b">
         <v>0</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
       <c r="D27">
         <v>1</v>
       </c>
@@ -1841,22 +1913,25 @@
         <v>1</v>
       </c>
       <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="b">
         <v>0</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
       <c r="D28">
         <v>1</v>
       </c>
@@ -1888,19 +1963,22 @@
         <v>1</v>
       </c>
       <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
         <v>0.9</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="b">
         <v>0</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
       <c r="D29">
         <v>1</v>
       </c>
@@ -1932,11 +2010,14 @@
         <v>1</v>
       </c>
       <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
         <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B4:N5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
+  <autoFilter ref="C4:O5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
@@ -1957,7 +2038,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A1:A1048576</xm:sqref>
+          <xm:sqref>A1:B1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
fixed issue in rotation generator (added E1 set so that of couldnt provide E in yr1) and altered sheep stuff a litte and altered read xl function to read in arrays as numpy if arg is true
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D29667C-43AE-4519-B3B5-08FC488FC52E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA307AA1-B1D9-4421-B6A7-BE273F22CCFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="45972" yWindow="84" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$O$5</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>sam</t>
   </si>
@@ -248,6 +248,18 @@
   </si>
   <si>
     <t>full output</t>
+  </si>
+  <si>
+    <t>saa</t>
+  </si>
+  <si>
+    <t>g2_BM_included</t>
+  </si>
+  <si>
+    <t>g2_BT_included</t>
+  </si>
+  <si>
+    <t>g2_BMT_included</t>
   </si>
 </sst>
 </file>
@@ -359,7 +371,97 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -680,13 +782,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -694,7 +796,7 @@
     <col min="3" max="3" width="17.5546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
@@ -734,8 +836,17 @@
       <c r="O1" s="6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
@@ -775,8 +886,17 @@
       <c r="O2" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
@@ -816,8 +936,11 @@
       <c r="O3" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -859,8 +982,11 @@
       <c r="O4" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -918,8 +1044,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="9">
+        <f t="shared" ref="P5:R5" si="1">IF(OR(P1="sam",P1="sai"),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -965,8 +1103,17 @@
       <c r="O6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -1012,8 +1159,17 @@
       <c r="O7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1059,8 +1215,17 @@
       <c r="O8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1106,8 +1271,17 @@
       <c r="O9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1153,8 +1327,17 @@
       <c r="O10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1200,8 +1383,17 @@
       <c r="O11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1247,8 +1439,17 @@
       <c r="O12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -1294,8 +1495,17 @@
       <c r="O13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -1341,8 +1551,17 @@
       <c r="O14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -1388,8 +1607,17 @@
       <c r="O15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -1435,8 +1663,17 @@
       <c r="O16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -1482,8 +1719,17 @@
       <c r="O17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -1529,8 +1775,17 @@
       <c r="O18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -1576,8 +1831,17 @@
       <c r="O19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -1623,8 +1887,17 @@
       <c r="O20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -1670,8 +1943,17 @@
       <c r="O21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -1717,8 +1999,17 @@
       <c r="O22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -1764,8 +2055,17 @@
       <c r="O23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -1811,8 +2111,17 @@
       <c r="O24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -1858,8 +2167,17 @@
       <c r="O25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -1905,8 +2223,17 @@
       <c r="O26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -1952,8 +2279,17 @@
       <c r="O27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -1999,8 +2335,17 @@
       <c r="O28">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -2046,16 +2391,36 @@
       <c r="O29">
         <v>1.1000000000000001</v>
       </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="C4:O5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="saa">
+      <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="sap">
+      <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="sam">
+      <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,A1)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>

</xml_diff>

<commit_message>
third lot of inputs coded
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA307AA1-B1D9-4421-B6A7-BE273F22CCFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D4DB4A-A280-4857-A3E2-382700F596F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="84" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$O$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$T$5</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -121,8 +121,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>sam</t>
   </si>
@@ -253,13 +275,25 @@
     <t>saa</t>
   </si>
   <si>
-    <t>g2_BM_included</t>
-  </si>
-  <si>
-    <t>g2_BT_included</t>
-  </si>
-  <si>
-    <t>g2_BMT_included</t>
+    <t>sav</t>
+  </si>
+  <si>
+    <t>sap</t>
+  </si>
+  <si>
+    <t>g3_BM_included</t>
+  </si>
+  <si>
+    <t>g3_BT_included</t>
+  </si>
+  <si>
+    <t>g3_BMT_included</t>
+  </si>
+  <si>
+    <t>TOL_1_inc</t>
+  </si>
+  <si>
+    <t>TOL_2_inc</t>
   </si>
 </sst>
 </file>
@@ -371,7 +405,54 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -434,46 +515,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFEBAC9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -782,13 +838,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q3" sqref="Q3"/>
+      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,24 +852,24 @@
     <col min="3" max="3" width="17.5546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>0</v>
@@ -837,84 +893,101 @@
         <v>0</v>
       </c>
       <c r="P1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="J2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>45</v>
-      </c>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="6" t="s">
         <v>6</v>
       </c>
@@ -936,11 +1009,26 @@
       <c r="O3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
+      <c r="P3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -951,42 +1039,47 @@
         <v>5</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7" t="s">
+      <c r="O4" s="7"/>
+      <c r="P4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -996,68 +1089,92 @@
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="9">
-        <f t="shared" ref="D5:O5" si="0">IF(OR(D1="sam",D1="sai"),1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="M5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="N5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O5" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P5" s="9">
-        <f t="shared" ref="P5:R5" si="1">IF(OR(P1="sam",P1="sai"),1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="9">
-        <f t="shared" si="1"/>
+      <c r="D5" s="9" t="str" cm="1">
+        <f t="array" ref="D5">_xlfn.IFS(OR(D1="sam",D1="sai"),1,D1="sav","-",OR(D1="sap",D1="saa"),0)</f>
+        <v>-</v>
+      </c>
+      <c r="E5" s="9" t="str" cm="1">
+        <f t="array" ref="E5">_xlfn.IFS(OR(E1="sam",E1="sai"),1,E1="sav","-",OR(E1="sap",E1="saa"),0)</f>
+        <v>-</v>
+      </c>
+      <c r="F5" s="9" t="str" cm="1">
+        <f t="array" ref="F5">_xlfn.IFS(OR(F1="sam",F1="sai"),1,F1="sav","-",OR(F1="sap",F1="saa"),0)</f>
+        <v>-</v>
+      </c>
+      <c r="G5" s="9" t="str" cm="1">
+        <f t="array" ref="G5">_xlfn.IFS(OR(G1="sam",G1="sai"),1,G1="sav","-",OR(G1="sap",G1="saa"),0)</f>
+        <v>-</v>
+      </c>
+      <c r="H5" s="9" t="str" cm="1">
+        <f t="array" ref="H5">_xlfn.IFS(OR(H1="sam",H1="sai"),1,H1="sav","-",OR(H1="sap",H1="saa"),0)</f>
+        <v>-</v>
+      </c>
+      <c r="I5" s="9" cm="1">
+        <f t="array" ref="I5">_xlfn.IFS(OR(I1="sam",I1="sai"),1,I1="sav","-",OR(I1="sap",I1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="9" cm="1">
+        <f t="array" ref="J5">_xlfn.IFS(OR(J1="sam",J1="sai"),1,J1="sav","-",OR(J1="sap",J1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="9" cm="1">
+        <f t="array" ref="K5">_xlfn.IFS(OR(K1="sam",K1="sai"),1,K1="sav","-",OR(K1="sap",K1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="9" cm="1">
+        <f t="array" ref="L5">_xlfn.IFS(OR(L1="sam",L1="sai"),1,L1="sav","-",OR(L1="sap",L1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="9" cm="1">
+        <f t="array" ref="M5">_xlfn.IFS(OR(M1="sam",M1="sai"),1,M1="sav","-",OR(M1="sap",M1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="9" cm="1">
+        <f t="array" ref="N5">_xlfn.IFS(OR(N1="sam",N1="sai"),1,N1="sav","-",OR(N1="sap",N1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="9" cm="1">
+        <f t="array" ref="O5">_xlfn.IFS(OR(O1="sam",O1="sai"),1,O1="sav","-",OR(O1="sap",O1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="P5" s="9" cm="1">
+        <f t="array" ref="P5">_xlfn.IFS(OR(P1="sam",P1="sai"),1,P1="sav","-",OR(P1="sap",P1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="9" cm="1">
+        <f t="array" ref="Q5">_xlfn.IFS(OR(Q1="sam",Q1="sai"),1,Q1="sav","-",OR(Q1="sap",Q1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="R5" s="9" cm="1">
+        <f t="array" ref="R5">_xlfn.IFS(OR(R1="sam",R1="sai"),1,R1="sav","-",OR(R1="sap",R1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="S5" s="9" cm="1">
+        <f t="array" ref="S5">_xlfn.IFS(OR(S1="sam",S1="sai"),1,S1="sav","-",OR(S1="sap",S1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="T5" s="9" cm="1">
+        <f t="array" ref="T5">_xlfn.IFS(OR(T1="sam",T1="sai"),1,T1="sav","-",OR(T1="sap",T1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="U5" s="9" cm="1">
+        <f t="array" ref="U5">_xlfn.IFS(OR(U1="sam",U1="sai"),1,U1="sav","-",OR(U1="sap",U1="saa"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="9" cm="1">
+        <f t="array" ref="V5">_xlfn.IFS(OR(V1="sam",V1="sai"),1,V1="sav","-",OR(V1="sap",V1="saa"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="9" cm="1">
+        <f t="array" ref="W5">_xlfn.IFS(OR(W1="sam",W1="sai"),1,W1="sav","-",OR(W1="sap",W1="saa"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="9" cm="1">
+        <f t="array" ref="X5">_xlfn.IFS(OR(X1="sam",X1="sai"),1,X1="sav","-",OR(X1="sap",X1="saa"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -1067,24 +1184,29 @@
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="str">
+        <f>D5</f>
+        <v>-</v>
+      </c>
+      <c r="E6" t="str">
+        <f>E5</f>
+        <v>-</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:H6" si="0">F5</f>
+        <v>-</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="I6">
         <v>0.9</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
       <c r="J6">
         <v>1</v>
       </c>
@@ -1112,8 +1234,23 @@
       <c r="R6">
         <v>1</v>
       </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -1123,24 +1260,29 @@
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="str">
+        <f t="shared" ref="D7:D29" si="1">D6</f>
+        <v>-</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" ref="E7:E29" si="2">E6</f>
+        <v>-</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" ref="F7:F29" si="3">F6</f>
+        <v>-</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" ref="G7:G29" si="4">G6</f>
+        <v>-</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" ref="H7:H29" si="5">H6</f>
+        <v>-</v>
+      </c>
+      <c r="I7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
       <c r="J7">
         <v>1</v>
       </c>
@@ -1168,8 +1310,23 @@
       <c r="R7">
         <v>1</v>
       </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1179,27 +1336,32 @@
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
         <v>0.9</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
       <c r="K8">
         <v>1</v>
       </c>
@@ -1224,8 +1386,23 @@
       <c r="R8">
         <v>1</v>
       </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1235,27 +1412,32 @@
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
       <c r="K9">
         <v>1</v>
       </c>
@@ -1280,8 +1462,23 @@
       <c r="R9">
         <v>1</v>
       </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>1</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1291,30 +1488,35 @@
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
         <v>0.9</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
       <c r="L10">
         <v>1</v>
       </c>
@@ -1336,8 +1538,23 @@
       <c r="R10">
         <v>1</v>
       </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1347,30 +1564,35 @@
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
       <c r="L11">
         <v>1</v>
       </c>
@@ -1392,8 +1614,23 @@
       <c r="R11">
         <v>1</v>
       </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1403,33 +1640,38 @@
       <c r="C12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
         <v>0.9</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
       <c r="M12">
         <v>1</v>
       </c>
@@ -1448,8 +1690,23 @@
       <c r="R12">
         <v>1</v>
       </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -1459,33 +1716,38 @@
       <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
       <c r="M13">
         <v>1</v>
       </c>
@@ -1504,8 +1766,23 @@
       <c r="R13">
         <v>1</v>
       </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -1515,36 +1792,41 @@
       <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
         <v>0.9</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
       <c r="N14">
         <v>1</v>
       </c>
@@ -1560,8 +1842,23 @@
       <c r="R14">
         <v>1</v>
       </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -1571,36 +1868,41 @@
       <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
       <c r="N15">
         <v>1</v>
       </c>
@@ -1616,8 +1918,23 @@
       <c r="R15">
         <v>1</v>
       </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -1627,39 +1944,44 @@
       <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
         <v>0.9</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
       <c r="O16">
         <v>1</v>
       </c>
@@ -1672,8 +1994,23 @@
       <c r="R16">
         <v>1</v>
       </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -1683,39 +2020,44 @@
       <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
       <c r="O17">
         <v>1</v>
       </c>
@@ -1728,8 +2070,23 @@
       <c r="R17">
         <v>1</v>
       </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -1739,42 +2096,47 @@
       <c r="C18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
       <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
         <v>0.9</v>
       </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
       <c r="P18">
         <v>1</v>
       </c>
@@ -1784,8 +2146,23 @@
       <c r="R18">
         <v>1</v>
       </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -1795,42 +2172,47 @@
       <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19">
-        <v>1</v>
-      </c>
       <c r="P19">
         <v>1</v>
       </c>
@@ -1840,8 +2222,23 @@
       <c r="R19">
         <v>1</v>
       </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -1851,20 +2248,25 @@
       <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -1873,31 +2275,46 @@
         <v>1</v>
       </c>
       <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
         <v>0.9</v>
       </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
       <c r="Q20">
         <v>1</v>
       </c>
       <c r="R20">
         <v>1</v>
       </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -1907,20 +2324,25 @@
       <c r="C21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -1929,31 +2351,46 @@
         <v>1</v>
       </c>
       <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
       <c r="Q21">
         <v>1</v>
       </c>
       <c r="R21">
         <v>1</v>
       </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -1963,20 +2400,25 @@
       <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1988,28 +2430,43 @@
         <v>1</v>
       </c>
       <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
         <v>0.9</v>
       </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22">
-        <v>1</v>
-      </c>
-      <c r="P22">
-        <v>1</v>
-      </c>
-      <c r="Q22">
-        <v>1</v>
-      </c>
       <c r="R22">
         <v>1</v>
       </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2019,20 +2476,25 @@
       <c r="C23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -2044,28 +2506,43 @@
         <v>1</v>
       </c>
       <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23">
-        <v>1</v>
-      </c>
-      <c r="P23">
-        <v>1</v>
-      </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
       <c r="R23">
         <v>1</v>
       </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2075,20 +2552,25 @@
       <c r="C24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -2103,25 +2585,40 @@
         <v>1</v>
       </c>
       <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
         <v>0.9</v>
       </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-      <c r="P24">
-        <v>1</v>
-      </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="R24">
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2131,20 +2628,25 @@
       <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -2159,25 +2661,40 @@
         <v>1</v>
       </c>
       <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="R25">
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="W25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2187,20 +2704,25 @@
       <c r="C26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -2218,22 +2740,37 @@
         <v>1</v>
       </c>
       <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
         <v>0.9</v>
       </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
-        <v>1</v>
-      </c>
-      <c r="Q26">
-        <v>1</v>
-      </c>
-      <c r="R26">
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -2243,20 +2780,25 @@
       <c r="C27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I27">
         <v>1</v>
@@ -2274,22 +2816,37 @@
         <v>1</v>
       </c>
       <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="P27">
-        <v>1</v>
-      </c>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-      <c r="R27">
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -2299,20 +2856,25 @@
       <c r="C28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -2333,19 +2895,34 @@
         <v>1</v>
       </c>
       <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
         <v>0.9</v>
       </c>
-      <c r="P28">
-        <v>1</v>
-      </c>
-      <c r="Q28">
-        <v>1</v>
-      </c>
-      <c r="R28">
+      <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -2355,20 +2932,25 @@
       <c r="C29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -2389,38 +2971,57 @@
         <v>1</v>
       </c>
       <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P29">
-        <v>1</v>
-      </c>
-      <c r="Q29">
-        <v>1</v>
-      </c>
-      <c r="R29">
+      <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C4:O5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
+  <autoFilter ref="C4:T5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="saa">
-      <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="sam">
+      <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="sam">
-      <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="saa">
+      <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,A1)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>

</xml_diff>

<commit_message>
equation systems started and other sheep functions started
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D4DB4A-A280-4857-A3E2-382700F596F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70446D0B-C4EC-4846-B1E5-E015B3A53376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$T$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$U$5</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -41,6 +41,30 @@
     <author>Michael Young</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CCB77013-F05A-42FB-A15C-BBB0BA6C23F4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+to keep the conditional formatting rules tidy, you can only insert a blank row or column (cant copy and insert paste) then you can copy the formula from a given row and paste it into your newly inserted row. </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C3" authorId="0" shapeId="0" xr:uid="{3BDB7BEB-FC53-4975-ADDB-A81C02A033DC}">
       <text>
         <r>
@@ -144,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>sam</t>
   </si>
@@ -294,6 +318,12 @@
   </si>
   <si>
     <t>TOL_2_inc</t>
+  </si>
+  <si>
+    <t>Note on formatting</t>
+  </si>
+  <si>
+    <t>eqn_compare</t>
   </si>
 </sst>
 </file>
@@ -377,7 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -400,22 +430,15 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -469,7 +492,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -480,6 +503,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -509,7 +539,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="8" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -520,6 +550,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -838,13 +875,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:X29"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,7 +889,10 @@
     <col min="3" max="3" width="17.5546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
@@ -872,7 +912,7 @@
         <v>43</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>0</v>
@@ -908,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="V1" s="6" t="s">
         <v>42</v>
@@ -916,11 +956,14 @@
       <c r="W1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
@@ -940,11 +983,11 @@
         <v>47</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="K2" s="6" t="s">
         <v>1</v>
       </c>
@@ -958,10 +1001,10 @@
         <v>1</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>10</v>
@@ -975,11 +1018,14 @@
       <c r="T2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="6"/>
+      <c r="U2" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
     </row>
-    <row r="3" spans="1:24" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
@@ -988,9 +1034,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="I3" s="6"/>
       <c r="J3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1024,11 +1068,14 @@
       <c r="T3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="6"/>
+      <c r="U3" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
     </row>
-    <row r="4" spans="1:24" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1044,42 +1091,43 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="7"/>
+      <c r="K4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -1109,9 +1157,9 @@
         <f t="array" ref="H5">_xlfn.IFS(OR(H1="sam",H1="sai"),1,H1="sav","-",OR(H1="sap",H1="saa"),0)</f>
         <v>-</v>
       </c>
-      <c r="I5" s="9" cm="1">
+      <c r="I5" s="9" t="str" cm="1">
         <f t="array" ref="I5">_xlfn.IFS(OR(I1="sam",I1="sai"),1,I1="sav","-",OR(I1="sap",I1="saa"),0)</f>
-        <v>1</v>
+        <v>-</v>
       </c>
       <c r="J5" s="9" cm="1">
         <f t="array" ref="J5">_xlfn.IFS(OR(J1="sam",J1="sai"),1,J1="sav","-",OR(J1="sap",J1="saa"),0)</f>
@@ -1159,7 +1207,7 @@
       </c>
       <c r="U5" s="9" cm="1">
         <f t="array" ref="U5">_xlfn.IFS(OR(U1="sam",U1="sai"),1,U1="sav","-",OR(U1="sap",U1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" s="9" cm="1">
         <f t="array" ref="V5">_xlfn.IFS(OR(V1="sam",V1="sai"),1,V1="sav","-",OR(V1="sap",V1="saa"),0)</f>
@@ -1173,8 +1221,12 @@
         <f t="array" ref="X5">_xlfn.IFS(OR(X1="sam",X1="sai"),1,X1="sav","-",OR(X1="sap",X1="saa"),0)</f>
         <v>0</v>
       </c>
+      <c r="Y5" s="9" cm="1">
+        <f t="array" ref="Y5">_xlfn.IFS(OR(Y1="sam",Y1="sai"),1,Y1="sav","-",OR(Y1="sap",Y1="saa"),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -1204,12 +1256,13 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="str">
+        <f t="shared" ref="I6" si="1">I5</f>
+        <v>-</v>
+      </c>
+      <c r="J6">
         <v>0.9</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
       <c r="K6">
         <v>1</v>
       </c>
@@ -1249,8 +1302,11 @@
       <c r="W6">
         <v>1</v>
       </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -1261,31 +1317,32 @@
         <v>12</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D7:D29" si="1">D6</f>
+        <f t="shared" ref="D7:D29" si="2">D6</f>
         <v>-</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E7:E29" si="2">E6</f>
+        <f t="shared" ref="E7:E29" si="3">E6</f>
         <v>-</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ref="F7:F29" si="3">F6</f>
+        <f t="shared" ref="F7:F29" si="4">F6</f>
         <v>-</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" ref="G7:G29" si="4">G6</f>
+        <f t="shared" ref="G7:G29" si="5">G6</f>
         <v>-</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7:H29" si="5">H6</f>
-        <v>-</v>
-      </c>
-      <c r="I7">
+        <f t="shared" ref="H7:I29" si="6">H6</f>
+        <v>-</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" ref="I7" si="7">I6</f>
+        <v>-</v>
+      </c>
+      <c r="J7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
       <c r="K7">
         <v>1</v>
       </c>
@@ -1325,8 +1382,11 @@
       <c r="W7">
         <v>1</v>
       </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1337,34 +1397,35 @@
         <v>13</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" ref="I8" si="8">I7</f>
+        <v>-</v>
       </c>
       <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
         <v>0.9</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
       <c r="L8">
         <v>1</v>
       </c>
@@ -1401,8 +1462,11 @@
       <c r="W8">
         <v>1</v>
       </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1413,34 +1477,35 @@
         <v>14</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" ref="I9" si="9">I8</f>
+        <v>-</v>
       </c>
       <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
       <c r="L9">
         <v>1</v>
       </c>
@@ -1477,8 +1542,11 @@
       <c r="W9">
         <v>1</v>
       </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1489,37 +1557,38 @@
         <v>15</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" ref="I10" si="10">I9</f>
+        <v>-</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
         <v>0.9</v>
       </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
       <c r="M10">
         <v>1</v>
       </c>
@@ -1553,8 +1622,11 @@
       <c r="W10">
         <v>1</v>
       </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1565,37 +1637,38 @@
         <v>16</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" ref="I11" si="11">I10</f>
+        <v>-</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
       <c r="M11">
         <v>1</v>
       </c>
@@ -1629,8 +1702,11 @@
       <c r="W11">
         <v>1</v>
       </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1641,27 +1717,28 @@
         <v>22</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" ref="I12" si="12">I11</f>
+        <v>-</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1670,11 +1747,11 @@
         <v>1</v>
       </c>
       <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
         <v>0.9</v>
       </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
       <c r="N12">
         <v>1</v>
       </c>
@@ -1705,8 +1782,11 @@
       <c r="W12">
         <v>1</v>
       </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -1717,27 +1797,28 @@
         <v>17</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" ref="I13" si="13">I12</f>
+        <v>-</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1746,11 +1827,11 @@
         <v>1</v>
       </c>
       <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
       <c r="N13">
         <v>1</v>
       </c>
@@ -1781,8 +1862,11 @@
       <c r="W13">
         <v>1</v>
       </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -1793,27 +1877,28 @@
         <v>18</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" ref="I14" si="14">I13</f>
+        <v>-</v>
       </c>
       <c r="J14">
         <v>1</v>
@@ -1825,11 +1910,11 @@
         <v>1</v>
       </c>
       <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
         <v>0.9</v>
       </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
       <c r="O14">
         <v>1</v>
       </c>
@@ -1857,8 +1942,11 @@
       <c r="W14">
         <v>1</v>
       </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -1869,27 +1957,28 @@
         <v>19</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" ref="I15" si="15">I14</f>
+        <v>-</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1901,11 +1990,11 @@
         <v>1</v>
       </c>
       <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
       <c r="O15">
         <v>1</v>
       </c>
@@ -1933,8 +2022,11 @@
       <c r="W15">
         <v>1</v>
       </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -1945,27 +2037,28 @@
         <v>20</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" ref="I16" si="16">I15</f>
+        <v>-</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1980,11 +2073,11 @@
         <v>1</v>
       </c>
       <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
         <v>0.9</v>
       </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
       <c r="P16">
         <v>1</v>
       </c>
@@ -2009,8 +2102,11 @@
       <c r="W16">
         <v>1</v>
       </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -2021,27 +2117,28 @@
         <v>21</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" ref="I17" si="17">I16</f>
+        <v>-</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -2056,11 +2153,11 @@
         <v>1</v>
       </c>
       <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O17">
-        <v>1</v>
-      </c>
       <c r="P17">
         <v>1</v>
       </c>
@@ -2085,8 +2182,11 @@
       <c r="W17">
         <v>1</v>
       </c>
+      <c r="X17">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -2097,27 +2197,28 @@
         <v>23</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" ref="I18" si="18">I17</f>
+        <v>-</v>
       </c>
       <c r="J18">
         <v>1</v>
@@ -2135,11 +2236,11 @@
         <v>1</v>
       </c>
       <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
         <v>0.9</v>
       </c>
-      <c r="P18">
-        <v>1</v>
-      </c>
       <c r="Q18">
         <v>1</v>
       </c>
@@ -2161,8 +2262,11 @@
       <c r="W18">
         <v>1</v>
       </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -2173,27 +2277,28 @@
         <v>24</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" ref="I19" si="19">I18</f>
+        <v>-</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -2211,11 +2316,11 @@
         <v>1</v>
       </c>
       <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P19">
-        <v>1</v>
-      </c>
       <c r="Q19">
         <v>1</v>
       </c>
@@ -2237,8 +2342,11 @@
       <c r="W19">
         <v>1</v>
       </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -2249,27 +2357,28 @@
         <v>25</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" ref="I20" si="20">I19</f>
+        <v>-</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -2290,11 +2399,11 @@
         <v>1</v>
       </c>
       <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
         <v>0.9</v>
       </c>
-      <c r="Q20">
-        <v>1</v>
-      </c>
       <c r="R20">
         <v>1</v>
       </c>
@@ -2313,8 +2422,11 @@
       <c r="W20">
         <v>1</v>
       </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -2325,27 +2437,28 @@
         <v>26</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" ref="I21" si="21">I20</f>
+        <v>-</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -2366,11 +2479,11 @@
         <v>1</v>
       </c>
       <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
       <c r="R21">
         <v>1</v>
       </c>
@@ -2389,8 +2502,11 @@
       <c r="W21">
         <v>1</v>
       </c>
+      <c r="X21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -2401,27 +2517,28 @@
         <v>27</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" ref="I22" si="22">I21</f>
+        <v>-</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -2445,11 +2562,11 @@
         <v>1</v>
       </c>
       <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
         <v>0.9</v>
       </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
       <c r="S22">
         <v>1</v>
       </c>
@@ -2465,8 +2582,11 @@
       <c r="W22">
         <v>1</v>
       </c>
+      <c r="X22">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2477,27 +2597,28 @@
         <v>28</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" ref="I23" si="23">I22</f>
+        <v>-</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2521,11 +2642,11 @@
         <v>1</v>
       </c>
       <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
       <c r="S23">
         <v>1</v>
       </c>
@@ -2541,8 +2662,11 @@
       <c r="W23">
         <v>1</v>
       </c>
+      <c r="X23">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2553,27 +2677,28 @@
         <v>29</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I24">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" ref="I24" si="24">I23</f>
+        <v>-</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2600,11 +2725,11 @@
         <v>1</v>
       </c>
       <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
         <v>0.9</v>
       </c>
-      <c r="S24">
-        <v>1</v>
-      </c>
       <c r="T24">
         <v>1</v>
       </c>
@@ -2617,8 +2742,11 @@
       <c r="W24">
         <v>1</v>
       </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2629,27 +2757,28 @@
         <v>30</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" ref="I25" si="25">I24</f>
+        <v>-</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -2676,11 +2805,11 @@
         <v>1</v>
       </c>
       <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S25">
-        <v>1</v>
-      </c>
       <c r="T25">
         <v>1</v>
       </c>
@@ -2693,8 +2822,11 @@
       <c r="W25">
         <v>1</v>
       </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2705,27 +2837,28 @@
         <v>31</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I26">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" ref="I26" si="26">I25</f>
+        <v>-</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -2755,11 +2888,11 @@
         <v>1</v>
       </c>
       <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
         <v>0.9</v>
       </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
       <c r="U26">
         <v>1</v>
       </c>
@@ -2769,8 +2902,11 @@
       <c r="W26">
         <v>1</v>
       </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -2781,27 +2917,28 @@
         <v>32</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" ref="I27" si="27">I26</f>
+        <v>-</v>
       </c>
       <c r="J27">
         <v>1</v>
@@ -2831,11 +2968,11 @@
         <v>1</v>
       </c>
       <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T27">
-        <v>1</v>
-      </c>
       <c r="U27">
         <v>1</v>
       </c>
@@ -2845,8 +2982,11 @@
       <c r="W27">
         <v>1</v>
       </c>
+      <c r="X27">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -2857,27 +2997,28 @@
         <v>33</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" ref="I28" si="28">I27</f>
+        <v>-</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2910,19 +3051,22 @@
         <v>1</v>
       </c>
       <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="U28">
         <v>0.9</v>
       </c>
-      <c r="U28">
-        <v>1</v>
-      </c>
       <c r="V28">
         <v>1</v>
       </c>
       <c r="W28">
         <v>1</v>
       </c>
+      <c r="X28">
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -2933,27 +3077,28 @@
         <v>34</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I29">
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" ref="I29" si="29">I28</f>
+        <v>-</v>
       </c>
       <c r="J29">
         <v>1</v>
@@ -2986,31 +3131,34 @@
         <v>1</v>
       </c>
       <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="U29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="U29">
-        <v>1</v>
-      </c>
       <c r="V29">
         <v>1</v>
       </c>
       <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C4:T5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
+  <autoFilter ref="C4:U5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="11" priority="21" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="10" priority="22" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="9" priority="23" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3021,7 +3169,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
+          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,A1)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>

</xml_diff>

<commit_message>
updates to SA function and application
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70446D0B-C4EC-4846-B1E5-E015B3A53376}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0832096-A184-44D6-AF7C-EC6D881E6A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>sam</t>
   </si>
@@ -305,25 +305,16 @@
     <t>sap</t>
   </si>
   <si>
-    <t>g3_BM_included</t>
-  </si>
-  <si>
-    <t>g3_BT_included</t>
-  </si>
-  <si>
-    <t>g3_BMT_included</t>
-  </si>
-  <si>
-    <t>TOL_1_inc</t>
-  </si>
-  <si>
-    <t>TOL_2_inc</t>
-  </si>
-  <si>
     <t>Note on formatting</t>
   </si>
   <si>
     <t>eqn_compare</t>
+  </si>
+  <si>
+    <t>TOL_inc</t>
+  </si>
+  <si>
+    <t>g3_included</t>
   </si>
 </sst>
 </file>
@@ -438,81 +429,7 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -881,17 +798,17 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="17.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="52.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -963,27 +880,27 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="G2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>8</v>
@@ -1025,7 +942,7 @@
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
     </row>
-    <row r="3" spans="1:25" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1075,7 +992,7 @@
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
     </row>
-    <row r="4" spans="1:25" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1085,12 +1002,22 @@
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="D4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="8"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
         <v>35</v>
@@ -1127,7 +1054,7 @@
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -1226,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -1306,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -1333,7 +1260,7 @@
         <v>-</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7:I29" si="6">H6</f>
+        <f t="shared" ref="H7:H29" si="6">H6</f>
         <v>-</v>
       </c>
       <c r="I7" t="str">
@@ -1386,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1466,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1546,7 +1473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1626,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1706,7 +1633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1786,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -1866,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -1946,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -2026,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -2106,7 +2033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -2186,7 +2113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -2266,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -2346,7 +2273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -2426,7 +2353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -2506,7 +2433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -2586,7 +2513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2666,7 +2593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2746,7 +2673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2826,7 +2753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2906,7 +2833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -2986,7 +2913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -3066,7 +2993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -3149,16 +3076,16 @@
   </sheetData>
   <autoFilter ref="C4:U5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="21" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="22" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="23" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="1" priority="23" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
corepyomo fixes (carry over cashflow) add sav, sar and sat sa to exp and exp1
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0832096-A184-44D6-AF7C-EC6D881E6A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956BAF21-AB86-49F1-A7B9-20E093004A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$U$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$V$5</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
   <si>
     <t>sam</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>g3_included</t>
+  </si>
+  <si>
+    <t>woolp_mpg</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,118 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -792,13 +906,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:Y29"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -806,7 +920,7 @@
     <col min="3" max="3" width="17.54296875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>45</v>
       </c>
@@ -832,7 +946,7 @@
         <v>43</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>0</v>
@@ -868,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="W1" s="6" t="s">
         <v>42</v>
@@ -876,11 +990,14 @@
       <c r="X1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
@@ -903,11 +1020,11 @@
         <v>46</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="L2" s="6" t="s">
         <v>1</v>
       </c>
@@ -921,10 +1038,10 @@
         <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="R2" s="6" t="s">
         <v>10</v>
@@ -938,11 +1055,14 @@
       <c r="U2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="6"/>
+      <c r="V2" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
     </row>
-    <row r="3" spans="1:25" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
@@ -952,9 +1072,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
         <v>6</v>
       </c>
@@ -988,11 +1106,14 @@
       <c r="U3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="V3" s="6"/>
+      <c r="V3" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:25" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1018,45 +1139,46 @@
         <v>37</v>
       </c>
       <c r="I4" s="8"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7" t="s">
+      <c r="J4" s="8"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="M4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1088,9 +1210,9 @@
         <f t="array" ref="I5">_xlfn.IFS(OR(I1="sam",I1="sai"),1,I1="sav","-",OR(I1="sap",I1="saa"),0)</f>
         <v>-</v>
       </c>
-      <c r="J5" s="9" cm="1">
+      <c r="J5" s="9" t="str" cm="1">
         <f t="array" ref="J5">_xlfn.IFS(OR(J1="sam",J1="sai"),1,J1="sav","-",OR(J1="sap",J1="saa"),0)</f>
-        <v>1</v>
+        <v>-</v>
       </c>
       <c r="K5" s="9" cm="1">
         <f t="array" ref="K5">_xlfn.IFS(OR(K1="sam",K1="sai"),1,K1="sav","-",OR(K1="sap",K1="saa"),0)</f>
@@ -1138,7 +1260,7 @@
       </c>
       <c r="V5" s="9" cm="1">
         <f t="array" ref="V5">_xlfn.IFS(OR(V1="sam",V1="sai"),1,V1="sav","-",OR(V1="sap",V1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="9" cm="1">
         <f t="array" ref="W5">_xlfn.IFS(OR(W1="sam",W1="sai"),1,W1="sav","-",OR(W1="sap",W1="saa"),0)</f>
@@ -1152,13 +1274,17 @@
         <f t="array" ref="Y5">_xlfn.IFS(OR(Y1="sam",Y1="sai"),1,Y1="sav","-",OR(Y1="sap",Y1="saa"),0)</f>
         <v>0</v>
       </c>
+      <c r="Z5" s="9" cm="1">
+        <f t="array" ref="Z5">_xlfn.IFS(OR(Z1="sam",Z1="sai"),1,Z1="sav","-",OR(Z1="sap",Z1="saa"),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="b">
         <v>1</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
@@ -1184,15 +1310,16 @@
         <v>-</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6" si="1">I5</f>
-        <v>-</v>
-      </c>
-      <c r="J6">
+        <f t="shared" ref="I6:J6" si="1">I5</f>
+        <v>-</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" ref="J6" si="2">J5</f>
+        <v>-</v>
+      </c>
+      <c r="K6">
         <v>0.9</v>
       </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
       <c r="L6">
         <v>1</v>
       </c>
@@ -1232,8 +1359,11 @@
       <c r="X6">
         <v>1</v>
       </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -1244,35 +1374,36 @@
         <v>12</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D7:D29" si="2">D6</f>
+        <f t="shared" ref="D7:D29" si="3">D6</f>
         <v>-</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E7:E29" si="3">E6</f>
+        <f t="shared" ref="E7:E29" si="4">E6</f>
         <v>-</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ref="F7:F29" si="4">F6</f>
+        <f t="shared" ref="F7:F29" si="5">F6</f>
         <v>-</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" ref="G7:G29" si="5">G6</f>
+        <f t="shared" ref="G7:G29" si="6">G6</f>
         <v>-</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7:H29" si="6">H6</f>
+        <f t="shared" ref="H7:H29" si="7">H6</f>
         <v>-</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" ref="I7" si="7">I6</f>
-        <v>-</v>
-      </c>
-      <c r="J7">
+        <f t="shared" ref="I7:J7" si="8">I6</f>
+        <v>-</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" ref="J7" si="9">J6</f>
+        <v>-</v>
+      </c>
+      <c r="K7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
       <c r="L7">
         <v>1</v>
       </c>
@@ -1312,8 +1443,11 @@
       <c r="X7">
         <v>1</v>
       </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1324,38 +1458,39 @@
         <v>13</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" ref="I8" si="8">I7</f>
-        <v>-</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
+        <f t="shared" ref="I8:J8" si="10">I7</f>
+        <v>-</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" ref="J8" si="11">J7</f>
+        <v>-</v>
       </c>
       <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
         <v>0.9</v>
       </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
       <c r="M8">
         <v>1</v>
       </c>
@@ -1392,8 +1527,11 @@
       <c r="X8">
         <v>1</v>
       </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1404,38 +1542,39 @@
         <v>14</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" ref="I9" si="9">I8</f>
-        <v>-</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
+        <f t="shared" ref="I9:J9" si="12">I8</f>
+        <v>-</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ref="J9" si="13">J8</f>
+        <v>-</v>
       </c>
       <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
       <c r="M9">
         <v>1</v>
       </c>
@@ -1472,8 +1611,11 @@
       <c r="X9">
         <v>1</v>
       </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1484,41 +1626,42 @@
         <v>15</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" ref="I10" si="10">I9</f>
-        <v>-</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
+        <f t="shared" ref="I10:J10" si="14">I9</f>
+        <v>-</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" ref="J10" si="15">J9</f>
+        <v>-</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
         <v>0.9</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
       <c r="N10">
         <v>1</v>
       </c>
@@ -1552,8 +1695,11 @@
       <c r="X10">
         <v>1</v>
       </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1564,41 +1710,42 @@
         <v>16</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" ref="I11" si="11">I10</f>
-        <v>-</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
+        <f t="shared" ref="I11:J11" si="16">I10</f>
+        <v>-</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" ref="J11" si="17">J10</f>
+        <v>-</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
       <c r="N11">
         <v>1</v>
       </c>
@@ -1632,8 +1779,11 @@
       <c r="X11">
         <v>1</v>
       </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1644,31 +1794,32 @@
         <v>22</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" ref="I12" si="12">I11</f>
-        <v>-</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
+        <f t="shared" ref="I12:J12" si="18">I11</f>
+        <v>-</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" ref="J12" si="19">J11</f>
+        <v>-</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1677,11 +1828,11 @@
         <v>1</v>
       </c>
       <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
         <v>0.9</v>
       </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
       <c r="O12">
         <v>1</v>
       </c>
@@ -1712,8 +1863,11 @@
       <c r="X12">
         <v>1</v>
       </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -1724,31 +1878,32 @@
         <v>17</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13" si="13">I12</f>
-        <v>-</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
+        <f t="shared" ref="I13:J13" si="20">I12</f>
+        <v>-</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ref="J13" si="21">J12</f>
+        <v>-</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1757,11 +1912,11 @@
         <v>1</v>
       </c>
       <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
       <c r="O13">
         <v>1</v>
       </c>
@@ -1792,8 +1947,11 @@
       <c r="X13">
         <v>1</v>
       </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -1804,31 +1962,32 @@
         <v>18</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" ref="I14" si="14">I13</f>
-        <v>-</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
+        <f t="shared" ref="I14:J14" si="22">I13</f>
+        <v>-</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" ref="J14" si="23">J13</f>
+        <v>-</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1840,11 +1999,11 @@
         <v>1</v>
       </c>
       <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
         <v>0.9</v>
       </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
       <c r="P14">
         <v>1</v>
       </c>
@@ -1872,8 +2031,11 @@
       <c r="X14">
         <v>1</v>
       </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -1884,31 +2046,32 @@
         <v>19</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" ref="I15" si="15">I14</f>
-        <v>-</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
+        <f t="shared" ref="I15:J15" si="24">I14</f>
+        <v>-</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" ref="J15" si="25">J14</f>
+        <v>-</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1920,11 +2083,11 @@
         <v>1</v>
       </c>
       <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
       <c r="P15">
         <v>1</v>
       </c>
@@ -1952,8 +2115,11 @@
       <c r="X15">
         <v>1</v>
       </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -1964,31 +2130,32 @@
         <v>20</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" ref="I16" si="16">I15</f>
-        <v>-</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
+        <f t="shared" ref="I16:J16" si="26">I15</f>
+        <v>-</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" ref="J16" si="27">J15</f>
+        <v>-</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2003,11 +2170,11 @@
         <v>1</v>
       </c>
       <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
         <v>0.9</v>
       </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
       <c r="Q16">
         <v>1</v>
       </c>
@@ -2032,8 +2199,11 @@
       <c r="X16">
         <v>1</v>
       </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -2044,31 +2214,32 @@
         <v>21</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" ref="I17" si="17">I16</f>
-        <v>-</v>
-      </c>
-      <c r="J17">
-        <v>1</v>
+        <f t="shared" ref="I17:J17" si="28">I16</f>
+        <v>-</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" ref="J17" si="29">J16</f>
+        <v>-</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2083,11 +2254,11 @@
         <v>1</v>
       </c>
       <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
       <c r="Q17">
         <v>1</v>
       </c>
@@ -2112,8 +2283,11 @@
       <c r="X17">
         <v>1</v>
       </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -2124,31 +2298,32 @@
         <v>23</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" ref="I18" si="18">I17</f>
-        <v>-</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
+        <f t="shared" ref="I18:J18" si="30">I17</f>
+        <v>-</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" ref="J18" si="31">J17</f>
+        <v>-</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2166,11 +2341,11 @@
         <v>1</v>
       </c>
       <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
         <v>0.9</v>
       </c>
-      <c r="Q18">
-        <v>1</v>
-      </c>
       <c r="R18">
         <v>1</v>
       </c>
@@ -2192,8 +2367,11 @@
       <c r="X18">
         <v>1</v>
       </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -2204,31 +2382,32 @@
         <v>24</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" ref="I19" si="19">I18</f>
-        <v>-</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
+        <f t="shared" ref="I19:J19" si="32">I18</f>
+        <v>-</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" ref="J19" si="33">J18</f>
+        <v>-</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -2246,11 +2425,11 @@
         <v>1</v>
       </c>
       <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
       <c r="R19">
         <v>1</v>
       </c>
@@ -2272,8 +2451,11 @@
       <c r="X19">
         <v>1</v>
       </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -2284,31 +2466,32 @@
         <v>25</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" ref="I20" si="20">I19</f>
-        <v>-</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
+        <f t="shared" ref="I20:J20" si="34">I19</f>
+        <v>-</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" ref="J20" si="35">J19</f>
+        <v>-</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -2329,11 +2512,11 @@
         <v>1</v>
       </c>
       <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20">
         <v>0.9</v>
       </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
       <c r="S20">
         <v>1</v>
       </c>
@@ -2352,8 +2535,11 @@
       <c r="X20">
         <v>1</v>
       </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -2364,31 +2550,32 @@
         <v>26</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" ref="I21" si="21">I20</f>
-        <v>-</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
+        <f t="shared" ref="I21:J21" si="36">I20</f>
+        <v>-</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" ref="J21" si="37">J20</f>
+        <v>-</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -2409,11 +2596,11 @@
         <v>1</v>
       </c>
       <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
       <c r="S21">
         <v>1</v>
       </c>
@@ -2432,8 +2619,11 @@
       <c r="X21">
         <v>1</v>
       </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -2444,31 +2634,32 @@
         <v>27</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" ref="I22" si="22">I21</f>
-        <v>-</v>
-      </c>
-      <c r="J22">
-        <v>1</v>
+        <f t="shared" ref="I22:J22" si="38">I21</f>
+        <v>-</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" ref="J22" si="39">J21</f>
+        <v>-</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -2492,11 +2683,11 @@
         <v>1</v>
       </c>
       <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
         <v>0.9</v>
       </c>
-      <c r="S22">
-        <v>1</v>
-      </c>
       <c r="T22">
         <v>1</v>
       </c>
@@ -2512,8 +2703,11 @@
       <c r="X22">
         <v>1</v>
       </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2524,31 +2718,32 @@
         <v>28</v>
       </c>
       <c r="D23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" ref="I23" si="23">I22</f>
-        <v>-</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
+        <f t="shared" ref="I23:J23" si="40">I22</f>
+        <v>-</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" ref="J23" si="41">J22</f>
+        <v>-</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2572,11 +2767,11 @@
         <v>1</v>
       </c>
       <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S23">
-        <v>1</v>
-      </c>
       <c r="T23">
         <v>1</v>
       </c>
@@ -2592,8 +2787,11 @@
       <c r="X23">
         <v>1</v>
       </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2604,31 +2802,32 @@
         <v>29</v>
       </c>
       <c r="D24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" ref="I24" si="24">I23</f>
-        <v>-</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
+        <f t="shared" ref="I24:J24" si="42">I23</f>
+        <v>-</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" ref="J24" si="43">J23</f>
+        <v>-</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -2655,11 +2854,11 @@
         <v>1</v>
       </c>
       <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
         <v>0.9</v>
       </c>
-      <c r="T24">
-        <v>1</v>
-      </c>
       <c r="U24">
         <v>1</v>
       </c>
@@ -2672,8 +2871,11 @@
       <c r="X24">
         <v>1</v>
       </c>
+      <c r="Y24">
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2684,31 +2886,32 @@
         <v>30</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" ref="I25" si="25">I24</f>
-        <v>-</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
+        <f t="shared" ref="I25:J25" si="44">I24</f>
+        <v>-</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" ref="J25" si="45">J24</f>
+        <v>-</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -2735,11 +2938,11 @@
         <v>1</v>
       </c>
       <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T25">
-        <v>1</v>
-      </c>
       <c r="U25">
         <v>1</v>
       </c>
@@ -2752,8 +2955,11 @@
       <c r="X25">
         <v>1</v>
       </c>
+      <c r="Y25">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2764,31 +2970,32 @@
         <v>31</v>
       </c>
       <c r="D26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" ref="I26" si="26">I25</f>
-        <v>-</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
+        <f t="shared" ref="I26:J26" si="46">I25</f>
+        <v>-</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" ref="J26" si="47">J25</f>
+        <v>-</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -2818,11 +3025,11 @@
         <v>1</v>
       </c>
       <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
         <v>0.9</v>
       </c>
-      <c r="U26">
-        <v>1</v>
-      </c>
       <c r="V26">
         <v>1</v>
       </c>
@@ -2832,8 +3039,11 @@
       <c r="X26">
         <v>1</v>
       </c>
+      <c r="Y26">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -2844,31 +3054,32 @@
         <v>32</v>
       </c>
       <c r="D27" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" ref="I27" si="27">I26</f>
-        <v>-</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
+        <f t="shared" ref="I27:J27" si="48">I26</f>
+        <v>-</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" ref="J27" si="49">J26</f>
+        <v>-</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -2898,11 +3109,11 @@
         <v>1</v>
       </c>
       <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="U27">
-        <v>1</v>
-      </c>
       <c r="V27">
         <v>1</v>
       </c>
@@ -2912,8 +3123,11 @@
       <c r="X27">
         <v>1</v>
       </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -2924,31 +3138,32 @@
         <v>33</v>
       </c>
       <c r="D28" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" ref="I28" si="28">I27</f>
-        <v>-</v>
-      </c>
-      <c r="J28">
-        <v>1</v>
+        <f t="shared" ref="I28:J28" si="50">I27</f>
+        <v>-</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" ref="J28" si="51">J27</f>
+        <v>-</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -2981,19 +3196,22 @@
         <v>1</v>
       </c>
       <c r="U28">
+        <v>1</v>
+      </c>
+      <c r="V28">
         <v>0.9</v>
       </c>
-      <c r="V28">
-        <v>1</v>
-      </c>
       <c r="W28">
         <v>1</v>
       </c>
       <c r="X28">
         <v>1</v>
       </c>
+      <c r="Y28">
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -3004,31 +3222,32 @@
         <v>34</v>
       </c>
       <c r="D29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
       <c r="F29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" ref="I29" si="29">I28</f>
-        <v>-</v>
-      </c>
-      <c r="J29">
-        <v>1</v>
+        <f t="shared" ref="I29:J29" si="52">I28</f>
+        <v>-</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" ref="J29" si="53">J28</f>
+        <v>-</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -3061,31 +3280,34 @@
         <v>1</v>
       </c>
       <c r="U29">
+        <v>1</v>
+      </c>
+      <c r="V29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="V29">
-        <v>1</v>
-      </c>
       <c r="W29">
         <v>1</v>
       </c>
       <c r="X29">
+        <v>1</v>
+      </c>
+      <c r="Y29">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C4:U5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
+  <autoFilter ref="C4:V5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="23" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
cashflow fixed change to exp.py
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956BAF21-AB86-49F1-A7B9-20E093004A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F3DCAD-F0D4-4288-A404-CAB5580BAD35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -432,118 +432,7 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -912,12 +801,13 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="17.54296875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
@@ -1310,12 +1200,11 @@
         <v>-</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6:J6" si="1">I5</f>
-        <v>-</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" ref="J6" si="2">J5</f>
-        <v>-</v>
+        <f t="shared" ref="I6" si="1">I5</f>
+        <v>-</v>
+      </c>
+      <c r="J6">
+        <v>100000000</v>
       </c>
       <c r="K6">
         <v>0.9</v>
@@ -1374,32 +1263,32 @@
         <v>12</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D7:D29" si="3">D6</f>
+        <f t="shared" ref="D7:D29" si="2">D6</f>
         <v>-</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E7:E29" si="4">E6</f>
+        <f t="shared" ref="E7:E29" si="3">E6</f>
         <v>-</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ref="F7:F29" si="5">F6</f>
+        <f t="shared" ref="F7:F29" si="4">F6</f>
         <v>-</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" ref="G7:G29" si="6">G6</f>
+        <f t="shared" ref="G7:G29" si="5">G6</f>
         <v>-</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7:H29" si="7">H6</f>
+        <f t="shared" ref="H7:H29" si="6">H6</f>
         <v>-</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" ref="I7:J7" si="8">I6</f>
-        <v>-</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" ref="J7" si="9">J6</f>
-        <v>-</v>
+        <f t="shared" ref="I7" si="7">I6</f>
+        <v>-</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7" si="8">J6</f>
+        <v>100000000</v>
       </c>
       <c r="K7">
         <v>1.1000000000000001</v>
@@ -1458,32 +1347,32 @@
         <v>13</v>
       </c>
       <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E8" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E8" t="str">
+      <c r="F8" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I8" t="str">
-        <f t="shared" ref="I8:J8" si="10">I7</f>
-        <v>-</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" ref="J8" si="11">J7</f>
-        <v>-</v>
+        <f t="shared" ref="I8" si="9">I7</f>
+        <v>-</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8" si="10">J7</f>
+        <v>100000000</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1542,32 +1431,32 @@
         <v>14</v>
       </c>
       <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E9" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E9" t="str">
+      <c r="F9" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H9" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I9" t="str">
-        <f t="shared" ref="I9:J9" si="12">I8</f>
-        <v>-</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" ref="J9" si="13">J8</f>
-        <v>-</v>
+        <f t="shared" ref="I9" si="11">I8</f>
+        <v>-</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9" si="12">J8</f>
+        <v>100000000</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1626,32 +1515,32 @@
         <v>15</v>
       </c>
       <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E10" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E10" t="str">
+      <c r="F10" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I10" t="str">
-        <f t="shared" ref="I10:J10" si="14">I9</f>
-        <v>-</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" ref="J10" si="15">J9</f>
-        <v>-</v>
+        <f t="shared" ref="I10" si="13">I9</f>
+        <v>-</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10" si="14">J9</f>
+        <v>100000000</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1710,32 +1599,32 @@
         <v>16</v>
       </c>
       <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E11" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E11" t="str">
+      <c r="F11" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H11" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I11" t="str">
-        <f t="shared" ref="I11:J11" si="16">I10</f>
-        <v>-</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" ref="J11" si="17">J10</f>
-        <v>-</v>
+        <f t="shared" ref="I11" si="15">I10</f>
+        <v>-</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11" si="16">J10</f>
+        <v>100000000</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1794,32 +1683,32 @@
         <v>22</v>
       </c>
       <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E12" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E12" t="str">
+      <c r="F12" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H12" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I12" t="str">
-        <f t="shared" ref="I12:J12" si="18">I11</f>
-        <v>-</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" ref="J12" si="19">J11</f>
-        <v>-</v>
+        <f t="shared" ref="I12" si="17">I11</f>
+        <v>-</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J12" si="18">J11</f>
+        <v>100000000</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1878,32 +1767,32 @@
         <v>17</v>
       </c>
       <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E13" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E13" t="str">
+      <c r="F13" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H13" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13:J13" si="20">I12</f>
-        <v>-</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" ref="J13" si="21">J12</f>
-        <v>-</v>
+        <f t="shared" ref="I13" si="19">I12</f>
+        <v>-</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ref="J13" si="20">J12</f>
+        <v>100000000</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1962,32 +1851,32 @@
         <v>18</v>
       </c>
       <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E14" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E14" t="str">
+      <c r="F14" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H14" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I14" t="str">
-        <f t="shared" ref="I14:J14" si="22">I13</f>
-        <v>-</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" ref="J14" si="23">J13</f>
-        <v>-</v>
+        <f t="shared" ref="I14" si="21">I13</f>
+        <v>-</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14" si="22">J13</f>
+        <v>100000000</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -2046,32 +1935,32 @@
         <v>19</v>
       </c>
       <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E15" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E15" t="str">
+      <c r="F15" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H15" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I15" t="str">
-        <f t="shared" ref="I15:J15" si="24">I14</f>
-        <v>-</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" ref="J15" si="25">J14</f>
-        <v>-</v>
+        <f t="shared" ref="I15" si="23">I14</f>
+        <v>-</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ref="J15" si="24">J14</f>
+        <v>100000000</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2130,32 +2019,32 @@
         <v>20</v>
       </c>
       <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E16" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E16" t="str">
+      <c r="F16" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H16" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I16" t="str">
-        <f t="shared" ref="I16:J16" si="26">I15</f>
-        <v>-</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" ref="J16" si="27">J15</f>
-        <v>-</v>
+        <f t="shared" ref="I16" si="25">I15</f>
+        <v>-</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16" si="26">J15</f>
+        <v>100000000</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2214,32 +2103,32 @@
         <v>21</v>
       </c>
       <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E17" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E17" t="str">
+      <c r="F17" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H17" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I17" t="str">
-        <f t="shared" ref="I17:J17" si="28">I16</f>
-        <v>-</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" ref="J17" si="29">J16</f>
-        <v>-</v>
+        <f t="shared" ref="I17" si="27">I16</f>
+        <v>-</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17" si="28">J16</f>
+        <v>100000000</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2298,32 +2187,32 @@
         <v>23</v>
       </c>
       <c r="D18" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E18" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E18" t="str">
+      <c r="F18" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H18" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I18" t="str">
-        <f t="shared" ref="I18:J18" si="30">I17</f>
-        <v>-</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" ref="J18" si="31">J17</f>
-        <v>-</v>
+        <f t="shared" ref="I18" si="29">I17</f>
+        <v>-</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ref="J18" si="30">J17</f>
+        <v>100000000</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2382,32 +2271,32 @@
         <v>24</v>
       </c>
       <c r="D19" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E19" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E19" t="str">
+      <c r="F19" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H19" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I19" t="str">
-        <f t="shared" ref="I19:J19" si="32">I18</f>
-        <v>-</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" ref="J19" si="33">J18</f>
-        <v>-</v>
+        <f t="shared" ref="I19" si="31">I18</f>
+        <v>-</v>
+      </c>
+      <c r="J19">
+        <f t="shared" ref="J19" si="32">J18</f>
+        <v>100000000</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -2466,32 +2355,32 @@
         <v>25</v>
       </c>
       <c r="D20" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E20" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E20" t="str">
+      <c r="F20" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F20" t="str">
+      <c r="G20" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H20" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I20" t="str">
-        <f t="shared" ref="I20:J20" si="34">I19</f>
-        <v>-</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" ref="J20" si="35">J19</f>
-        <v>-</v>
+        <f t="shared" ref="I20" si="33">I19</f>
+        <v>-</v>
+      </c>
+      <c r="J20">
+        <f t="shared" ref="J20" si="34">J19</f>
+        <v>100000000</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -2550,32 +2439,32 @@
         <v>26</v>
       </c>
       <c r="D21" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E21" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E21" t="str">
+      <c r="F21" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F21" t="str">
+      <c r="G21" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G21" t="str">
+      <c r="H21" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H21" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I21" t="str">
-        <f t="shared" ref="I21:J21" si="36">I20</f>
-        <v>-</v>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" ref="J21" si="37">J20</f>
-        <v>-</v>
+        <f t="shared" ref="I21" si="35">I20</f>
+        <v>-</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ref="J21" si="36">J20</f>
+        <v>100000000</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -2634,32 +2523,32 @@
         <v>27</v>
       </c>
       <c r="D22" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E22" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E22" t="str">
+      <c r="F22" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F22" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G22" t="str">
+      <c r="H22" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H22" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I22" t="str">
-        <f t="shared" ref="I22:J22" si="38">I21</f>
-        <v>-</v>
-      </c>
-      <c r="J22" t="str">
-        <f t="shared" ref="J22" si="39">J21</f>
-        <v>-</v>
+        <f t="shared" ref="I22" si="37">I21</f>
+        <v>-</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22" si="38">J21</f>
+        <v>100000000</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -2718,32 +2607,32 @@
         <v>28</v>
       </c>
       <c r="D23" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E23" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E23" t="str">
+      <c r="F23" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F23" t="str">
+      <c r="G23" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G23" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H23" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I23" t="str">
-        <f t="shared" ref="I23:J23" si="40">I22</f>
-        <v>-</v>
-      </c>
-      <c r="J23" t="str">
-        <f t="shared" ref="J23" si="41">J22</f>
-        <v>-</v>
+        <f t="shared" ref="I23" si="39">I22</f>
+        <v>-</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23" si="40">J22</f>
+        <v>100000000</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2802,32 +2691,32 @@
         <v>29</v>
       </c>
       <c r="D24" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E24" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E24" t="str">
+      <c r="F24" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F24" t="str">
+      <c r="G24" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G24" t="str">
+      <c r="H24" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H24" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I24" t="str">
-        <f t="shared" ref="I24:J24" si="42">I23</f>
-        <v>-</v>
-      </c>
-      <c r="J24" t="str">
-        <f t="shared" ref="J24" si="43">J23</f>
-        <v>-</v>
+        <f t="shared" ref="I24" si="41">I23</f>
+        <v>-</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24" si="42">J23</f>
+        <v>100000000</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -2886,32 +2775,32 @@
         <v>30</v>
       </c>
       <c r="D25" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E25" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E25" t="str">
+      <c r="F25" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F25" t="str">
+      <c r="G25" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G25" t="str">
+      <c r="H25" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H25" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I25" t="str">
-        <f t="shared" ref="I25:J25" si="44">I24</f>
-        <v>-</v>
-      </c>
-      <c r="J25" t="str">
-        <f t="shared" ref="J25" si="45">J24</f>
-        <v>-</v>
+        <f t="shared" ref="I25" si="43">I24</f>
+        <v>-</v>
+      </c>
+      <c r="J25">
+        <f t="shared" ref="J25" si="44">J24</f>
+        <v>100000000</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -2970,32 +2859,32 @@
         <v>31</v>
       </c>
       <c r="D26" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E26" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E26" t="str">
+      <c r="F26" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F26" t="str">
+      <c r="G26" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G26" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H26" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I26" t="str">
-        <f t="shared" ref="I26:J26" si="46">I25</f>
-        <v>-</v>
-      </c>
-      <c r="J26" t="str">
-        <f t="shared" ref="J26" si="47">J25</f>
-        <v>-</v>
+        <f t="shared" ref="I26" si="45">I25</f>
+        <v>-</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ref="J26" si="46">J25</f>
+        <v>100000000</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -3054,32 +2943,32 @@
         <v>32</v>
       </c>
       <c r="D27" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E27" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E27" t="str">
+      <c r="F27" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F27" t="str">
+      <c r="G27" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G27" t="str">
+      <c r="H27" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H27" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I27" t="str">
-        <f t="shared" ref="I27:J27" si="48">I26</f>
-        <v>-</v>
-      </c>
-      <c r="J27" t="str">
-        <f t="shared" ref="J27" si="49">J26</f>
-        <v>-</v>
+        <f t="shared" ref="I27" si="47">I26</f>
+        <v>-</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27" si="48">J26</f>
+        <v>100000000</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3138,32 +3027,32 @@
         <v>33</v>
       </c>
       <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E28" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E28" t="str">
+      <c r="F28" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F28" t="str">
+      <c r="G28" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H28" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I28" t="str">
-        <f t="shared" ref="I28:J28" si="50">I27</f>
-        <v>-</v>
-      </c>
-      <c r="J28" t="str">
-        <f t="shared" ref="J28" si="51">J27</f>
-        <v>-</v>
+        <f t="shared" ref="I28" si="49">I27</f>
+        <v>-</v>
+      </c>
+      <c r="J28">
+        <f t="shared" ref="J28" si="50">J27</f>
+        <v>100000000</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -3222,32 +3111,32 @@
         <v>34</v>
       </c>
       <c r="D29" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="E29" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E29" t="str">
+      <c r="F29" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="F29" t="str">
+      <c r="G29" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="G29" t="str">
+      <c r="H29" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="H29" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
       <c r="I29" t="str">
-        <f t="shared" ref="I29:J29" si="52">I28</f>
-        <v>-</v>
-      </c>
-      <c r="J29" t="str">
-        <f t="shared" ref="J29" si="53">J28</f>
-        <v>-</v>
+        <f t="shared" ref="I29" si="51">I28</f>
+        <v>-</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ref="J29" si="52">J28</f>
+        <v>100000000</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -3298,16 +3187,16 @@
   </sheetData>
   <autoFilter ref="C4:V5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="1" priority="23" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
poc changes, dtype in divide function
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F3DCAD-F0D4-4288-A404-CAB5580BAD35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF82104-0302-4E89-BA89-A2385D14EB53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="30750" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -801,16 +801,16 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.54296875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>45</v>
       </c>
@@ -887,7 +887,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:26" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -1252,9 +1252,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -1336,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
pyomo component del update
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF82104-0302-4E89-BA89-A2385D14EB53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B89DA3-4F60-4699-AA70-69343606D978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30750" yWindow="1950" windowWidth="21600" windowHeight="11325" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -801,16 +801,16 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="17.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>45</v>
       </c>
@@ -887,7 +887,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
     </row>
-    <row r="4" spans="1:26" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="b">
         <v>0</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="b">
         <v>1</v>
       </c>
@@ -1336,9 +1336,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -1420,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
exp.py update to get the run selection working
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B89DA3-4F60-4699-AA70-69343606D978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AE1A17-6F14-446C-B120-A46EC3B8FC32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -798,10 +798,10 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="L26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="Z6" sqref="Z6:Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1251,10 +1251,14 @@
       <c r="Y6">
         <v>1</v>
       </c>
+      <c r="Z6">
+        <f>Z5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -1335,10 +1339,14 @@
       <c r="Y7">
         <v>1</v>
       </c>
+      <c r="Z7">
+        <f t="shared" ref="Z7:Z29" si="9">Z6</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
@@ -1367,11 +1375,11 @@
         <v>-</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" ref="I8" si="9">I7</f>
+        <f t="shared" ref="I8" si="10">I7</f>
         <v>-</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8" si="10">J7</f>
+        <f t="shared" ref="J8" si="11">J7</f>
         <v>100000000</v>
       </c>
       <c r="K8">
@@ -1418,6 +1426,10 @@
       </c>
       <c r="Y8">
         <v>1</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
@@ -1451,11 +1463,11 @@
         <v>-</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" ref="I9" si="11">I8</f>
+        <f t="shared" ref="I9" si="12">I8</f>
         <v>-</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J9" si="12">J8</f>
+        <f t="shared" ref="J9" si="13">J8</f>
         <v>100000000</v>
       </c>
       <c r="K9">
@@ -1502,6 +1514,10 @@
       </c>
       <c r="Y9">
         <v>1</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.35">
@@ -1535,11 +1551,11 @@
         <v>-</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" ref="I10" si="13">I9</f>
+        <f t="shared" ref="I10" si="14">I9</f>
         <v>-</v>
       </c>
       <c r="J10">
-        <f t="shared" ref="J10" si="14">J9</f>
+        <f t="shared" ref="J10" si="15">J9</f>
         <v>100000000</v>
       </c>
       <c r="K10">
@@ -1586,6 +1602,10 @@
       </c>
       <c r="Y10">
         <v>1</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.35">
@@ -1619,11 +1639,11 @@
         <v>-</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" ref="I11" si="15">I10</f>
+        <f t="shared" ref="I11" si="16">I10</f>
         <v>-</v>
       </c>
       <c r="J11">
-        <f t="shared" ref="J11" si="16">J10</f>
+        <f t="shared" ref="J11" si="17">J10</f>
         <v>100000000</v>
       </c>
       <c r="K11">
@@ -1670,6 +1690,10 @@
       </c>
       <c r="Y11">
         <v>1</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.35">
@@ -1703,11 +1727,11 @@
         <v>-</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" ref="I12" si="17">I11</f>
+        <f t="shared" ref="I12" si="18">I11</f>
         <v>-</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12" si="18">J11</f>
+        <f t="shared" ref="J12" si="19">J11</f>
         <v>100000000</v>
       </c>
       <c r="K12">
@@ -1754,6 +1778,10 @@
       </c>
       <c r="Y12">
         <v>1</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.35">
@@ -1787,11 +1815,11 @@
         <v>-</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13" si="19">I12</f>
+        <f t="shared" ref="I13" si="20">I12</f>
         <v>-</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13" si="20">J12</f>
+        <f t="shared" ref="J13" si="21">J12</f>
         <v>100000000</v>
       </c>
       <c r="K13">
@@ -1838,6 +1866,10 @@
       </c>
       <c r="Y13">
         <v>1</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.35">
@@ -1871,11 +1903,11 @@
         <v>-</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" ref="I14" si="21">I13</f>
+        <f t="shared" ref="I14" si="22">I13</f>
         <v>-</v>
       </c>
       <c r="J14">
-        <f t="shared" ref="J14" si="22">J13</f>
+        <f t="shared" ref="J14" si="23">J13</f>
         <v>100000000</v>
       </c>
       <c r="K14">
@@ -1922,6 +1954,10 @@
       </c>
       <c r="Y14">
         <v>1</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.35">
@@ -1955,11 +1991,11 @@
         <v>-</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" ref="I15" si="23">I14</f>
+        <f t="shared" ref="I15" si="24">I14</f>
         <v>-</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15" si="24">J14</f>
+        <f t="shared" ref="J15" si="25">J14</f>
         <v>100000000</v>
       </c>
       <c r="K15">
@@ -2006,6 +2042,10 @@
       </c>
       <c r="Y15">
         <v>1</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
@@ -2039,11 +2079,11 @@
         <v>-</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" ref="I16" si="25">I15</f>
+        <f t="shared" ref="I16" si="26">I15</f>
         <v>-</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16" si="26">J15</f>
+        <f t="shared" ref="J16" si="27">J15</f>
         <v>100000000</v>
       </c>
       <c r="K16">
@@ -2091,8 +2131,12 @@
       <c r="Y16">
         <v>1</v>
       </c>
+      <c r="Z16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -2123,11 +2167,11 @@
         <v>-</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" ref="I17" si="27">I16</f>
+        <f t="shared" ref="I17" si="28">I16</f>
         <v>-</v>
       </c>
       <c r="J17">
-        <f t="shared" ref="J17" si="28">J16</f>
+        <f t="shared" ref="J17" si="29">J16</f>
         <v>100000000</v>
       </c>
       <c r="K17">
@@ -2175,8 +2219,12 @@
       <c r="Y17">
         <v>1</v>
       </c>
+      <c r="Z17">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -2207,11 +2255,11 @@
         <v>-</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" ref="I18" si="29">I17</f>
+        <f t="shared" ref="I18" si="30">I17</f>
         <v>-</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18" si="30">J17</f>
+        <f t="shared" ref="J18" si="31">J17</f>
         <v>100000000</v>
       </c>
       <c r="K18">
@@ -2259,8 +2307,12 @@
       <c r="Y18">
         <v>1</v>
       </c>
+      <c r="Z18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -2291,11 +2343,11 @@
         <v>-</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" ref="I19" si="31">I18</f>
+        <f t="shared" ref="I19" si="32">I18</f>
         <v>-</v>
       </c>
       <c r="J19">
-        <f t="shared" ref="J19" si="32">J18</f>
+        <f t="shared" ref="J19" si="33">J18</f>
         <v>100000000</v>
       </c>
       <c r="K19">
@@ -2343,8 +2395,12 @@
       <c r="Y19">
         <v>1</v>
       </c>
+      <c r="Z19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -2375,11 +2431,11 @@
         <v>-</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" ref="I20" si="33">I19</f>
+        <f t="shared" ref="I20" si="34">I19</f>
         <v>-</v>
       </c>
       <c r="J20">
-        <f t="shared" ref="J20" si="34">J19</f>
+        <f t="shared" ref="J20" si="35">J19</f>
         <v>100000000</v>
       </c>
       <c r="K20">
@@ -2427,8 +2483,12 @@
       <c r="Y20">
         <v>1</v>
       </c>
+      <c r="Z20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -2459,11 +2519,11 @@
         <v>-</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" ref="I21" si="35">I20</f>
+        <f t="shared" ref="I21" si="36">I20</f>
         <v>-</v>
       </c>
       <c r="J21">
-        <f t="shared" ref="J21" si="36">J20</f>
+        <f t="shared" ref="J21" si="37">J20</f>
         <v>100000000</v>
       </c>
       <c r="K21">
@@ -2511,8 +2571,12 @@
       <c r="Y21">
         <v>1</v>
       </c>
+      <c r="Z21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -2543,11 +2607,11 @@
         <v>-</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" ref="I22" si="37">I21</f>
+        <f t="shared" ref="I22" si="38">I21</f>
         <v>-</v>
       </c>
       <c r="J22">
-        <f t="shared" ref="J22" si="38">J21</f>
+        <f t="shared" ref="J22" si="39">J21</f>
         <v>100000000</v>
       </c>
       <c r="K22">
@@ -2595,8 +2659,12 @@
       <c r="Y22">
         <v>1</v>
       </c>
+      <c r="Z22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2627,11 +2695,11 @@
         <v>-</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" ref="I23" si="39">I22</f>
+        <f t="shared" ref="I23" si="40">I22</f>
         <v>-</v>
       </c>
       <c r="J23">
-        <f t="shared" ref="J23" si="40">J22</f>
+        <f t="shared" ref="J23" si="41">J22</f>
         <v>100000000</v>
       </c>
       <c r="K23">
@@ -2679,8 +2747,12 @@
       <c r="Y23">
         <v>1</v>
       </c>
+      <c r="Z23">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2711,11 +2783,11 @@
         <v>-</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" ref="I24" si="41">I23</f>
+        <f t="shared" ref="I24" si="42">I23</f>
         <v>-</v>
       </c>
       <c r="J24">
-        <f t="shared" ref="J24" si="42">J23</f>
+        <f t="shared" ref="J24" si="43">J23</f>
         <v>100000000</v>
       </c>
       <c r="K24">
@@ -2763,8 +2835,12 @@
       <c r="Y24">
         <v>1</v>
       </c>
+      <c r="Z24">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2795,11 +2871,11 @@
         <v>-</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" ref="I25" si="43">I24</f>
+        <f t="shared" ref="I25" si="44">I24</f>
         <v>-</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25" si="44">J24</f>
+        <f t="shared" ref="J25" si="45">J24</f>
         <v>100000000</v>
       </c>
       <c r="K25">
@@ -2847,8 +2923,12 @@
       <c r="Y25">
         <v>1</v>
       </c>
+      <c r="Z25">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2879,11 +2959,11 @@
         <v>-</v>
       </c>
       <c r="I26" t="str">
-        <f t="shared" ref="I26" si="45">I25</f>
+        <f t="shared" ref="I26" si="46">I25</f>
         <v>-</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26" si="46">J25</f>
+        <f t="shared" ref="J26" si="47">J25</f>
         <v>100000000</v>
       </c>
       <c r="K26">
@@ -2931,8 +3011,12 @@
       <c r="Y26">
         <v>1</v>
       </c>
+      <c r="Z26">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -2963,11 +3047,11 @@
         <v>-</v>
       </c>
       <c r="I27" t="str">
-        <f t="shared" ref="I27" si="47">I26</f>
+        <f t="shared" ref="I27" si="48">I26</f>
         <v>-</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="J27" si="48">J26</f>
+        <f t="shared" ref="J27" si="49">J26</f>
         <v>100000000</v>
       </c>
       <c r="K27">
@@ -3015,8 +3099,12 @@
       <c r="Y27">
         <v>1</v>
       </c>
+      <c r="Z27">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -3047,11 +3135,11 @@
         <v>-</v>
       </c>
       <c r="I28" t="str">
-        <f t="shared" ref="I28" si="49">I27</f>
+        <f t="shared" ref="I28" si="50">I27</f>
         <v>-</v>
       </c>
       <c r="J28">
-        <f t="shared" ref="J28" si="50">J27</f>
+        <f t="shared" ref="J28" si="51">J27</f>
         <v>100000000</v>
       </c>
       <c r="K28">
@@ -3099,8 +3187,12 @@
       <c r="Y28">
         <v>1</v>
       </c>
+      <c r="Z28">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -3131,11 +3223,11 @@
         <v>-</v>
       </c>
       <c r="I29" t="str">
-        <f t="shared" ref="I29" si="51">I28</f>
+        <f t="shared" ref="I29" si="52">I28</f>
         <v>-</v>
       </c>
       <c r="J29">
-        <f t="shared" ref="J29" si="52">J28</f>
+        <f t="shared" ref="J29" si="53">J28</f>
         <v>100000000</v>
       </c>
       <c r="K29">
@@ -3182,6 +3274,10 @@
       </c>
       <c r="Y29">
         <v>1</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tidy set definitions up a little (still need to change feed period set and maybe labour) changed input headers to all start from 0
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AE1A17-6F14-446C-B120-A46EC3B8FC32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F51B810-875A-4747-B7BF-D4F605639511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -798,10 +798,10 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="L26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Z6" sqref="Z6:Z29"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1204,7 +1204,7 @@
         <v>-</v>
       </c>
       <c r="J6">
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K6">
         <v>0.9</v>
@@ -1292,7 +1292,7 @@
       </c>
       <c r="J7">
         <f t="shared" ref="J7" si="8">J6</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K7">
         <v>1.1000000000000001</v>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="J8">
         <f t="shared" ref="J8" si="11">J7</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="J9">
         <f t="shared" ref="J9" si="13">J8</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="J10">
         <f t="shared" ref="J10" si="15">J9</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="J11">
         <f t="shared" ref="J11" si="17">J10</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="J12">
         <f t="shared" ref="J12" si="19">J11</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1820,7 +1820,7 @@
       </c>
       <c r="J13">
         <f t="shared" ref="J13" si="21">J12</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="J14">
         <f t="shared" ref="J14" si="23">J13</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="J15">
         <f t="shared" ref="J15" si="25">J14</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="J16">
         <f t="shared" ref="J16" si="27">J15</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="J17">
         <f t="shared" ref="J17" si="29">J16</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="J18">
         <f t="shared" ref="J18" si="31">J17</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2348,7 +2348,7 @@
       </c>
       <c r="J19">
         <f t="shared" ref="J19" si="33">J18</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="J20">
         <f t="shared" ref="J20" si="35">J19</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="J21">
         <f t="shared" ref="J21" si="37">J20</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -2612,7 +2612,7 @@
       </c>
       <c r="J22">
         <f t="shared" ref="J22" si="39">J21</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="J23">
         <f t="shared" ref="J23" si="41">J22</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="J24">
         <f t="shared" ref="J24" si="43">J23</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="J25">
         <f t="shared" ref="J25" si="45">J24</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="J26">
         <f t="shared" ref="J26" si="47">J25</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -3052,7 +3052,7 @@
       </c>
       <c r="J27">
         <f t="shared" ref="J27" si="49">J26</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="J28">
         <f t="shared" ref="J28" si="51">J27</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -3228,7 +3228,7 @@
       </c>
       <c r="J29">
         <f t="shared" ref="J29" si="53">J28</f>
-        <v>100000000</v>
+        <v>9999</v>
       </c>
       <c r="K29">
         <v>1</v>

</xml_diff>

<commit_message>
fixed pyomo not running.
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F51B810-875A-4747-B7BF-D4F605639511}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4854B8E5-225A-4DA0-B441-088E2F8ECA31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -801,7 +801,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1100,9 +1100,8 @@
         <f t="array" ref="I5">_xlfn.IFS(OR(I1="sam",I1="sai"),1,I1="sav","-",OR(I1="sap",I1="saa"),0)</f>
         <v>-</v>
       </c>
-      <c r="J5" s="9" t="str" cm="1">
-        <f t="array" ref="J5">_xlfn.IFS(OR(J1="sam",J1="sai"),1,J1="sav","-",OR(J1="sap",J1="saa"),0)</f>
-        <v>-</v>
+      <c r="J5" s="9">
+        <v>1</v>
       </c>
       <c r="K5" s="9" cm="1">
         <f t="array" ref="K5">_xlfn.IFS(OR(K1="sam",K1="sai"),1,K1="sav","-",OR(K1="sap",K1="saa"),0)</f>
@@ -1204,10 +1203,10 @@
         <v>-</v>
       </c>
       <c r="J6">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -1292,7 +1291,7 @@
       </c>
       <c r="J7">
         <f t="shared" ref="J7" si="8">J6</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>1.1000000000000001</v>
@@ -1380,7 +1379,7 @@
       </c>
       <c r="J8">
         <f t="shared" ref="J8" si="11">J7</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1468,7 +1467,7 @@
       </c>
       <c r="J9">
         <f t="shared" ref="J9" si="13">J8</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1556,7 +1555,7 @@
       </c>
       <c r="J10">
         <f t="shared" ref="J10" si="15">J9</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1644,7 +1643,7 @@
       </c>
       <c r="J11">
         <f t="shared" ref="J11" si="17">J10</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1732,7 +1731,7 @@
       </c>
       <c r="J12">
         <f t="shared" ref="J12" si="19">J11</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1820,7 +1819,7 @@
       </c>
       <c r="J13">
         <f t="shared" ref="J13" si="21">J12</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1908,7 +1907,7 @@
       </c>
       <c r="J14">
         <f t="shared" ref="J14" si="23">J13</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1996,7 +1995,7 @@
       </c>
       <c r="J15">
         <f t="shared" ref="J15" si="25">J14</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2084,7 +2083,7 @@
       </c>
       <c r="J16">
         <f t="shared" ref="J16" si="27">J15</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2172,7 +2171,7 @@
       </c>
       <c r="J17">
         <f t="shared" ref="J17" si="29">J16</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2260,7 +2259,7 @@
       </c>
       <c r="J18">
         <f t="shared" ref="J18" si="31">J17</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2348,7 +2347,7 @@
       </c>
       <c r="J19">
         <f t="shared" ref="J19" si="33">J18</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -2436,7 +2435,7 @@
       </c>
       <c r="J20">
         <f t="shared" ref="J20" si="35">J19</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -2524,7 +2523,7 @@
       </c>
       <c r="J21">
         <f t="shared" ref="J21" si="37">J20</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -2612,7 +2611,7 @@
       </c>
       <c r="J22">
         <f t="shared" ref="J22" si="39">J21</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -2700,7 +2699,7 @@
       </c>
       <c r="J23">
         <f t="shared" ref="J23" si="41">J22</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2788,7 +2787,7 @@
       </c>
       <c r="J24">
         <f t="shared" ref="J24" si="43">J23</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -2876,7 +2875,7 @@
       </c>
       <c r="J25">
         <f t="shared" ref="J25" si="45">J24</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -2964,7 +2963,7 @@
       </c>
       <c r="J26">
         <f t="shared" ref="J26" si="47">J25</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -3052,7 +3051,7 @@
       </c>
       <c r="J27">
         <f t="shared" ref="J27" si="49">J26</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3140,7 +3139,7 @@
       </c>
       <c r="J28">
         <f t="shared" ref="J28" si="51">J27</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -3228,7 +3227,7 @@
       </c>
       <c r="J29">
         <f t="shared" ref="J29" si="53">J28</f>
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="K29">
         <v>1</v>

</xml_diff>

<commit_message>
force precalcs option added in exp.py
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ADF94A-8752-4F28-BEF4-3B41A768D3C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB9EAC0-E917-43F2-B84F-AE36C1C60F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -801,7 +801,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1100,8 +1100,9 @@
         <f t="array" ref="I5">_xlfn.IFS(OR(I1="sam",I1="sai"),1,I1="sav","-",OR(I1="sap",I1="saa"),0)</f>
         <v>-</v>
       </c>
-      <c r="J5" s="9">
-        <v>1</v>
+      <c r="J5" s="9" t="str" cm="1">
+        <f t="array" ref="J5">_xlfn.IFS(OR(J1="sam",J1="sai"),1,J1="sav","-",OR(J1="sap",J1="saa"),0)</f>
+        <v>-</v>
       </c>
       <c r="K5" s="9" cm="1">
         <f t="array" ref="K5">_xlfn.IFS(OR(K1="sam",K1="sai"),1,K1="sav","-",OR(K1="sap",K1="saa"),0)</f>
@@ -1203,7 +1204,7 @@
         <v>-</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K6">
         <v>0.9</v>
@@ -1291,7 +1292,7 @@
       </c>
       <c r="J7">
         <f t="shared" ref="J7" si="8">J6</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K7">
         <v>1.1000000000000001</v>
@@ -1379,7 +1380,7 @@
       </c>
       <c r="J8">
         <f t="shared" ref="J8" si="11">J7</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1467,7 +1468,7 @@
       </c>
       <c r="J9">
         <f t="shared" ref="J9" si="13">J8</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1555,7 +1556,7 @@
       </c>
       <c r="J10">
         <f t="shared" ref="J10" si="15">J9</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1643,7 +1644,7 @@
       </c>
       <c r="J11">
         <f t="shared" ref="J11" si="17">J10</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1731,7 +1732,7 @@
       </c>
       <c r="J12">
         <f t="shared" ref="J12" si="19">J11</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1819,7 +1820,7 @@
       </c>
       <c r="J13">
         <f t="shared" ref="J13" si="21">J12</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1907,7 +1908,7 @@
       </c>
       <c r="J14">
         <f t="shared" ref="J14" si="23">J13</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1995,7 +1996,7 @@
       </c>
       <c r="J15">
         <f t="shared" ref="J15" si="25">J14</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2083,7 +2084,7 @@
       </c>
       <c r="J16">
         <f t="shared" ref="J16" si="27">J15</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2171,7 +2172,7 @@
       </c>
       <c r="J17">
         <f t="shared" ref="J17" si="29">J16</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2259,7 +2260,7 @@
       </c>
       <c r="J18">
         <f t="shared" ref="J18" si="31">J17</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2347,7 +2348,7 @@
       </c>
       <c r="J19">
         <f t="shared" ref="J19" si="33">J18</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -2435,7 +2436,7 @@
       </c>
       <c r="J20">
         <f t="shared" ref="J20" si="35">J19</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -2523,7 +2524,7 @@
       </c>
       <c r="J21">
         <f t="shared" ref="J21" si="37">J20</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -2611,7 +2612,7 @@
       </c>
       <c r="J22">
         <f t="shared" ref="J22" si="39">J21</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -2699,7 +2700,7 @@
       </c>
       <c r="J23">
         <f t="shared" ref="J23" si="41">J22</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2787,7 +2788,7 @@
       </c>
       <c r="J24">
         <f t="shared" ref="J24" si="43">J23</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -2875,7 +2876,7 @@
       </c>
       <c r="J25">
         <f t="shared" ref="J25" si="45">J24</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -2963,7 +2964,7 @@
       </c>
       <c r="J26">
         <f t="shared" ref="J26" si="47">J25</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -3051,7 +3052,7 @@
       </c>
       <c r="J27">
         <f t="shared" ref="J27" si="49">J26</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3139,7 +3140,7 @@
       </c>
       <c r="J28">
         <f t="shared" ref="J28" si="51">J27</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -3227,7 +3228,7 @@
       </c>
       <c r="J29">
         <f t="shared" ref="J29" si="53">J28</f>
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="K29">
         <v>1</v>

</xml_diff>

<commit_message>
update BoundsPyomo.py errosion constraint stoping pasture rotations
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB9EAC0-E917-43F2-B84F-AE36C1C60F3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F029CF7B-AD4B-4872-831B-5C9BC4E596A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -801,7 +801,7 @@
       <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1200,11 +1200,12 @@
         <v>-</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6" si="1">I5</f>
-        <v>-</v>
-      </c>
-      <c r="J6">
-        <v>900</v>
+        <f t="shared" ref="I6:J6" si="1">I5</f>
+        <v>-</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
       <c r="K6">
         <v>0.9</v>
@@ -1290,9 +1291,9 @@
         <f t="shared" ref="I7" si="7">I6</f>
         <v>-</v>
       </c>
-      <c r="J7">
+      <c r="J7" t="str">
         <f t="shared" ref="J7" si="8">J6</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K7">
         <v>1.1000000000000001</v>
@@ -1378,9 +1379,9 @@
         <f t="shared" ref="I8" si="10">I7</f>
         <v>-</v>
       </c>
-      <c r="J8">
+      <c r="J8" t="str">
         <f t="shared" ref="J8" si="11">J7</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1466,9 +1467,9 @@
         <f t="shared" ref="I9" si="12">I8</f>
         <v>-</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="str">
         <f t="shared" ref="J9" si="13">J8</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1554,9 +1555,9 @@
         <f t="shared" ref="I10" si="14">I9</f>
         <v>-</v>
       </c>
-      <c r="J10">
+      <c r="J10" t="str">
         <f t="shared" ref="J10" si="15">J9</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1642,9 +1643,9 @@
         <f t="shared" ref="I11" si="16">I10</f>
         <v>-</v>
       </c>
-      <c r="J11">
+      <c r="J11" t="str">
         <f t="shared" ref="J11" si="17">J10</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1730,9 +1731,9 @@
         <f t="shared" ref="I12" si="18">I11</f>
         <v>-</v>
       </c>
-      <c r="J12">
+      <c r="J12" t="str">
         <f t="shared" ref="J12" si="19">J11</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1818,9 +1819,9 @@
         <f t="shared" ref="I13" si="20">I12</f>
         <v>-</v>
       </c>
-      <c r="J13">
+      <c r="J13" t="str">
         <f t="shared" ref="J13" si="21">J12</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1906,9 +1907,9 @@
         <f t="shared" ref="I14" si="22">I13</f>
         <v>-</v>
       </c>
-      <c r="J14">
+      <c r="J14" t="str">
         <f t="shared" ref="J14" si="23">J13</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1994,9 +1995,9 @@
         <f t="shared" ref="I15" si="24">I14</f>
         <v>-</v>
       </c>
-      <c r="J15">
+      <c r="J15" t="str">
         <f t="shared" ref="J15" si="25">J14</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2082,9 +2083,9 @@
         <f t="shared" ref="I16" si="26">I15</f>
         <v>-</v>
       </c>
-      <c r="J16">
+      <c r="J16" t="str">
         <f t="shared" ref="J16" si="27">J15</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2170,9 +2171,9 @@
         <f t="shared" ref="I17" si="28">I16</f>
         <v>-</v>
       </c>
-      <c r="J17">
+      <c r="J17" t="str">
         <f t="shared" ref="J17" si="29">J16</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -2258,9 +2259,9 @@
         <f t="shared" ref="I18" si="30">I17</f>
         <v>-</v>
       </c>
-      <c r="J18">
+      <c r="J18" t="str">
         <f t="shared" ref="J18" si="31">J17</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -2346,9 +2347,9 @@
         <f t="shared" ref="I19" si="32">I18</f>
         <v>-</v>
       </c>
-      <c r="J19">
+      <c r="J19" t="str">
         <f t="shared" ref="J19" si="33">J18</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -2434,9 +2435,9 @@
         <f t="shared" ref="I20" si="34">I19</f>
         <v>-</v>
       </c>
-      <c r="J20">
+      <c r="J20" t="str">
         <f t="shared" ref="J20" si="35">J19</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -2522,9 +2523,9 @@
         <f t="shared" ref="I21" si="36">I20</f>
         <v>-</v>
       </c>
-      <c r="J21">
+      <c r="J21" t="str">
         <f t="shared" ref="J21" si="37">J20</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -2610,9 +2611,9 @@
         <f t="shared" ref="I22" si="38">I21</f>
         <v>-</v>
       </c>
-      <c r="J22">
+      <c r="J22" t="str">
         <f t="shared" ref="J22" si="39">J21</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -2698,9 +2699,9 @@
         <f t="shared" ref="I23" si="40">I22</f>
         <v>-</v>
       </c>
-      <c r="J23">
+      <c r="J23" t="str">
         <f t="shared" ref="J23" si="41">J22</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -2786,9 +2787,9 @@
         <f t="shared" ref="I24" si="42">I23</f>
         <v>-</v>
       </c>
-      <c r="J24">
+      <c r="J24" t="str">
         <f t="shared" ref="J24" si="43">J23</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -2874,9 +2875,9 @@
         <f t="shared" ref="I25" si="44">I24</f>
         <v>-</v>
       </c>
-      <c r="J25">
+      <c r="J25" t="str">
         <f t="shared" ref="J25" si="45">J24</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -2962,9 +2963,9 @@
         <f t="shared" ref="I26" si="46">I25</f>
         <v>-</v>
       </c>
-      <c r="J26">
+      <c r="J26" t="str">
         <f t="shared" ref="J26" si="47">J25</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -3050,9 +3051,9 @@
         <f t="shared" ref="I27" si="48">I26</f>
         <v>-</v>
       </c>
-      <c r="J27">
+      <c r="J27" t="str">
         <f t="shared" ref="J27" si="49">J26</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3138,9 +3139,9 @@
         <f t="shared" ref="I28" si="50">I27</f>
         <v>-</v>
       </c>
-      <c r="J28">
+      <c r="J28" t="str">
         <f t="shared" ref="J28" si="51">J27</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -3226,9 +3227,9 @@
         <f t="shared" ref="I29" si="52">I28</f>
         <v>-</v>
       </c>
-      <c r="J29">
+      <c r="J29" t="str">
         <f t="shared" ref="J29" si="53">J28</f>
-        <v>900</v>
+        <v>-</v>
       </c>
       <c r="K29">
         <v>1</v>

</xml_diff>

<commit_message>
reports partly updated and exp.xl updated
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F029CF7B-AD4B-4872-831B-5C9BC4E596A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40DD900-0640-4764-96A4-107CAEB48152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$V$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$X$5</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
   <si>
     <t>sam</t>
   </si>
@@ -318,6 +318,24 @@
   </si>
   <si>
     <t>woolp_mpg</t>
+  </si>
+  <si>
+    <t>bnd_total_pas_area</t>
+  </si>
+  <si>
+    <t>bnd_pasarea_inc</t>
+  </si>
+  <si>
+    <t>Pas area 20%</t>
+  </si>
+  <si>
+    <t>Pas area 40%</t>
+  </si>
+  <si>
+    <t>Pas area 60%</t>
+  </si>
+  <si>
+    <t>Pas area 80%</t>
   </si>
 </sst>
 </file>
@@ -795,22 +813,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6:J6"/>
+      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="17.54296875" style="3" customWidth="1"/>
     <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>45</v>
       </c>
@@ -839,10 +858,10 @@
         <v>43</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>0</v>
@@ -875,19 +894,25 @@
         <v>0</v>
       </c>
       <c r="W1" s="6" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="X1" s="6" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="Y1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
@@ -913,14 +938,14 @@
         <v>49</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="N2" s="6" t="s">
         <v>1</v>
       </c>
@@ -931,13 +956,13 @@
         <v>1</v>
       </c>
       <c r="Q2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="T2" s="6" t="s">
         <v>10</v>
@@ -948,11 +973,17 @@
       <c r="V2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
+      <c r="W2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
@@ -963,12 +994,8 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
       <c r="M3" s="6" t="s">
         <v>6</v>
       </c>
@@ -999,11 +1026,17 @@
       <c r="V3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
+      <c r="W3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
     </row>
-    <row r="4" spans="1:26" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1030,45 +1063,47 @@
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7" t="s">
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="O4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7" t="s">
+      <c r="S4" s="7"/>
+      <c r="T4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="U4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
       <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1104,13 +1139,13 @@
         <f t="array" ref="J5">_xlfn.IFS(OR(J1="sam",J1="sai"),1,J1="sav","-",OR(J1="sap",J1="saa"),0)</f>
         <v>-</v>
       </c>
-      <c r="K5" s="9" cm="1">
+      <c r="K5" s="9" t="str" cm="1">
         <f t="array" ref="K5">_xlfn.IFS(OR(K1="sam",K1="sai"),1,K1="sav","-",OR(K1="sap",K1="saa"),0)</f>
-        <v>1</v>
-      </c>
-      <c r="L5" s="9" cm="1">
+        <v>-</v>
+      </c>
+      <c r="L5" s="9" t="str" cm="1">
         <f t="array" ref="L5">_xlfn.IFS(OR(L1="sam",L1="sai"),1,L1="sav","-",OR(L1="sap",L1="saa"),0)</f>
-        <v>1</v>
+        <v>-</v>
       </c>
       <c r="M5" s="9" cm="1">
         <f t="array" ref="M5">_xlfn.IFS(OR(M1="sam",M1="sai"),1,M1="sav","-",OR(M1="sap",M1="saa"),0)</f>
@@ -1154,11 +1189,11 @@
       </c>
       <c r="W5" s="9" cm="1">
         <f t="array" ref="W5">_xlfn.IFS(OR(W1="sam",W1="sai"),1,W1="sav","-",OR(W1="sap",W1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5" s="9" cm="1">
         <f t="array" ref="X5">_xlfn.IFS(OR(X1="sam",X1="sai"),1,X1="sav","-",OR(X1="sap",X1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5" s="9" cm="1">
         <f t="array" ref="Y5">_xlfn.IFS(OR(Y1="sam",Y1="sai"),1,Y1="sav","-",OR(Y1="sap",Y1="saa"),0)</f>
@@ -1168,13 +1203,21 @@
         <f t="array" ref="Z5">_xlfn.IFS(OR(Z1="sam",Z1="sai"),1,Z1="sav","-",OR(Z1="sap",Z1="saa"),0)</f>
         <v>0</v>
       </c>
+      <c r="AA5" s="9" cm="1">
+        <f t="array" ref="AA5">_xlfn.IFS(OR(AA1="sam",AA1="sai"),1,AA1="sav","-",OR(AA1="sap",AA1="saa"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="9" cm="1">
+        <f t="array" ref="AB5">_xlfn.IFS(OR(AB1="sam",AB1="sai"),1,AB1="sav","-",OR(AB1="sap",AB1="saa"),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="b">
         <v>1</v>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>11</v>
@@ -1200,22 +1243,24 @@
         <v>-</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6:J6" si="1">I5</f>
+        <f t="shared" ref="I6:L6" si="1">I5</f>
         <v>-</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="K6">
+      <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="M6">
         <v>0.9</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
       <c r="N6">
         <v>1</v>
       </c>
@@ -1253,11 +1298,17 @@
         <v>1</v>
       </c>
       <c r="Z6">
-        <f>Z5</f>
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <f>AB5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="b">
         <v>0</v>
       </c>
@@ -1268,7 +1319,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D7:D29" si="2">D6</f>
+        <f t="shared" ref="D7:D33" si="2">D6</f>
         <v>-</v>
       </c>
       <c r="E7" t="str">
@@ -1292,18 +1343,20 @@
         <v>-</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ref="J7" si="8">J6</f>
-        <v>-</v>
-      </c>
-      <c r="K7">
+        <f t="shared" ref="J7:L7" si="8">J6</f>
+        <v>-</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+      <c r="M7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
       <c r="N7">
         <v>1</v>
       </c>
@@ -1341,11 +1394,17 @@
         <v>1</v>
       </c>
       <c r="Z7">
-        <f t="shared" ref="Z7:Z29" si="9">Z6</f>
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" ref="AB7:AB29" si="9">AB6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" t="b">
         <v>0</v>
       </c>
@@ -1380,21 +1439,23 @@
         <v>-</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" ref="J8" si="11">J7</f>
-        <v>-</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
+        <f t="shared" ref="J8:L8" si="11">J7</f>
+        <v>-</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="11"/>
+        <v>-</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="11"/>
+        <v>-</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
         <v>0.9</v>
       </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
       <c r="O8">
         <v>1</v>
       </c>
@@ -1429,11 +1490,17 @@
         <v>1</v>
       </c>
       <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" t="b">
         <v>0</v>
       </c>
@@ -1468,21 +1535,23 @@
         <v>-</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" ref="J9" si="13">J8</f>
-        <v>-</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
+        <f t="shared" ref="J9:L9" si="13">J8</f>
+        <v>-</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="13"/>
+        <v>-</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="13"/>
+        <v>-</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
       <c r="O9">
         <v>1</v>
       </c>
@@ -1517,11 +1586,17 @@
         <v>1</v>
       </c>
       <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" t="b">
         <v>0</v>
       </c>
@@ -1556,24 +1631,26 @@
         <v>-</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" ref="J10" si="15">J9</f>
-        <v>-</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
+        <f t="shared" ref="J10:L10" si="15">J9</f>
+        <v>-</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="15"/>
+        <v>-</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="15"/>
+        <v>-</v>
       </c>
       <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
         <v>0.9</v>
       </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
       <c r="P10">
         <v>1</v>
       </c>
@@ -1605,11 +1682,17 @@
         <v>1</v>
       </c>
       <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="b">
         <v>0</v>
       </c>
@@ -1644,24 +1727,26 @@
         <v>-</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" ref="J11" si="17">J10</f>
-        <v>-</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
+        <f t="shared" ref="J11:L11" si="17">J10</f>
+        <v>-</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="17"/>
+        <v>-</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="17"/>
+        <v>-</v>
       </c>
       <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
       <c r="P11">
         <v>1</v>
       </c>
@@ -1693,11 +1778,17 @@
         <v>1</v>
       </c>
       <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" t="b">
         <v>0</v>
       </c>
@@ -1732,27 +1823,29 @@
         <v>-</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12" si="19">J11</f>
-        <v>-</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
+        <f t="shared" ref="J12:L12" si="19">J11</f>
+        <v>-</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="19"/>
+        <v>-</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="19"/>
+        <v>-</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
       <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
         <v>0.9</v>
       </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
       <c r="Q12">
         <v>1</v>
       </c>
@@ -1781,11 +1874,17 @@
         <v>1</v>
       </c>
       <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" t="b">
         <v>0</v>
       </c>
@@ -1820,27 +1919,29 @@
         <v>-</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" ref="J13" si="21">J12</f>
-        <v>-</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
+        <f t="shared" ref="J13:L13" si="21">J12</f>
+        <v>-</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
       <c r="Q13">
         <v>1</v>
       </c>
@@ -1869,11 +1970,17 @@
         <v>1</v>
       </c>
       <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>1</v>
+      </c>
+      <c r="AB13">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -1908,14 +2015,16 @@
         <v>-</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" ref="J14" si="23">J13</f>
-        <v>-</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
+        <f t="shared" ref="J14:L14" si="23">J13</f>
+        <v>-</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
       </c>
       <c r="M14">
         <v>1</v>
@@ -1924,14 +2033,14 @@
         <v>1</v>
       </c>
       <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
         <v>0.9</v>
       </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
       <c r="R14">
         <v>1</v>
       </c>
@@ -1957,11 +2066,17 @@
         <v>1</v>
       </c>
       <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" t="b">
         <v>0</v>
       </c>
@@ -1996,14 +2111,16 @@
         <v>-</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" ref="J15" si="25">J14</f>
-        <v>-</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
+        <f t="shared" ref="J15:L15" si="25">J14</f>
+        <v>-</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
       </c>
       <c r="M15">
         <v>1</v>
@@ -2012,14 +2129,14 @@
         <v>1</v>
       </c>
       <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
       <c r="R15">
         <v>1</v>
       </c>
@@ -2045,11 +2162,17 @@
         <v>1</v>
       </c>
       <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" t="b">
         <v>0</v>
       </c>
@@ -2084,14 +2207,16 @@
         <v>-</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" ref="J16" si="27">J15</f>
-        <v>-</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
+        <f t="shared" ref="J16:L16" si="27">J15</f>
+        <v>-</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -2103,14 +2228,14 @@
         <v>1</v>
       </c>
       <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
         <v>0.9</v>
       </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
       <c r="S16">
         <v>1</v>
       </c>
@@ -2133,11 +2258,17 @@
         <v>1</v>
       </c>
       <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" t="b">
         <v>0</v>
       </c>
@@ -2172,14 +2303,16 @@
         <v>-</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" ref="J17" si="29">J16</f>
-        <v>-</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
+        <f t="shared" ref="J17:L17" si="29">J16</f>
+        <v>-</v>
+      </c>
+      <c r="K17" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -2191,14 +2324,14 @@
         <v>1</v>
       </c>
       <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
       <c r="S17">
         <v>1</v>
       </c>
@@ -2221,11 +2354,17 @@
         <v>1</v>
       </c>
       <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -2260,14 +2399,16 @@
         <v>-</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18" si="31">J17</f>
-        <v>-</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
+        <f t="shared" ref="J18:L18" si="31">J17</f>
+        <v>-</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -2282,14 +2423,14 @@
         <v>1</v>
       </c>
       <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
         <v>0.9</v>
       </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-      <c r="S18">
-        <v>1</v>
-      </c>
       <c r="T18">
         <v>1</v>
       </c>
@@ -2309,11 +2450,17 @@
         <v>1</v>
       </c>
       <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" t="b">
         <v>0</v>
       </c>
@@ -2348,14 +2495,16 @@
         <v>-</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" ref="J19" si="33">J18</f>
-        <v>-</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
+        <f t="shared" ref="J19:L19" si="33">J18</f>
+        <v>-</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -2370,14 +2519,14 @@
         <v>1</v>
       </c>
       <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
       <c r="T19">
         <v>1</v>
       </c>
@@ -2397,11 +2546,17 @@
         <v>1</v>
       </c>
       <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" t="b">
         <v>0</v>
       </c>
@@ -2436,14 +2591,16 @@
         <v>-</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" ref="J20" si="35">J19</f>
-        <v>-</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
+        <f t="shared" ref="J20:L20" si="35">J19</f>
+        <v>-</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -2461,14 +2618,14 @@
         <v>1</v>
       </c>
       <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20">
         <v>0.9</v>
       </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-      <c r="T20">
-        <v>1</v>
-      </c>
       <c r="U20">
         <v>1</v>
       </c>
@@ -2485,11 +2642,17 @@
         <v>1</v>
       </c>
       <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" t="b">
         <v>0</v>
       </c>
@@ -2524,14 +2687,16 @@
         <v>-</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" ref="J21" si="37">J20</f>
-        <v>-</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
+        <f t="shared" ref="J21:L21" si="37">J20</f>
+        <v>-</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -2549,14 +2714,14 @@
         <v>1</v>
       </c>
       <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="T21">
-        <v>1</v>
-      </c>
       <c r="U21">
         <v>1</v>
       </c>
@@ -2573,11 +2738,17 @@
         <v>1</v>
       </c>
       <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" t="b">
         <v>0</v>
       </c>
@@ -2612,14 +2783,16 @@
         <v>-</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" ref="J22" si="39">J21</f>
-        <v>-</v>
-      </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <v>1</v>
+        <f t="shared" ref="J22:L22" si="39">J21</f>
+        <v>-</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -2640,14 +2813,14 @@
         <v>1</v>
       </c>
       <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
         <v>0.9</v>
       </c>
-      <c r="T22">
-        <v>1</v>
-      </c>
-      <c r="U22">
-        <v>1</v>
-      </c>
       <c r="V22">
         <v>1</v>
       </c>
@@ -2661,11 +2834,17 @@
         <v>1</v>
       </c>
       <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" t="b">
         <v>0</v>
       </c>
@@ -2700,14 +2879,16 @@
         <v>-</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ref="J23" si="41">J22</f>
-        <v>-</v>
-      </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
+        <f t="shared" ref="J23:L23" si="41">J22</f>
+        <v>-</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="41"/>
+        <v>-</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="41"/>
+        <v>-</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -2728,14 +2909,14 @@
         <v>1</v>
       </c>
       <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T23">
-        <v>1</v>
-      </c>
-      <c r="U23">
-        <v>1</v>
-      </c>
       <c r="V23">
         <v>1</v>
       </c>
@@ -2749,11 +2930,17 @@
         <v>1</v>
       </c>
       <c r="Z23">
+        <v>1</v>
+      </c>
+      <c r="AA23">
+        <v>1</v>
+      </c>
+      <c r="AB23">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24" t="b">
         <v>0</v>
       </c>
@@ -2788,14 +2975,16 @@
         <v>-</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" ref="J24" si="43">J23</f>
-        <v>-</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>1</v>
+        <f t="shared" ref="J24:L24" si="43">J23</f>
+        <v>-</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="43"/>
+        <v>-</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="43"/>
+        <v>-</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -2819,14 +3008,14 @@
         <v>1</v>
       </c>
       <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24">
         <v>0.9</v>
       </c>
-      <c r="U24">
-        <v>1</v>
-      </c>
-      <c r="V24">
-        <v>1</v>
-      </c>
       <c r="W24">
         <v>1</v>
       </c>
@@ -2837,11 +3026,17 @@
         <v>1</v>
       </c>
       <c r="Z24">
+        <v>1</v>
+      </c>
+      <c r="AA24">
+        <v>1</v>
+      </c>
+      <c r="AB24">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" t="b">
         <v>0</v>
       </c>
@@ -2876,14 +3071,16 @@
         <v>-</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" ref="J25" si="45">J24</f>
-        <v>-</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>1</v>
+        <f t="shared" ref="J25:L25" si="45">J24</f>
+        <v>-</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="45"/>
+        <v>-</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="45"/>
+        <v>-</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -2907,14 +3104,14 @@
         <v>1</v>
       </c>
       <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="U25">
-        <v>1</v>
-      </c>
-      <c r="V25">
-        <v>1</v>
-      </c>
       <c r="W25">
         <v>1</v>
       </c>
@@ -2925,11 +3122,17 @@
         <v>1</v>
       </c>
       <c r="Z25">
+        <v>1</v>
+      </c>
+      <c r="AA25">
+        <v>1</v>
+      </c>
+      <c r="AB25">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" t="b">
         <v>0</v>
       </c>
@@ -2964,14 +3167,16 @@
         <v>-</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" ref="J26" si="47">J25</f>
-        <v>-</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26">
-        <v>1</v>
+        <f t="shared" ref="J26:L26" si="47">J25</f>
+        <v>-</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="47"/>
+        <v>-</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="47"/>
+        <v>-</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -2998,14 +3203,14 @@
         <v>1</v>
       </c>
       <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26">
         <v>0.9</v>
       </c>
-      <c r="V26">
-        <v>1</v>
-      </c>
-      <c r="W26">
-        <v>1</v>
-      </c>
       <c r="X26">
         <v>1</v>
       </c>
@@ -3013,11 +3218,17 @@
         <v>1</v>
       </c>
       <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+      <c r="AB26">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27" t="b">
         <v>0</v>
       </c>
@@ -3052,14 +3263,16 @@
         <v>-</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" ref="J27" si="49">J26</f>
-        <v>-</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
+        <f t="shared" ref="J27:L27" si="49">J26</f>
+        <v>-</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -3086,14 +3299,14 @@
         <v>1</v>
       </c>
       <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="W27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="V27">
-        <v>1</v>
-      </c>
-      <c r="W27">
-        <v>1</v>
-      </c>
       <c r="X27">
         <v>1</v>
       </c>
@@ -3101,11 +3314,17 @@
         <v>1</v>
       </c>
       <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A28" t="b">
         <v>0</v>
       </c>
@@ -3140,14 +3359,16 @@
         <v>-</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" ref="J28" si="51">J27</f>
-        <v>-</v>
-      </c>
-      <c r="K28">
-        <v>1</v>
-      </c>
-      <c r="L28">
-        <v>1</v>
+        <f t="shared" ref="J28:L28" si="51">J27</f>
+        <v>-</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="51"/>
+        <v>-</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="51"/>
+        <v>-</v>
       </c>
       <c r="M28">
         <v>1</v>
@@ -3177,23 +3398,29 @@
         <v>1</v>
       </c>
       <c r="V28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>1</v>
+      </c>
+      <c r="X28">
         <v>0.9</v>
       </c>
-      <c r="W28">
-        <v>1</v>
-      </c>
-      <c r="X28">
-        <v>1</v>
-      </c>
       <c r="Y28">
         <v>1</v>
       </c>
       <c r="Z28">
+        <v>1</v>
+      </c>
+      <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AB28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A29" t="b">
         <v>0</v>
       </c>
@@ -3228,14 +3455,16 @@
         <v>-</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" ref="J29" si="53">J28</f>
-        <v>-</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>1</v>
+        <f t="shared" ref="J29:L29" si="53">J28</f>
+        <v>-</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="53"/>
+        <v>-</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="53"/>
+        <v>-</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -3265,24 +3494,466 @@
         <v>1</v>
       </c>
       <c r="V29">
+        <v>1</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="X29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="W29">
-        <v>1</v>
-      </c>
-      <c r="X29">
-        <v>1</v>
-      </c>
       <c r="Y29">
         <v>1</v>
       </c>
       <c r="Z29">
+        <v>1</v>
+      </c>
+      <c r="AA29">
+        <v>1</v>
+      </c>
+      <c r="AB29">
         <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A30" t="b">
+        <v>1</v>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" t="str">
+        <f>D$5</f>
+        <v>-</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" ref="E30:AB33" si="54">E$5</f>
+        <v>-</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="K30">
+        <v>200</v>
+      </c>
+      <c r="L30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AB30">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A31" t="b">
+        <v>1</v>
+      </c>
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" ref="D31:D33" si="55">D$5</f>
+        <v>-</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="K31">
+        <v>800</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="55"/>
+        <v>-</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="K32">
+        <v>1200</v>
+      </c>
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="A33" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="55"/>
+        <v>-</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="K33">
+        <v>1600</v>
+      </c>
+      <c r="L33" t="b">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AB33">
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C4:V5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
+  <autoFilter ref="C4:X5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
   <conditionalFormatting sqref="A1:XFD1">
     <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>"sav"</formula>

</xml_diff>

<commit_message>
fix pyomo error (block delete) reporting
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40DD900-0640-4764-96A4-107CAEB48152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F983A07-A89A-410C-84C7-62C9D3DFA144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -816,10 +816,10 @@
   <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A5:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -1319,7 +1319,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D7:D33" si="2">D6</f>
+        <f t="shared" ref="D7:D29" si="2">D6</f>
         <v>-</v>
       </c>
       <c r="E7" t="str">

</xml_diff>

<commit_message>
tweaks to reading exp.xl to handle column adds
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A23A47-D468-49AD-8F8D-1BBA82B94808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B6A02A-6C77-4293-BA59-5E9373AFD152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$4:$X$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$Y$5</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -38,10 +38,36 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Michael Young (21512438)</author>
     <author>Michael Young</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CCB77013-F05A-42FB-A15C-BBB0BA6C23F4}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{37D6CE8F-CE51-4B7D-8E5C-A1A0A18133AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Michael Young (21512438): 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Can add cols that are just for personal use (eg not used by code) by adding the word Drop in the top row.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{CCB77013-F05A-42FB-A15C-BBB0BA6C23F4}">
       <text>
         <r>
           <rPr>
@@ -65,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{3BDB7BEB-FC53-4975-ADDB-A81C02A033DC}">
+    <comment ref="D3" authorId="1" shapeId="0" xr:uid="{3BDB7BEB-FC53-4975-ADDB-A81C02A033DC}">
       <text>
         <r>
           <rPr>
@@ -90,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{7875E08E-43A6-4F76-BAD2-431E3C040A9B}">
+    <comment ref="D4" authorId="1" shapeId="0" xr:uid="{7875E08E-43A6-4F76-BAD2-431E3C040A9B}">
       <text>
         <r>
           <rPr>
@@ -116,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{86423575-3B9D-46A2-9D4D-B5C8EEE47047}">
+    <comment ref="D5" authorId="1" shapeId="0" xr:uid="{86423575-3B9D-46A2-9D4D-B5C8EEE47047}">
       <text>
         <r>
           <rPr>
@@ -168,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>sam</t>
   </si>
@@ -336,6 +362,12 @@
   </si>
   <si>
     <t>Pas area 10%</t>
+  </si>
+  <si>
+    <t>Drop</t>
+  </si>
+  <si>
+    <t>Trial Number</t>
   </si>
 </sst>
 </file>
@@ -419,7 +451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -444,6 +476,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -813,31 +848,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:AB33"/>
+  <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="A29:A30"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="17.54296875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>43</v>
@@ -864,7 +899,7 @@
         <v>43</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>0</v>
@@ -900,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="Z1" s="6" t="s">
         <v>42</v>
@@ -908,22 +943,22 @@
       <c r="AA1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="5" t="s">
+    <row r="2" spans="1:29" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>47</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>48</v>
@@ -932,23 +967,23 @@
         <v>48</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="O2" s="6" t="s">
         <v>1</v>
       </c>
@@ -962,10 +997,10 @@
         <v>1</v>
       </c>
       <c r="S2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="U2" s="6" t="s">
         <v>10</v>
@@ -979,15 +1014,17 @@
       <c r="X2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Y2" s="6"/>
+      <c r="Y2" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="1:29" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -996,9 +1033,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="M3" s="6"/>
       <c r="N3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1032,88 +1067,93 @@
       <c r="X3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="6"/>
+      <c r="Y3" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="Z3" s="6"/>
       <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
     </row>
-    <row r="4" spans="1:28" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7" t="s">
+      <c r="M4" s="8"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="P4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7" t="s">
+      <c r="T4" s="7"/>
+      <c r="U4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A5" t="b">
-        <v>1</v>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" s="9" t="str" cm="1">
-        <f t="array" ref="D5">_xlfn.IFS(OR(D1="sam",D1="sai"),1,D1="sav","-",OR(D1="sap",D1="saa"),0)</f>
-        <v>-</v>
       </c>
       <c r="E5" s="9" t="str" cm="1">
         <f t="array" ref="E5">_xlfn.IFS(OR(E1="sam",E1="sai"),1,E1="sav","-",OR(E1="sap",E1="saa"),0)</f>
@@ -1147,9 +1187,9 @@
         <f t="array" ref="L5">_xlfn.IFS(OR(L1="sam",L1="sai"),1,L1="sav","-",OR(L1="sap",L1="saa"),0)</f>
         <v>-</v>
       </c>
-      <c r="M5" s="9" cm="1">
+      <c r="M5" s="9" t="str" cm="1">
         <f t="array" ref="M5">_xlfn.IFS(OR(M1="sam",M1="sai"),1,M1="sav","-",OR(M1="sap",M1="saa"),0)</f>
-        <v>1</v>
+        <v>-</v>
       </c>
       <c r="N5" s="9" cm="1">
         <f t="array" ref="N5">_xlfn.IFS(OR(N1="sam",N1="sai"),1,N1="sav","-",OR(N1="sap",N1="saa"),0)</f>
@@ -1197,7 +1237,7 @@
       </c>
       <c r="Y5" s="9" cm="1">
         <f t="array" ref="Y5">_xlfn.IFS(OR(Y1="sam",Y1="sai"),1,Y1="sav","-",OR(Y1="sap",Y1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5" s="9" cm="1">
         <f t="array" ref="Z5">_xlfn.IFS(OR(Z1="sam",Z1="sai"),1,Z1="sav","-",OR(Z1="sap",Z1="saa"),0)</f>
@@ -1211,31 +1251,34 @@
         <f t="array" ref="AB5">_xlfn.IFS(OR(AB1="sam",AB1="sai"),1,AB1="sav","-",OR(AB1="sap",AB1="saa"),0)</f>
         <v>0</v>
       </c>
+      <c r="AC5" s="9" cm="1">
+        <f t="array" ref="AC5">_xlfn.IFS(OR(AC1="sam",AC1="sai"),1,AC1="sav","-",OR(AC1="sap",AC1="saa"),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A6" t="b">
-        <v>0</v>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" t="str">
-        <f>D5</f>
-        <v>-</v>
       </c>
       <c r="E6" t="str">
         <f>E5</f>
         <v>-</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ref="F6:H6" si="0">F5</f>
+        <f>F5</f>
         <v>-</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G6:I6" si="0">G5</f>
         <v>-</v>
       </c>
       <c r="H6" t="str">
@@ -1243,11 +1286,11 @@
         <v>-</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6:L6" si="1">I5</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J6:M6" si="1">J5</f>
         <v>-</v>
       </c>
       <c r="K6" t="str">
@@ -1258,12 +1301,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="M6">
+      <c r="M6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="N6">
         <v>0.9</v>
       </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
       <c r="O6">
         <v>1</v>
       </c>
@@ -1304,62 +1348,65 @@
         <v>1</v>
       </c>
       <c r="AB6">
-        <f>AB5</f>
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <f>AC5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A7" t="b">
-        <v>0</v>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="str">
-        <f t="shared" ref="D7:D29" si="2">D6</f>
-        <v>-</v>
-      </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E7:E29" si="3">E6</f>
+        <f t="shared" ref="E7:E29" si="2">E6</f>
         <v>-</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ref="F7:F29" si="4">F6</f>
+        <f t="shared" ref="F7:F29" si="3">F6</f>
         <v>-</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" ref="G7:G29" si="5">G6</f>
+        <f t="shared" ref="G7:G29" si="4">G6</f>
         <v>-</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7:H29" si="6">H6</f>
+        <f t="shared" ref="H7:H29" si="5">H6</f>
         <v>-</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" ref="I7" si="7">I6</f>
+        <f t="shared" ref="I7:I29" si="6">I6</f>
         <v>-</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ref="J7:L7" si="8">J6</f>
+        <f t="shared" ref="J7" si="7">J6</f>
         <v>-</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="K7:M7" si="8">K6</f>
         <v>-</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="M7">
+      <c r="M7" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+      <c r="N7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
       <c r="O7">
         <v>1</v>
       </c>
@@ -1400,65 +1447,68 @@
         <v>1</v>
       </c>
       <c r="AB7">
-        <f t="shared" ref="AB7:AB29" si="9">AB6</f>
+        <v>1</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" ref="AC7:AC29" si="9">AC6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A8" t="b">
-        <v>0</v>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>3</v>
       </c>
       <c r="B8" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="str">
+      <c r="E8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E8" t="str">
+      <c r="F8" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I8" t="str">
-        <f t="shared" ref="I8" si="10">I7</f>
-        <v>-</v>
-      </c>
       <c r="J8" t="str">
-        <f t="shared" ref="J8:L8" si="11">J7</f>
+        <f t="shared" ref="J8" si="10">J7</f>
         <v>-</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="K8:M8" si="11">K7</f>
         <v>-</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="11"/>
         <v>-</v>
       </c>
-      <c r="M8">
-        <v>1</v>
+      <c r="M8" t="str">
+        <f t="shared" si="11"/>
+        <v>-</v>
       </c>
       <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
         <v>0.9</v>
       </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
       <c r="P8">
         <v>1</v>
       </c>
@@ -1496,65 +1546,68 @@
         <v>1</v>
       </c>
       <c r="AB8">
+        <v>1</v>
+      </c>
+      <c r="AC8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A9" t="b">
-        <v>0</v>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>4</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="str">
+      <c r="E9" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E9" t="str">
+      <c r="F9" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" ref="I9" si="12">I8</f>
-        <v>-</v>
-      </c>
       <c r="J9" t="str">
-        <f t="shared" ref="J9:L9" si="13">J8</f>
+        <f t="shared" ref="J9" si="12">J8</f>
         <v>-</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="K9:M9" si="13">K8</f>
         <v>-</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="13"/>
         <v>-</v>
       </c>
-      <c r="M9">
-        <v>1</v>
+      <c r="M9" t="str">
+        <f t="shared" si="13"/>
+        <v>-</v>
       </c>
       <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
       <c r="P9">
         <v>1</v>
       </c>
@@ -1592,68 +1645,71 @@
         <v>1</v>
       </c>
       <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A10" t="b">
-        <v>0</v>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>5</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" t="str">
+      <c r="E10" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E10" t="str">
+      <c r="F10" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" ref="I10" si="14">I9</f>
-        <v>-</v>
-      </c>
       <c r="J10" t="str">
-        <f t="shared" ref="J10:L10" si="15">J9</f>
+        <f t="shared" ref="J10" si="14">J9</f>
         <v>-</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="K10:M10" si="15">K9</f>
         <v>-</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="15"/>
         <v>-</v>
       </c>
-      <c r="M10">
-        <v>1</v>
+      <c r="M10" t="str">
+        <f t="shared" si="15"/>
+        <v>-</v>
       </c>
       <c r="N10">
         <v>1</v>
       </c>
       <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
         <v>0.9</v>
       </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
       <c r="Q10">
         <v>1</v>
       </c>
@@ -1688,68 +1744,71 @@
         <v>1</v>
       </c>
       <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A11" t="b">
-        <v>0</v>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>6</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D11" t="str">
+      <c r="E11" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E11" t="str">
+      <c r="F11" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" ref="I11" si="16">I10</f>
-        <v>-</v>
-      </c>
       <c r="J11" t="str">
-        <f t="shared" ref="J11:L11" si="17">J10</f>
+        <f t="shared" ref="J11" si="16">J10</f>
         <v>-</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="K11:M11" si="17">K10</f>
         <v>-</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="17"/>
         <v>-</v>
       </c>
-      <c r="M11">
-        <v>1</v>
+      <c r="M11" t="str">
+        <f t="shared" si="17"/>
+        <v>-</v>
       </c>
       <c r="N11">
         <v>1</v>
       </c>
       <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
       <c r="Q11">
         <v>1</v>
       </c>
@@ -1784,58 +1843,61 @@
         <v>1</v>
       </c>
       <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AC11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A12" t="b">
-        <v>0</v>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>7</v>
       </c>
       <c r="B12" t="b">
         <v>0</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D12" t="str">
+      <c r="E12" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E12" t="str">
+      <c r="F12" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" ref="I12" si="18">I11</f>
-        <v>-</v>
-      </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12:L12" si="19">J11</f>
+        <f t="shared" ref="J12" si="18">J11</f>
         <v>-</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="K12:M12" si="19">K11</f>
         <v>-</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="19"/>
         <v>-</v>
       </c>
-      <c r="M12">
-        <v>1</v>
+      <c r="M12" t="str">
+        <f t="shared" si="19"/>
+        <v>-</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -1844,11 +1906,11 @@
         <v>1</v>
       </c>
       <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
         <v>0.9</v>
       </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
       <c r="R12">
         <v>1</v>
       </c>
@@ -1880,58 +1942,61 @@
         <v>1</v>
       </c>
       <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A13" t="b">
-        <v>0</v>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>8</v>
       </c>
       <c r="B13" t="b">
         <v>0</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="str">
+      <c r="E13" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E13" t="str">
+      <c r="F13" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" ref="I13" si="20">I12</f>
-        <v>-</v>
-      </c>
       <c r="J13" t="str">
-        <f t="shared" ref="J13:L13" si="21">J12</f>
+        <f t="shared" ref="J13" si="20">J12</f>
         <v>-</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="K13:M13" si="21">K12</f>
         <v>-</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="21"/>
         <v>-</v>
       </c>
-      <c r="M13">
-        <v>1</v>
+      <c r="M13" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -1940,11 +2005,11 @@
         <v>1</v>
       </c>
       <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
       <c r="R13">
         <v>1</v>
       </c>
@@ -1976,58 +2041,61 @@
         <v>1</v>
       </c>
       <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A14" t="b">
-        <v>0</v>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>9</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="str">
+      <c r="E14" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E14" t="str">
+      <c r="F14" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H14" t="str">
+      <c r="I14" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" ref="I14" si="22">I13</f>
-        <v>-</v>
-      </c>
       <c r="J14" t="str">
-        <f t="shared" ref="J14:L14" si="23">J13</f>
+        <f t="shared" ref="J14" si="22">J13</f>
         <v>-</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="K14:M14" si="23">K13</f>
         <v>-</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="23"/>
         <v>-</v>
       </c>
-      <c r="M14">
-        <v>1</v>
+      <c r="M14" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -2039,11 +2107,11 @@
         <v>1</v>
       </c>
       <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
         <v>0.9</v>
       </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
       <c r="S14">
         <v>1</v>
       </c>
@@ -2072,58 +2140,61 @@
         <v>1</v>
       </c>
       <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A15" t="b">
-        <v>0</v>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>10</v>
       </c>
       <c r="B15" t="b">
         <v>0</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D15" t="str">
+      <c r="E15" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E15" t="str">
+      <c r="F15" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H15" t="str">
+      <c r="I15" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" ref="I15" si="24">I14</f>
-        <v>-</v>
-      </c>
       <c r="J15" t="str">
-        <f t="shared" ref="J15:L15" si="25">J14</f>
+        <f t="shared" ref="J15" si="24">J14</f>
         <v>-</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="K15:M15" si="25">K14</f>
         <v>-</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="25"/>
         <v>-</v>
       </c>
-      <c r="M15">
-        <v>1</v>
+      <c r="M15" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -2135,11 +2206,11 @@
         <v>1</v>
       </c>
       <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
       <c r="S15">
         <v>1</v>
       </c>
@@ -2168,58 +2239,61 @@
         <v>1</v>
       </c>
       <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A16" t="b">
-        <v>0</v>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>11</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D16" t="str">
+      <c r="E16" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E16" t="str">
+      <c r="F16" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" ref="I16" si="26">I15</f>
-        <v>-</v>
-      </c>
       <c r="J16" t="str">
-        <f t="shared" ref="J16:L16" si="27">J15</f>
+        <f t="shared" ref="J16" si="26">J15</f>
         <v>-</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="K16:M16" si="27">K15</f>
         <v>-</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="27"/>
         <v>-</v>
       </c>
-      <c r="M16">
-        <v>1</v>
+      <c r="M16" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -2234,11 +2308,11 @@
         <v>1</v>
       </c>
       <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
         <v>0.9</v>
       </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
       <c r="T16">
         <v>1</v>
       </c>
@@ -2264,58 +2338,61 @@
         <v>1</v>
       </c>
       <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A17" t="b">
-        <v>0</v>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>12</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D17" t="str">
+      <c r="E17" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E17" t="str">
+      <c r="F17" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" ref="I17" si="28">I16</f>
-        <v>-</v>
-      </c>
       <c r="J17" t="str">
-        <f t="shared" ref="J17:L17" si="29">J16</f>
+        <f t="shared" ref="J17" si="28">J16</f>
         <v>-</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="K17:M17" si="29">K16</f>
         <v>-</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="29"/>
         <v>-</v>
       </c>
-      <c r="M17">
-        <v>1</v>
+      <c r="M17" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -2330,11 +2407,11 @@
         <v>1</v>
       </c>
       <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S17">
-        <v>1</v>
-      </c>
       <c r="T17">
         <v>1</v>
       </c>
@@ -2360,58 +2437,61 @@
         <v>1</v>
       </c>
       <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A18" t="b">
-        <v>0</v>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>13</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="str">
+      <c r="E18" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E18" t="str">
+      <c r="F18" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H18" t="str">
+      <c r="I18" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I18" t="str">
-        <f t="shared" ref="I18" si="30">I17</f>
-        <v>-</v>
-      </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18:L18" si="31">J17</f>
+        <f t="shared" ref="J18" si="30">J17</f>
         <v>-</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="K18:M18" si="31">K17</f>
         <v>-</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="31"/>
         <v>-</v>
       </c>
-      <c r="M18">
-        <v>1</v>
+      <c r="M18" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -2429,11 +2509,11 @@
         <v>1</v>
       </c>
       <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
         <v>0.9</v>
       </c>
-      <c r="T18">
-        <v>1</v>
-      </c>
       <c r="U18">
         <v>1</v>
       </c>
@@ -2456,58 +2536,61 @@
         <v>1</v>
       </c>
       <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A19" t="b">
-        <v>0</v>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>14</v>
       </c>
       <c r="B19" t="b">
         <v>0</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D19" t="str">
+      <c r="E19" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E19" t="str">
+      <c r="F19" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H19" t="str">
+      <c r="I19" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I19" t="str">
-        <f t="shared" ref="I19" si="32">I18</f>
-        <v>-</v>
-      </c>
       <c r="J19" t="str">
-        <f t="shared" ref="J19:L19" si="33">J18</f>
+        <f t="shared" ref="J19" si="32">J18</f>
         <v>-</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="K19:M19" si="33">K18</f>
         <v>-</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="33"/>
         <v>-</v>
       </c>
-      <c r="M19">
-        <v>1</v>
+      <c r="M19" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -2525,11 +2608,11 @@
         <v>1</v>
       </c>
       <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T19">
-        <v>1</v>
-      </c>
       <c r="U19">
         <v>1</v>
       </c>
@@ -2552,58 +2635,61 @@
         <v>1</v>
       </c>
       <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A20" t="b">
-        <v>0</v>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>15</v>
       </c>
       <c r="B20" t="b">
         <v>0</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20" t="str">
+      <c r="E20" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E20" t="str">
+      <c r="F20" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F20" t="str">
+      <c r="G20" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H20" t="str">
+      <c r="I20" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I20" t="str">
-        <f t="shared" ref="I20" si="34">I19</f>
-        <v>-</v>
-      </c>
       <c r="J20" t="str">
-        <f t="shared" ref="J20:L20" si="35">J19</f>
+        <f t="shared" ref="J20" si="34">J19</f>
         <v>-</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="K20:M20" si="35">K19</f>
         <v>-</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="35"/>
         <v>-</v>
       </c>
-      <c r="M20">
-        <v>1</v>
+      <c r="M20" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -2624,11 +2710,11 @@
         <v>1</v>
       </c>
       <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
         <v>0.9</v>
       </c>
-      <c r="U20">
-        <v>1</v>
-      </c>
       <c r="V20">
         <v>1</v>
       </c>
@@ -2648,58 +2734,61 @@
         <v>1</v>
       </c>
       <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A21" t="b">
-        <v>0</v>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>16</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D21" t="str">
+      <c r="E21" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E21" t="str">
+      <c r="F21" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F21" t="str">
+      <c r="G21" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G21" t="str">
+      <c r="H21" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H21" t="str">
+      <c r="I21" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I21" t="str">
-        <f t="shared" ref="I21" si="36">I20</f>
-        <v>-</v>
-      </c>
       <c r="J21" t="str">
-        <f t="shared" ref="J21:L21" si="37">J20</f>
+        <f t="shared" ref="J21" si="36">J20</f>
         <v>-</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="K21:M21" si="37">K20</f>
         <v>-</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="37"/>
         <v>-</v>
       </c>
-      <c r="M21">
-        <v>1</v>
+      <c r="M21" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -2720,11 +2809,11 @@
         <v>1</v>
       </c>
       <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="U21">
-        <v>1</v>
-      </c>
       <c r="V21">
         <v>1</v>
       </c>
@@ -2744,58 +2833,61 @@
         <v>1</v>
       </c>
       <c r="AB21">
+        <v>1</v>
+      </c>
+      <c r="AC21">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A22" t="b">
-        <v>0</v>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>17</v>
       </c>
       <c r="B22" t="b">
         <v>0</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D22" t="str">
+      <c r="E22" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E22" t="str">
+      <c r="F22" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F22" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G22" t="str">
+      <c r="H22" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H22" t="str">
+      <c r="I22" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I22" t="str">
-        <f t="shared" ref="I22" si="38">I21</f>
-        <v>-</v>
-      </c>
       <c r="J22" t="str">
-        <f t="shared" ref="J22:L22" si="39">J21</f>
+        <f t="shared" ref="J22" si="38">J21</f>
         <v>-</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="K22:M22" si="39">K21</f>
         <v>-</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="39"/>
         <v>-</v>
       </c>
-      <c r="M22">
-        <v>1</v>
+      <c r="M22" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
       </c>
       <c r="N22">
         <v>1</v>
@@ -2819,11 +2911,11 @@
         <v>1</v>
       </c>
       <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
         <v>0.9</v>
       </c>
-      <c r="V22">
-        <v>1</v>
-      </c>
       <c r="W22">
         <v>1</v>
       </c>
@@ -2840,58 +2932,61 @@
         <v>1</v>
       </c>
       <c r="AB22">
+        <v>1</v>
+      </c>
+      <c r="AC22">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A23" t="b">
-        <v>0</v>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>18</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D23" t="str">
+      <c r="E23" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E23" t="str">
+      <c r="F23" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F23" t="str">
+      <c r="G23" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G23" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H23" t="str">
+      <c r="I23" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I23" t="str">
-        <f t="shared" ref="I23" si="40">I22</f>
-        <v>-</v>
-      </c>
       <c r="J23" t="str">
-        <f t="shared" ref="J23:L23" si="41">J22</f>
+        <f t="shared" ref="J23" si="40">J22</f>
         <v>-</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="K23:M23" si="41">K22</f>
         <v>-</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="41"/>
         <v>-</v>
       </c>
-      <c r="M23">
-        <v>1</v>
+      <c r="M23" t="str">
+        <f t="shared" si="41"/>
+        <v>-</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -2915,11 +3010,11 @@
         <v>1</v>
       </c>
       <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="V23">
-        <v>1</v>
-      </c>
       <c r="W23">
         <v>1</v>
       </c>
@@ -2936,58 +3031,61 @@
         <v>1</v>
       </c>
       <c r="AB23">
+        <v>1</v>
+      </c>
+      <c r="AC23">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A24" t="b">
-        <v>0</v>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>19</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D24" t="str">
+      <c r="E24" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E24" t="str">
+      <c r="F24" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F24" t="str">
+      <c r="G24" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G24" t="str">
+      <c r="H24" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H24" t="str">
+      <c r="I24" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I24" t="str">
-        <f t="shared" ref="I24" si="42">I23</f>
-        <v>-</v>
-      </c>
       <c r="J24" t="str">
-        <f t="shared" ref="J24:L24" si="43">J23</f>
+        <f t="shared" ref="J24" si="42">J23</f>
         <v>-</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" ref="K24:M24" si="43">K23</f>
         <v>-</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="43"/>
         <v>-</v>
       </c>
-      <c r="M24">
-        <v>1</v>
+      <c r="M24" t="str">
+        <f t="shared" si="43"/>
+        <v>-</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -3014,11 +3112,11 @@
         <v>1</v>
       </c>
       <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
         <v>0.9</v>
       </c>
-      <c r="W24">
-        <v>1</v>
-      </c>
       <c r="X24">
         <v>1</v>
       </c>
@@ -3032,58 +3130,61 @@
         <v>1</v>
       </c>
       <c r="AB24">
+        <v>1</v>
+      </c>
+      <c r="AC24">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A25" t="b">
-        <v>0</v>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>20</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D25" t="str">
+      <c r="E25" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E25" t="str">
+      <c r="F25" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F25" t="str">
+      <c r="G25" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G25" t="str">
+      <c r="H25" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H25" t="str">
+      <c r="I25" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I25" t="str">
-        <f t="shared" ref="I25" si="44">I24</f>
-        <v>-</v>
-      </c>
       <c r="J25" t="str">
-        <f t="shared" ref="J25:L25" si="45">J24</f>
+        <f t="shared" ref="J25" si="44">J24</f>
         <v>-</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="K25:M25" si="45">K24</f>
         <v>-</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="45"/>
         <v>-</v>
       </c>
-      <c r="M25">
-        <v>1</v>
+      <c r="M25" t="str">
+        <f t="shared" si="45"/>
+        <v>-</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -3110,11 +3211,11 @@
         <v>1</v>
       </c>
       <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="W25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="W25">
-        <v>1</v>
-      </c>
       <c r="X25">
         <v>1</v>
       </c>
@@ -3128,58 +3229,61 @@
         <v>1</v>
       </c>
       <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A26" t="b">
-        <v>0</v>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>21</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D26" t="str">
+      <c r="E26" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E26" t="str">
+      <c r="F26" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F26" t="str">
+      <c r="G26" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G26" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H26" t="str">
+      <c r="I26" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I26" t="str">
-        <f t="shared" ref="I26" si="46">I25</f>
-        <v>-</v>
-      </c>
       <c r="J26" t="str">
-        <f t="shared" ref="J26:L26" si="47">J25</f>
+        <f t="shared" ref="J26" si="46">J25</f>
         <v>-</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" ref="K26:M26" si="47">K25</f>
         <v>-</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="47"/>
         <v>-</v>
       </c>
-      <c r="M26">
-        <v>1</v>
+      <c r="M26" t="str">
+        <f t="shared" si="47"/>
+        <v>-</v>
       </c>
       <c r="N26">
         <v>1</v>
@@ -3209,11 +3313,11 @@
         <v>1</v>
       </c>
       <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26">
         <v>0.9</v>
       </c>
-      <c r="X26">
-        <v>1</v>
-      </c>
       <c r="Y26">
         <v>1</v>
       </c>
@@ -3224,58 +3328,61 @@
         <v>1</v>
       </c>
       <c r="AB26">
+        <v>1</v>
+      </c>
+      <c r="AC26">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A27" t="b">
-        <v>0</v>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>22</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D27" t="str">
+      <c r="E27" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E27" t="str">
+      <c r="F27" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F27" t="str">
+      <c r="G27" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G27" t="str">
+      <c r="H27" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H27" t="str">
+      <c r="I27" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I27" t="str">
-        <f t="shared" ref="I27" si="48">I26</f>
-        <v>-</v>
-      </c>
       <c r="J27" t="str">
-        <f t="shared" ref="J27:L27" si="49">J26</f>
+        <f t="shared" ref="J27" si="48">J26</f>
         <v>-</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" ref="K27:M27" si="49">K26</f>
         <v>-</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="49"/>
         <v>-</v>
       </c>
-      <c r="M27">
-        <v>1</v>
+      <c r="M27" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
       </c>
       <c r="N27">
         <v>1</v>
@@ -3305,11 +3412,11 @@
         <v>1</v>
       </c>
       <c r="W27">
+        <v>1</v>
+      </c>
+      <c r="X27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="X27">
-        <v>1</v>
-      </c>
       <c r="Y27">
         <v>1</v>
       </c>
@@ -3320,58 +3427,61 @@
         <v>1</v>
       </c>
       <c r="AB27">
+        <v>1</v>
+      </c>
+      <c r="AC27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A28" t="b">
-        <v>0</v>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>23</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D28" t="str">
+      <c r="E28" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E28" t="str">
+      <c r="F28" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F28" t="str">
+      <c r="G28" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H28" t="str">
+      <c r="I28" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I28" t="str">
-        <f t="shared" ref="I28" si="50">I27</f>
-        <v>-</v>
-      </c>
       <c r="J28" t="str">
-        <f t="shared" ref="J28:L28" si="51">J27</f>
+        <f t="shared" ref="J28" si="50">J27</f>
         <v>-</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" ref="K28:M28" si="51">K27</f>
         <v>-</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="51"/>
         <v>-</v>
       </c>
-      <c r="M28">
-        <v>1</v>
+      <c r="M28" t="str">
+        <f t="shared" si="51"/>
+        <v>-</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -3404,11 +3514,11 @@
         <v>1</v>
       </c>
       <c r="X28">
+        <v>1</v>
+      </c>
+      <c r="Y28">
         <v>0.9</v>
       </c>
-      <c r="Y28">
-        <v>1</v>
-      </c>
       <c r="Z28">
         <v>1</v>
       </c>
@@ -3416,58 +3526,61 @@
         <v>1</v>
       </c>
       <c r="AB28">
+        <v>1</v>
+      </c>
+      <c r="AC28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A29" t="b">
-        <v>0</v>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>24</v>
       </c>
       <c r="B29" t="b">
         <v>0</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D29" t="str">
+      <c r="E29" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E29" t="str">
+      <c r="F29" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F29" t="str">
+      <c r="G29" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="G29" t="str">
+      <c r="H29" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="H29" t="str">
+      <c r="I29" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
-      <c r="I29" t="str">
-        <f t="shared" ref="I29" si="52">I28</f>
-        <v>-</v>
-      </c>
       <c r="J29" t="str">
-        <f t="shared" ref="J29:L29" si="53">J28</f>
+        <f t="shared" ref="J29" si="52">J28</f>
         <v>-</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="K29:M29" si="53">K28</f>
         <v>-</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="53"/>
         <v>-</v>
       </c>
-      <c r="M29">
-        <v>1</v>
+      <c r="M29" t="str">
+        <f t="shared" si="53"/>
+        <v>-</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -3500,11 +3613,11 @@
         <v>1</v>
       </c>
       <c r="X29">
+        <v>1</v>
+      </c>
+      <c r="Y29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Y29">
-        <v>1</v>
-      </c>
       <c r="Z29">
         <v>1</v>
       </c>
@@ -3512,30 +3625,32 @@
         <v>1</v>
       </c>
       <c r="AB29">
+        <v>1</v>
+      </c>
+      <c r="AC29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A30" t="b">
-        <v>0</v>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>25</v>
       </c>
       <c r="B30" t="b">
-        <v>0</v>
-      </c>
-      <c r="C30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D30" t="str">
-        <f>D$5</f>
-        <v>-</v>
-      </c>
       <c r="E30" t="str">
-        <f t="shared" ref="E30:AB33" si="54">E$5</f>
+        <f>E$5</f>
         <v>-</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" ref="F30:AC33" si="54">F$5</f>
         <v>-</v>
       </c>
       <c r="G30" t="str">
@@ -3554,14 +3669,14 @@
         <f t="shared" si="54"/>
         <v>-</v>
       </c>
-      <c r="K30">
+      <c r="K30" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="L30">
         <v>200</v>
       </c>
-      <c r="L30" t="b">
-        <v>1</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="54"/>
+      <c r="M30" t="b">
         <v>1</v>
       </c>
       <c r="N30">
@@ -3610,7 +3725,7 @@
       </c>
       <c r="Y30">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z30">
         <f t="shared" si="54"/>
@@ -3624,23 +3739,26 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
+      <c r="AC30">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A31" t="b">
-        <v>0</v>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>26</v>
       </c>
       <c r="B31" t="b">
-        <v>0</v>
-      </c>
-      <c r="C31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D31" t="str">
-        <f t="shared" ref="D31:D33" si="55">D$5</f>
-        <v>-</v>
-      </c>
       <c r="E31" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" ref="E31:E33" si="55">E$5</f>
         <v>-</v>
       </c>
       <c r="F31" t="str">
@@ -3663,14 +3781,14 @@
         <f t="shared" si="54"/>
         <v>-</v>
       </c>
-      <c r="K31">
+      <c r="K31" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="L31">
         <v>800</v>
       </c>
-      <c r="L31" t="b">
-        <v>1</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="54"/>
+      <c r="M31" t="b">
         <v>1</v>
       </c>
       <c r="N31">
@@ -3719,7 +3837,7 @@
       </c>
       <c r="Y31">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z31">
         <f t="shared" si="54"/>
@@ -3733,25 +3851,28 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
+      <c r="AC31">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A32" t="b">
-        <v>0</v>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>27</v>
       </c>
       <c r="B32" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D32" t="str">
+      <c r="E32" t="str">
         <f t="shared" si="55"/>
         <v>-</v>
       </c>
-      <c r="E32" t="str">
-        <f t="shared" si="54"/>
-        <v>-</v>
-      </c>
       <c r="F32" t="str">
         <f t="shared" si="54"/>
         <v>-</v>
@@ -3772,14 +3893,14 @@
         <f t="shared" si="54"/>
         <v>-</v>
       </c>
-      <c r="K32">
+      <c r="K32" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="L32">
         <v>1200</v>
       </c>
-      <c r="L32" t="b">
-        <v>1</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="54"/>
+      <c r="M32" t="b">
         <v>1</v>
       </c>
       <c r="N32">
@@ -3828,7 +3949,7 @@
       </c>
       <c r="Y32">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z32">
         <f t="shared" si="54"/>
@@ -3842,25 +3963,28 @@
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
+      <c r="AC32">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A33" t="b">
-        <v>0</v>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>28</v>
       </c>
       <c r="B33" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D33" t="str">
+      <c r="E33" t="str">
         <f t="shared" si="55"/>
         <v>-</v>
       </c>
-      <c r="E33" t="str">
-        <f t="shared" si="54"/>
-        <v>-</v>
-      </c>
       <c r="F33" t="str">
         <f t="shared" si="54"/>
         <v>-</v>
@@ -3881,14 +4005,14 @@
         <f t="shared" si="54"/>
         <v>-</v>
       </c>
-      <c r="K33">
+      <c r="K33" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="L33">
         <v>1600</v>
       </c>
-      <c r="L33" t="b">
-        <v>1</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="54"/>
+      <c r="M33" t="b">
         <v>1</v>
       </c>
       <c r="N33">
@@ -3937,7 +4061,7 @@
       </c>
       <c r="Y33">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z33">
         <f t="shared" si="54"/>
@@ -3948,12 +4072,16 @@
         <v>0</v>
       </c>
       <c r="AB33">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="AC33">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C4:X5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
+  <autoFilter ref="D4:Y5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
   <conditionalFormatting sqref="A1:XFD1">
     <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>"sav"</formula>
@@ -3976,7 +4104,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="24" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,A1)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(TRUE,B1)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -3989,7 +4117,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A1:B1048576</xm:sqref>
+          <xm:sqref>B1:C1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
report update and add mei
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B6A02A-6C77-4293-BA59-5E9373AFD152}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F554C81-4910-45C3-9661-BDC4E0712005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$Y$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$AC$4</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -88,6 +88,30 @@
           </rPr>
           <t xml:space="preserve">
 to keep the conditional formatting rules tidy, you can only insert a blank row or column (cant copy and insert paste) then you can copy the formula from a given row and paste it into your newly inserted row. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{10B3F34B-4772-43FF-8769-97F5228546B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Pandas doesn’t like it if you use % in the trial name description. The code will run fine you just wont be able to view the df.</t>
         </r>
       </text>
     </comment>
@@ -352,22 +376,22 @@
     <t>bnd_pasarea_inc</t>
   </si>
   <si>
-    <t>Pas area 40%</t>
-  </si>
-  <si>
-    <t>Pas area 60%</t>
-  </si>
-  <si>
-    <t>Pas area 80%</t>
-  </si>
-  <si>
-    <t>Pas area 10%</t>
-  </si>
-  <si>
     <t>Drop</t>
   </si>
   <si>
     <t>Trial Number</t>
+  </si>
+  <si>
+    <t>Pas area 10per</t>
+  </si>
+  <si>
+    <t>Pas area 40per</t>
+  </si>
+  <si>
+    <t>Pas area 60per</t>
+  </si>
+  <si>
+    <t>Pas area 80per</t>
   </si>
 </sst>
 </file>
@@ -851,10 +875,10 @@
   <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B30:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -866,7 +890,7 @@
   <sheetData>
     <row r="1" spans="1:29" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>45</v>
@@ -1076,7 +1100,7 @@
     </row>
     <row r="4" spans="1:29" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>40</v>
@@ -3643,7 +3667,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" t="str">
         <f>E$5</f>
@@ -3755,7 +3779,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" ref="E31:E33" si="55">E$5</f>
@@ -3867,7 +3891,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="55"/>
@@ -3979,7 +4003,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="55"/>
@@ -4081,7 +4105,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D4:Y5" xr:uid="{818CA8E6-CC86-4561-83A7-1B6023068E42}"/>
+  <autoFilter ref="D4:AC4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
   <conditionalFormatting sqref="A1:XFD1">
     <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
       <formula>"sav"</formula>

</xml_diff>

<commit_message>
more report changes and fixing mei
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F554C81-4910-45C3-9661-BDC4E0712005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639110FB-09F3-48E6-AF07-F379CE91E95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -878,17 +878,17 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B30:B33"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.54296875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -974,7 +974,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:29" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1098,7 +1098,7 @@
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
     </row>
-    <row r="4" spans="1:29" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -1166,7 +1166,7 @@
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>9</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>16</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>19</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>22</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>23</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>24</v>
       </c>
@@ -3656,12 +3656,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>25</v>
       </c>
       <c r="B30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -3768,12 +3768,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>26</v>
       </c>
       <c r="B31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -3880,12 +3880,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>27</v>
       </c>
       <c r="B32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -3992,12 +3992,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>28</v>
       </c>
       <c r="B33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
more report changes and fixing mei and nw remove feedpools set from harv stub nap con
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639110FB-09F3-48E6-AF07-F379CE91E95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FB7852-024A-45BB-9CEE-924124C82C05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$AC$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$AD$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -115,6 +115,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{28A87732-DFBE-4E72-8AD9-CC58CDE1082B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Must match the key assigned in Sensitivity.py</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D3" authorId="1" shapeId="0" xr:uid="{3BDB7BEB-FC53-4975-ADDB-A81C02A033DC}">
       <text>
         <r>
@@ -162,7 +186,7 @@
           <t xml:space="preserve">
 Optional
 - needed for arrays
-- can handel complex slicing I think</t>
+- can handel complex slicing. Use commer between each axis slice. Eg 2:3,1:2</t>
         </r>
       </text>
     </comment>
@@ -218,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
   <si>
     <t>sam</t>
   </si>
@@ -392,6 +416,15 @@
   </si>
   <si>
     <t>Pas area 80per</t>
+  </si>
+  <si>
+    <t>Both TOL inc</t>
+  </si>
+  <si>
+    <t>scan_og1</t>
+  </si>
+  <si>
+    <t>2:3,:</t>
   </si>
 </sst>
 </file>
@@ -509,7 +542,54 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -872,23 +952,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:AC33"/>
+  <dimension ref="A1:AD34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30:B33"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="17.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -926,7 +1006,7 @@
         <v>43</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>0</v>
@@ -962,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="AA1" s="6" t="s">
         <v>42</v>
@@ -970,11 +1050,14 @@
       <c r="AB1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
@@ -994,23 +1077,23 @@
         <v>48</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="P2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1024,10 +1107,10 @@
         <v>1</v>
       </c>
       <c r="T2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="V2" s="6" t="s">
         <v>10</v>
@@ -1041,11 +1124,14 @@
       <c r="Y2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="6"/>
+      <c r="Z2" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
     </row>
-    <row r="3" spans="1:29" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1058,9 +1144,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="N3" s="6"/>
       <c r="O3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1094,11 +1178,14 @@
       <c r="Y3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="Z3" s="6"/>
+      <c r="Z3" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
     </row>
-    <row r="4" spans="1:29" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -1126,48 +1213,52 @@
       <c r="I4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7" t="s">
+      <c r="N4" s="8"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="Q4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="R4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="S4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="T4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7" t="s">
+      <c r="U4" s="7"/>
+      <c r="V4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="Z4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f>ROW(A5)-5</f>
         <v>0</v>
       </c>
       <c r="B5" t="b">
@@ -1215,9 +1306,9 @@
         <f t="array" ref="M5">_xlfn.IFS(OR(M1="sam",M1="sai"),1,M1="sav","-",OR(M1="sap",M1="saa"),0)</f>
         <v>-</v>
       </c>
-      <c r="N5" s="9" cm="1">
+      <c r="N5" s="9" t="str" cm="1">
         <f t="array" ref="N5">_xlfn.IFS(OR(N1="sam",N1="sai"),1,N1="sav","-",OR(N1="sap",N1="saa"),0)</f>
-        <v>1</v>
+        <v>-</v>
       </c>
       <c r="O5" s="9" cm="1">
         <f t="array" ref="O5">_xlfn.IFS(OR(O1="sam",O1="sai"),1,O1="sav","-",OR(O1="sap",O1="saa"),0)</f>
@@ -1265,7 +1356,7 @@
       </c>
       <c r="Z5" s="9" cm="1">
         <f t="array" ref="Z5">_xlfn.IFS(OR(Z1="sam",Z1="sai"),1,Z1="sav","-",OR(Z1="sap",Z1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5" s="9" cm="1">
         <f t="array" ref="AA5">_xlfn.IFS(OR(AA1="sam",AA1="sai"),1,AA1="sav","-",OR(AA1="sap",AA1="saa"),0)</f>
@@ -1279,9 +1370,14 @@
         <f t="array" ref="AC5">_xlfn.IFS(OR(AC1="sam",AC1="sai"),1,AC1="sav","-",OR(AC1="sap",AC1="saa"),0)</f>
         <v>0</v>
       </c>
+      <c r="AD5" s="9" cm="1">
+        <f t="array" ref="AD5">_xlfn.IFS(OR(AD1="sam",AD1="sai"),1,AD1="sav","-",OR(AD1="sap",AD1="saa"),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" ref="A6:A34" si="0">ROW(A6)-5</f>
         <v>1</v>
       </c>
       <c r="B6" t="b">
@@ -1302,85 +1398,90 @@
         <v>-</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" ref="G6:I6" si="0">G5</f>
+        <f>G5</f>
         <v>-</v>
       </c>
       <c r="H6" t="str">
+        <f>H5</f>
+        <v>-</v>
+      </c>
+      <c r="I6" t="str">
+        <f>I5</f>
+        <v>-</v>
+      </c>
+      <c r="J6" t="str">
+        <f>J5</f>
+        <v>-</v>
+      </c>
+      <c r="K6" t="str">
+        <f>K5</f>
+        <v>-</v>
+      </c>
+      <c r="L6" t="str">
+        <f>L5</f>
+        <v>-</v>
+      </c>
+      <c r="M6" t="str">
+        <f>M5</f>
+        <v>-</v>
+      </c>
+      <c r="N6" t="str">
+        <f>N5</f>
+        <v>-</v>
+      </c>
+      <c r="O6">
+        <v>0.9</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <f>AD5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7">
         <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" ref="J6:M6" si="1">J5</f>
-        <v>-</v>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="L6" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="N6">
-        <v>0.9</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6">
-        <v>1</v>
-      </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6">
-        <v>1</v>
-      </c>
-      <c r="X6">
-        <v>1</v>
-      </c>
-      <c r="Y6">
-        <v>1</v>
-      </c>
-      <c r="Z6">
-        <v>1</v>
-      </c>
-      <c r="AA6">
-        <v>1</v>
-      </c>
-      <c r="AB6">
-        <v>1</v>
-      </c>
-      <c r="AC6">
-        <f>AC5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="b">
@@ -1393,47 +1494,48 @@
         <v>12</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E7:E29" si="2">E6</f>
+        <f t="shared" ref="E7:E29" si="1">E6</f>
         <v>-</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ref="F7:F29" si="3">F6</f>
+        <f t="shared" ref="F7:F29" si="2">F6</f>
         <v>-</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" ref="G7:G29" si="4">G6</f>
+        <f t="shared" ref="G7:G29" si="3">G6</f>
         <v>-</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" ref="H7:H29" si="5">H6</f>
+        <f t="shared" ref="H7:H29" si="4">H6</f>
         <v>-</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" ref="I7:I29" si="6">I6</f>
+        <f t="shared" ref="I7:J29" si="5">I6</f>
         <v>-</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ref="J7" si="7">J6</f>
+        <f t="shared" ref="J7" si="6">J6</f>
         <v>-</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" ref="K7:M7" si="8">K6</f>
+        <f t="shared" ref="K7" si="7">K6</f>
         <v>-</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="L7:N7" si="8">L6</f>
         <v>-</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="N7">
+      <c r="N7" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+      <c r="O7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
       <c r="P7">
         <v>1</v>
       </c>
@@ -1474,12 +1576,16 @@
         <v>1</v>
       </c>
       <c r="AC7">
-        <f t="shared" ref="AC7:AC29" si="9">AC6</f>
+        <v>1</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" ref="AD7:AD29" si="9">AD6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B8" t="b">
@@ -1492,23 +1598,23 @@
         <v>13</v>
       </c>
       <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F8" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" t="str">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="6"/>
         <v>-</v>
       </c>
       <c r="J8" t="str">
@@ -1516,26 +1622,27 @@
         <v>-</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" ref="K8:M8" si="11">K7</f>
+        <f t="shared" ref="K8" si="11">K7</f>
         <v>-</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="L8:N8" si="12">L7</f>
         <v>-</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="11"/>
-        <v>-</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>-</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="12"/>
+        <v>-</v>
       </c>
       <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
         <v>0.9</v>
       </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
       <c r="Q8">
         <v>1</v>
       </c>
@@ -1573,12 +1680,16 @@
         <v>1</v>
       </c>
       <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B9" t="b">
@@ -1591,50 +1702,51 @@
         <v>14</v>
       </c>
       <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F9" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I9" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J9" t="str">
-        <f t="shared" ref="J9" si="12">J8</f>
+        <f t="shared" ref="J9" si="13">J8</f>
         <v>-</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" ref="K9:M9" si="13">K8</f>
+        <f t="shared" ref="K9" si="14">K8</f>
         <v>-</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="L9:N9" si="15">L8</f>
         <v>-</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="13"/>
-        <v>-</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
+        <f t="shared" si="15"/>
+        <v>-</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="15"/>
+        <v>-</v>
       </c>
       <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
       <c r="Q9">
         <v>1</v>
       </c>
@@ -1672,12 +1784,16 @@
         <v>1</v>
       </c>
       <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AD9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B10" t="b">
@@ -1690,53 +1806,54 @@
         <v>15</v>
       </c>
       <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F10" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I10" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J10" t="str">
-        <f t="shared" ref="J10" si="14">J9</f>
+        <f t="shared" ref="J10" si="16">J9</f>
         <v>-</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" ref="K10:M10" si="15">K9</f>
+        <f t="shared" ref="K10" si="17">K9</f>
         <v>-</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="L10:N10" si="18">L9</f>
         <v>-</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="15"/>
-        <v>-</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
+        <f t="shared" si="18"/>
+        <v>-</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="18"/>
+        <v>-</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
       <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
         <v>0.9</v>
       </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
       <c r="R10">
         <v>1</v>
       </c>
@@ -1771,12 +1888,16 @@
         <v>1</v>
       </c>
       <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B11" t="b">
@@ -1789,53 +1910,54 @@
         <v>16</v>
       </c>
       <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F11" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I11" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J11" t="str">
-        <f t="shared" ref="J11" si="16">J10</f>
+        <f t="shared" ref="J11" si="19">J10</f>
         <v>-</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" ref="K11:M11" si="17">K10</f>
+        <f t="shared" ref="K11" si="20">K10</f>
         <v>-</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="L11:N11" si="21">L10</f>
         <v>-</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="17"/>
-        <v>-</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
       <c r="R11">
         <v>1</v>
       </c>
@@ -1870,12 +1992,16 @@
         <v>1</v>
       </c>
       <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B12" t="b">
@@ -1888,43 +2014,44 @@
         <v>22</v>
       </c>
       <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F12" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12" si="18">J11</f>
+        <f t="shared" ref="J12" si="22">J11</f>
         <v>-</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" ref="K12:M12" si="19">K11</f>
+        <f t="shared" ref="K12" si="23">K11</f>
         <v>-</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="L12:N12" si="24">L11</f>
         <v>-</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="19"/>
-        <v>-</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
       </c>
       <c r="O12">
         <v>1</v>
@@ -1933,11 +2060,11 @@
         <v>1</v>
       </c>
       <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
         <v>0.9</v>
       </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
       <c r="S12">
         <v>1</v>
       </c>
@@ -1969,12 +2096,16 @@
         <v>1</v>
       </c>
       <c r="AC12">
+        <v>1</v>
+      </c>
+      <c r="AD12">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B13" t="b">
@@ -1987,43 +2118,44 @@
         <v>17</v>
       </c>
       <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F13" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I13" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J13" t="str">
-        <f t="shared" ref="J13" si="20">J12</f>
+        <f t="shared" ref="J13" si="25">J12</f>
         <v>-</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" ref="K13:M13" si="21">K12</f>
+        <f t="shared" ref="K13" si="26">K12</f>
         <v>-</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="L13:N13" si="27">L12</f>
         <v>-</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="21"/>
-        <v>-</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
       </c>
       <c r="O13">
         <v>1</v>
@@ -2032,11 +2164,11 @@
         <v>1</v>
       </c>
       <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
       <c r="S13">
         <v>1</v>
       </c>
@@ -2068,12 +2200,16 @@
         <v>1</v>
       </c>
       <c r="AC13">
+        <v>1</v>
+      </c>
+      <c r="AD13">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B14" t="b">
@@ -2086,43 +2222,44 @@
         <v>18</v>
       </c>
       <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F14" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F14" t="str">
+      <c r="G14" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H14" t="str">
+      <c r="I14" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I14" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J14" t="str">
-        <f t="shared" ref="J14" si="22">J13</f>
+        <f t="shared" ref="J14" si="28">J13</f>
         <v>-</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" ref="K14:M14" si="23">K13</f>
+        <f t="shared" ref="K14" si="29">K13</f>
         <v>-</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="L14:N14" si="30">L13</f>
         <v>-</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="23"/>
-        <v>-</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
       </c>
       <c r="O14">
         <v>1</v>
@@ -2134,11 +2271,11 @@
         <v>1</v>
       </c>
       <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
         <v>0.9</v>
       </c>
-      <c r="S14">
-        <v>1</v>
-      </c>
       <c r="T14">
         <v>1</v>
       </c>
@@ -2167,12 +2304,16 @@
         <v>1</v>
       </c>
       <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AD14">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B15" t="b">
@@ -2185,43 +2326,44 @@
         <v>19</v>
       </c>
       <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F15" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H15" t="str">
+      <c r="I15" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I15" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J15" t="str">
-        <f t="shared" ref="J15" si="24">J14</f>
+        <f t="shared" ref="J15" si="31">J14</f>
         <v>-</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" ref="K15:M15" si="25">K14</f>
+        <f t="shared" ref="K15" si="32">K14</f>
         <v>-</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="L15:N15" si="33">L14</f>
         <v>-</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="25"/>
-        <v>-</v>
-      </c>
-      <c r="N15">
-        <v>1</v>
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
       </c>
       <c r="O15">
         <v>1</v>
@@ -2233,11 +2375,11 @@
         <v>1</v>
       </c>
       <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
       <c r="T15">
         <v>1</v>
       </c>
@@ -2266,12 +2408,16 @@
         <v>1</v>
       </c>
       <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B16" t="b">
@@ -2284,43 +2430,44 @@
         <v>20</v>
       </c>
       <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F16" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I16" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J16" t="str">
-        <f t="shared" ref="J16" si="26">J15</f>
+        <f t="shared" ref="J16" si="34">J15</f>
         <v>-</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" ref="K16:M16" si="27">K15</f>
+        <f t="shared" ref="K16" si="35">K15</f>
         <v>-</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="L16:N16" si="36">L15</f>
         <v>-</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="27"/>
-        <v>-</v>
-      </c>
-      <c r="N16">
-        <v>1</v>
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
       </c>
       <c r="O16">
         <v>1</v>
@@ -2335,11 +2482,11 @@
         <v>1</v>
       </c>
       <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
         <v>0.9</v>
       </c>
-      <c r="T16">
-        <v>1</v>
-      </c>
       <c r="U16">
         <v>1</v>
       </c>
@@ -2365,12 +2512,16 @@
         <v>1</v>
       </c>
       <c r="AC16">
+        <v>1</v>
+      </c>
+      <c r="AD16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B17" t="b">
@@ -2383,43 +2534,44 @@
         <v>21</v>
       </c>
       <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F17" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I17" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J17" t="str">
-        <f t="shared" ref="J17" si="28">J16</f>
+        <f t="shared" ref="J17" si="37">J16</f>
         <v>-</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" ref="K17:M17" si="29">K16</f>
+        <f t="shared" ref="K17" si="38">K16</f>
         <v>-</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="L17:N17" si="39">L16</f>
         <v>-</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="29"/>
-        <v>-</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
       </c>
       <c r="O17">
         <v>1</v>
@@ -2434,11 +2586,11 @@
         <v>1</v>
       </c>
       <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
       <c r="U17">
         <v>1</v>
       </c>
@@ -2464,12 +2616,16 @@
         <v>1</v>
       </c>
       <c r="AC17">
+        <v>1</v>
+      </c>
+      <c r="AD17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B18" t="b">
@@ -2482,43 +2638,44 @@
         <v>23</v>
       </c>
       <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F18" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H18" t="str">
+      <c r="I18" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I18" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18" si="30">J17</f>
+        <f t="shared" ref="J18" si="40">J17</f>
         <v>-</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" ref="K18:M18" si="31">K17</f>
+        <f t="shared" ref="K18" si="41">K17</f>
         <v>-</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="L18:N18" si="42">L17</f>
         <v>-</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="31"/>
-        <v>-</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
+        <f t="shared" si="42"/>
+        <v>-</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="42"/>
+        <v>-</v>
       </c>
       <c r="O18">
         <v>1</v>
@@ -2536,11 +2693,11 @@
         <v>1</v>
       </c>
       <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
         <v>0.9</v>
       </c>
-      <c r="U18">
-        <v>1</v>
-      </c>
       <c r="V18">
         <v>1</v>
       </c>
@@ -2563,12 +2720,16 @@
         <v>1</v>
       </c>
       <c r="AC18">
+        <v>1</v>
+      </c>
+      <c r="AD18">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B19" t="b">
@@ -2581,43 +2742,44 @@
         <v>24</v>
       </c>
       <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F19" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H19" t="str">
+      <c r="I19" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I19" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J19" t="str">
-        <f t="shared" ref="J19" si="32">J18</f>
+        <f t="shared" ref="J19" si="43">J18</f>
         <v>-</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" ref="K19:M19" si="33">K18</f>
+        <f t="shared" ref="K19" si="44">K18</f>
         <v>-</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="L19:N19" si="45">L18</f>
         <v>-</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="33"/>
-        <v>-</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
+        <f t="shared" si="45"/>
+        <v>-</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="45"/>
+        <v>-</v>
       </c>
       <c r="O19">
         <v>1</v>
@@ -2635,11 +2797,11 @@
         <v>1</v>
       </c>
       <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="U19">
-        <v>1</v>
-      </c>
       <c r="V19">
         <v>1</v>
       </c>
@@ -2662,12 +2824,16 @@
         <v>1</v>
       </c>
       <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B20" t="b">
@@ -2680,43 +2846,44 @@
         <v>25</v>
       </c>
       <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F20" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F20" t="str">
+      <c r="G20" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H20" t="str">
+      <c r="I20" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I20" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J20" t="str">
-        <f t="shared" ref="J20" si="34">J19</f>
+        <f t="shared" ref="J20" si="46">J19</f>
         <v>-</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" ref="K20:M20" si="35">K19</f>
+        <f t="shared" ref="K20" si="47">K19</f>
         <v>-</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="L20:N20" si="48">L19</f>
         <v>-</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="35"/>
-        <v>-</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
+        <f t="shared" si="48"/>
+        <v>-</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="48"/>
+        <v>-</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -2737,11 +2904,11 @@
         <v>1</v>
       </c>
       <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
         <v>0.9</v>
       </c>
-      <c r="V20">
-        <v>1</v>
-      </c>
       <c r="W20">
         <v>1</v>
       </c>
@@ -2761,12 +2928,16 @@
         <v>1</v>
       </c>
       <c r="AC20">
+        <v>1</v>
+      </c>
+      <c r="AD20">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21">
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B21" t="b">
@@ -2779,43 +2950,44 @@
         <v>26</v>
       </c>
       <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F21" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F21" t="str">
+      <c r="G21" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G21" t="str">
+      <c r="H21" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H21" t="str">
+      <c r="I21" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I21" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J21" t="str">
-        <f t="shared" ref="J21" si="36">J20</f>
+        <f t="shared" ref="J21" si="49">J20</f>
         <v>-</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" ref="K21:M21" si="37">K20</f>
+        <f t="shared" ref="K21" si="50">K20</f>
         <v>-</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="L21:N21" si="51">L20</f>
         <v>-</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="37"/>
-        <v>-</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
+        <f t="shared" si="51"/>
+        <v>-</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="51"/>
+        <v>-</v>
       </c>
       <c r="O21">
         <v>1</v>
@@ -2836,11 +3008,11 @@
         <v>1</v>
       </c>
       <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="V21">
-        <v>1</v>
-      </c>
       <c r="W21">
         <v>1</v>
       </c>
@@ -2860,12 +3032,16 @@
         <v>1</v>
       </c>
       <c r="AC21">
+        <v>1</v>
+      </c>
+      <c r="AD21">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B22" t="b">
@@ -2878,43 +3054,44 @@
         <v>27</v>
       </c>
       <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F22" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F22" t="str">
+      <c r="G22" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G22" t="str">
+      <c r="H22" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H22" t="str">
+      <c r="I22" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I22" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J22" t="str">
-        <f t="shared" ref="J22" si="38">J21</f>
+        <f t="shared" ref="J22" si="52">J21</f>
         <v>-</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" ref="K22:M22" si="39">K21</f>
+        <f t="shared" ref="K22" si="53">K21</f>
         <v>-</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="L22:N22" si="54">L21</f>
         <v>-</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="39"/>
-        <v>-</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
+        <f t="shared" si="54"/>
+        <v>-</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="54"/>
+        <v>-</v>
       </c>
       <c r="O22">
         <v>1</v>
@@ -2938,11 +3115,11 @@
         <v>1</v>
       </c>
       <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
         <v>0.9</v>
       </c>
-      <c r="W22">
-        <v>1</v>
-      </c>
       <c r="X22">
         <v>1</v>
       </c>
@@ -2959,12 +3136,16 @@
         <v>1</v>
       </c>
       <c r="AC22">
+        <v>1</v>
+      </c>
+      <c r="AD22">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B23" t="b">
@@ -2977,43 +3158,44 @@
         <v>28</v>
       </c>
       <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F23" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F23" t="str">
+      <c r="G23" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G23" t="str">
+      <c r="H23" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H23" t="str">
+      <c r="I23" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I23" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J23" t="str">
-        <f t="shared" ref="J23" si="40">J22</f>
+        <f t="shared" ref="J23" si="55">J22</f>
         <v>-</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" ref="K23:M23" si="41">K22</f>
+        <f t="shared" ref="K23" si="56">K22</f>
         <v>-</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="L23:N23" si="57">L22</f>
         <v>-</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="41"/>
-        <v>-</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
+        <f t="shared" si="57"/>
+        <v>-</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="57"/>
+        <v>-</v>
       </c>
       <c r="O23">
         <v>1</v>
@@ -3037,11 +3219,11 @@
         <v>1</v>
       </c>
       <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="W23">
-        <v>1</v>
-      </c>
       <c r="X23">
         <v>1</v>
       </c>
@@ -3058,12 +3240,16 @@
         <v>1</v>
       </c>
       <c r="AC23">
+        <v>1</v>
+      </c>
+      <c r="AD23">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B24" t="b">
@@ -3076,43 +3262,44 @@
         <v>29</v>
       </c>
       <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F24" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F24" t="str">
+      <c r="G24" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G24" t="str">
+      <c r="H24" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H24" t="str">
+      <c r="I24" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I24" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J24" t="str">
-        <f t="shared" ref="J24" si="42">J23</f>
+        <f t="shared" ref="J24" si="58">J23</f>
         <v>-</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" ref="K24:M24" si="43">K23</f>
+        <f t="shared" ref="K24" si="59">K23</f>
         <v>-</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" ref="L24:N24" si="60">L23</f>
         <v>-</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="43"/>
-        <v>-</v>
-      </c>
-      <c r="N24">
-        <v>1</v>
+        <f t="shared" si="60"/>
+        <v>-</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="60"/>
+        <v>-</v>
       </c>
       <c r="O24">
         <v>1</v>
@@ -3139,11 +3326,11 @@
         <v>1</v>
       </c>
       <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
         <v>0.9</v>
       </c>
-      <c r="X24">
-        <v>1</v>
-      </c>
       <c r="Y24">
         <v>1</v>
       </c>
@@ -3157,12 +3344,16 @@
         <v>1</v>
       </c>
       <c r="AC24">
+        <v>1</v>
+      </c>
+      <c r="AD24">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B25" t="b">
@@ -3175,43 +3366,44 @@
         <v>30</v>
       </c>
       <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F25" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F25" t="str">
+      <c r="G25" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G25" t="str">
+      <c r="H25" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H25" t="str">
+      <c r="I25" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I25" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J25" t="str">
-        <f t="shared" ref="J25" si="44">J24</f>
+        <f t="shared" ref="J25" si="61">J24</f>
         <v>-</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" ref="K25:M25" si="45">K24</f>
+        <f t="shared" ref="K25" si="62">K24</f>
         <v>-</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" ref="L25:N25" si="63">L24</f>
         <v>-</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="45"/>
-        <v>-</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
+        <f t="shared" si="63"/>
+        <v>-</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="63"/>
+        <v>-</v>
       </c>
       <c r="O25">
         <v>1</v>
@@ -3238,11 +3430,11 @@
         <v>1</v>
       </c>
       <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="X25">
-        <v>1</v>
-      </c>
       <c r="Y25">
         <v>1</v>
       </c>
@@ -3256,12 +3448,16 @@
         <v>1</v>
       </c>
       <c r="AC25">
+        <v>1</v>
+      </c>
+      <c r="AD25">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26">
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B26" t="b">
@@ -3274,43 +3470,44 @@
         <v>31</v>
       </c>
       <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F26" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F26" t="str">
+      <c r="G26" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G26" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H26" t="str">
+      <c r="I26" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I26" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J26" t="str">
-        <f t="shared" ref="J26" si="46">J25</f>
+        <f t="shared" ref="J26" si="64">J25</f>
         <v>-</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" ref="K26:M26" si="47">K25</f>
+        <f t="shared" ref="K26" si="65">K25</f>
         <v>-</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" ref="L26:N26" si="66">L25</f>
         <v>-</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="47"/>
-        <v>-</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
+        <f t="shared" si="66"/>
+        <v>-</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="66"/>
+        <v>-</v>
       </c>
       <c r="O26">
         <v>1</v>
@@ -3340,11 +3537,11 @@
         <v>1</v>
       </c>
       <c r="X26">
+        <v>1</v>
+      </c>
+      <c r="Y26">
         <v>0.9</v>
       </c>
-      <c r="Y26">
-        <v>1</v>
-      </c>
       <c r="Z26">
         <v>1</v>
       </c>
@@ -3355,12 +3552,16 @@
         <v>1</v>
       </c>
       <c r="AC26">
+        <v>1</v>
+      </c>
+      <c r="AD26">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27">
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B27" t="b">
@@ -3373,43 +3574,44 @@
         <v>32</v>
       </c>
       <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F27" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F27" t="str">
+      <c r="G27" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G27" t="str">
+      <c r="H27" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H27" t="str">
+      <c r="I27" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I27" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J27" t="str">
-        <f t="shared" ref="J27" si="48">J26</f>
+        <f t="shared" ref="J27" si="67">J26</f>
         <v>-</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" ref="K27:M27" si="49">K26</f>
+        <f t="shared" ref="K27" si="68">K26</f>
         <v>-</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" ref="L27:N27" si="69">L26</f>
         <v>-</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="49"/>
-        <v>-</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
+        <f t="shared" si="69"/>
+        <v>-</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="69"/>
+        <v>-</v>
       </c>
       <c r="O27">
         <v>1</v>
@@ -3439,11 +3641,11 @@
         <v>1</v>
       </c>
       <c r="X27">
+        <v>1</v>
+      </c>
+      <c r="Y27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
       <c r="Z27">
         <v>1</v>
       </c>
@@ -3454,12 +3656,16 @@
         <v>1</v>
       </c>
       <c r="AC27">
+        <v>1</v>
+      </c>
+      <c r="AD27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B28" t="b">
@@ -3472,43 +3678,44 @@
         <v>33</v>
       </c>
       <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F28" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F28" t="str">
+      <c r="G28" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H28" t="str">
+      <c r="I28" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I28" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J28" t="str">
-        <f t="shared" ref="J28" si="50">J27</f>
+        <f t="shared" ref="J28" si="70">J27</f>
         <v>-</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" ref="K28:M28" si="51">K27</f>
+        <f t="shared" ref="K28" si="71">K27</f>
         <v>-</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" ref="L28:N28" si="72">L27</f>
         <v>-</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" si="51"/>
-        <v>-</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
+        <f t="shared" si="72"/>
+        <v>-</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="72"/>
+        <v>-</v>
       </c>
       <c r="O28">
         <v>1</v>
@@ -3541,11 +3748,11 @@
         <v>1</v>
       </c>
       <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="Z28">
         <v>0.9</v>
       </c>
-      <c r="Z28">
-        <v>1</v>
-      </c>
       <c r="AA28">
         <v>1</v>
       </c>
@@ -3553,12 +3760,16 @@
         <v>1</v>
       </c>
       <c r="AC28">
+        <v>1</v>
+      </c>
+      <c r="AD28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B29" t="b">
@@ -3571,43 +3782,44 @@
         <v>34</v>
       </c>
       <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="F29" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F29" t="str">
+      <c r="G29" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G29" t="str">
+      <c r="H29" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
       </c>
-      <c r="H29" t="str">
+      <c r="I29" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="I29" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
       <c r="J29" t="str">
-        <f t="shared" ref="J29" si="52">J28</f>
+        <f t="shared" ref="J29" si="73">J28</f>
         <v>-</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" ref="K29:M29" si="53">K28</f>
+        <f t="shared" ref="K29" si="74">K28</f>
         <v>-</v>
       </c>
       <c r="L29" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="L29:N29" si="75">L28</f>
         <v>-</v>
       </c>
       <c r="M29" t="str">
-        <f t="shared" si="53"/>
-        <v>-</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
+        <f t="shared" si="75"/>
+        <v>-</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="75"/>
+        <v>-</v>
       </c>
       <c r="O29">
         <v>1</v>
@@ -3640,11 +3852,11 @@
         <v>1</v>
       </c>
       <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="Z29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Z29">
-        <v>1</v>
-      </c>
       <c r="AA29">
         <v>1</v>
       </c>
@@ -3652,12 +3864,16 @@
         <v>1</v>
       </c>
       <c r="AC29">
+        <v>1</v>
+      </c>
+      <c r="AD29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30">
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B30" t="b">
@@ -3674,102 +3890,107 @@
         <v>-</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ref="F30:AC33" si="54">F$5</f>
+        <f t="shared" ref="F30:AD34" si="76">F$5</f>
         <v>-</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="I30" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="54"/>
-        <v>-</v>
-      </c>
-      <c r="L30">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="M30">
         <v>200</v>
       </c>
-      <c r="M30" t="b">
-        <v>1</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="54"/>
+      <c r="N30" t="b">
         <v>1</v>
       </c>
       <c r="O30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="P30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="R30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="S30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="T30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="U30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="V30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="W30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="X30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="54"/>
-        <v>0</v>
+        <f t="shared" si="76"/>
+        <v>1</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="AB30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="AC30">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B31" t="b">
@@ -3782,106 +4003,111 @@
         <v>55</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" ref="E31:E33" si="55">E$5</f>
+        <f t="shared" ref="E31:E33" si="77">E$5</f>
         <v>-</v>
       </c>
       <c r="F31" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="I31" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="54"/>
-        <v>-</v>
-      </c>
-      <c r="L31">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="M31">
         <v>800</v>
       </c>
-      <c r="M31" t="b">
-        <v>1</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="54"/>
+      <c r="N31" t="b">
         <v>1</v>
       </c>
       <c r="O31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="P31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="R31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="S31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="T31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="U31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="V31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="W31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="X31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="54"/>
-        <v>0</v>
+        <f t="shared" si="76"/>
+        <v>1</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="AC31">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32">
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B32" t="b">
@@ -3894,106 +4120,111 @@
         <v>56</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="77"/>
         <v>-</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="I32" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="54"/>
-        <v>-</v>
-      </c>
-      <c r="L32">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="M32">
         <v>1200</v>
       </c>
-      <c r="M32" t="b">
-        <v>1</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="54"/>
+      <c r="N32" t="b">
         <v>1</v>
       </c>
       <c r="O32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="P32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="R32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="S32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="T32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="U32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="V32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="W32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="X32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="54"/>
-        <v>0</v>
+        <f t="shared" si="76"/>
+        <v>1</v>
       </c>
       <c r="AA32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="AB32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="AC32">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B33" t="b">
@@ -4006,117 +4237,238 @@
         <v>57</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="77"/>
         <v>-</v>
       </c>
       <c r="F33" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="I33" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>-</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="54"/>
-        <v>-</v>
-      </c>
-      <c r="L33">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="M33">
         <v>1600</v>
       </c>
-      <c r="M33" t="b">
-        <v>1</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="54"/>
+      <c r="N33" t="b">
         <v>1</v>
       </c>
       <c r="O33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="P33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="R33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="S33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="T33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="U33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="V33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="W33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="X33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>1</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="54"/>
-        <v>0</v>
+        <f t="shared" si="76"/>
+        <v>1</v>
       </c>
       <c r="AA33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="AB33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="AC33">
-        <f t="shared" si="54"/>
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="M34" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="N34" t="str">
+        <f t="shared" si="76"/>
+        <v>-</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="AC34">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D4:AC4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
+  <autoFilter ref="D4:AD4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="21" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="8" priority="22" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="22" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="7" priority="23" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="23" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4127,7 +4479,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
+          <x14:cfRule type="containsText" priority="25" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,B1)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
@@ -4141,7 +4493,24 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B1:C1048576</xm:sqref>
+          <xm:sqref>B35:C1048576 B34 B1:C33</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
+            <xm:f>NOT(ISERROR(SEARCH(TRUE,C34)))</xm:f>
+            <xm:f>TRUE</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C34</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Fix FEC reporting (not complete)
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DADDB03-F833-4B24-B15A-F717B13B584B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AC30B1-BA8A-4E1E-A674-286896554828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="3120" yWindow="840" windowWidth="18870" windowHeight="15360" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$AE$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -220,14 +212,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -944,10 +936,10 @@
   <dimension ref="A1:AE35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4579,7 +4571,7 @@
         <v>30</v>
       </c>
       <c r="B35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
fec fixed and working (i think)
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AC30B1-BA8A-4E1E-A674-286896554828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A2D6E8-4904-41E9-B152-6EF9F9CF8937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="840" windowWidth="18870" windowHeight="15360" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -212,14 +220,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -234,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="63">
   <si>
     <t>sam</t>
   </si>
@@ -540,7 +548,27 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -933,23 +961,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:AE35"/>
+  <dimension ref="A1:AE36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="17.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -1041,7 +1069,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1118,7 +1146,7 @@
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
     </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1173,7 +1201,7 @@
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
     </row>
-    <row r="4" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -1245,7 +1273,7 @@
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5">
         <f>ROW(A5)-5</f>
         <v>0</v>
@@ -1368,9 +1396,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f t="shared" ref="A6:A35" si="0">ROW(A6)-5</f>
+        <f t="shared" ref="A6:A36" si="0">ROW(A6)-5</f>
         <v>1</v>
       </c>
       <c r="B6" t="b">
@@ -1476,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1584,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1692,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1800,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1908,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2016,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2124,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2232,7 +2260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2340,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2448,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2556,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2664,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2772,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2880,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2988,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3096,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3204,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3312,7 +3340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3420,7 +3448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3528,7 +3556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3636,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3744,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3852,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3960,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3979,7 +4007,7 @@
         <v>-</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ref="E30:AE35" si="100">F$5</f>
+        <f t="shared" ref="E30:AE36" si="100">F$5</f>
         <v>-</v>
       </c>
       <c r="G30" t="str">
@@ -4081,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4202,7 +4230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4323,7 +4351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4444,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4565,124 +4593,246 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="M35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="N35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AB35">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AC35">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="F35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="G35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="H35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="I35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="J35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="K35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="L35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="M35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="N35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="O35" t="b">
-        <v>1</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="T35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="U35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="V35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="W35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="X35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Y35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Z35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="AA35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="AB35">
-        <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="AC35">
-        <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="AD35">
-        <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="AE35">
+      <c r="E36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="O36" t="b">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Z36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AB36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AE36">
         <f t="shared" si="100"/>
         <v>0</v>
       </c>
@@ -4690,16 +4840,16 @@
   </sheetData>
   <autoFilter ref="D4:AE4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="7" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="8" priority="26" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="25" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="7" priority="27" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="26" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="6" priority="28" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4710,7 +4860,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="27" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
+          <x14:cfRule type="containsText" priority="29" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,B1)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
@@ -4724,10 +4874,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B36:C1048576 B34 B1:C33</xm:sqref>
+          <xm:sqref>B37:C1048576 B1:C33 B34:B35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,C34)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
@@ -4744,8 +4894,8 @@
           <xm:sqref>C34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{68BE4C5B-1861-4433-9716-6C3C5697FFFA}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,B35)))</xm:f>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{DDDE047A-6A94-4B19-BC19-507EF1A1F811}">
+            <xm:f>NOT(ISERROR(SEARCH(TRUE,B36)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -4758,10 +4908,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B35</xm:sqref>
+          <xm:sqref>B36:C36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{DDDE047A-6A94-4B19-BC19-507EF1A1F811}">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{A0A976DA-27E6-4B6E-9D9F-24E8BBBA62F3}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,C35)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>

</xml_diff>

<commit_message>
fixes to allow two genotypes
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE22694-C1D2-4352-8BDC-13FE8C1F235A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B054CFD6-74FA-4330-A18D-C7631E14A228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
   <si>
     <t>sam</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>BBT inc</t>
+  </si>
+  <si>
+    <t>TOL 2 only</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,27 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -944,13 +967,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:AE36"/>
+  <dimension ref="A1:AE37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1262,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
@@ -1381,7 +1404,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f t="shared" ref="A6:A36" si="0">ROW(A6)-5</f>
+        <f t="shared" ref="A6:A37" si="0">ROW(A6)-5</f>
         <v>1</v>
       </c>
       <c r="B6" t="b">
@@ -3990,7 +4013,7 @@
         <v>-</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ref="E30:AE36" si="100">F$5</f>
+        <f t="shared" ref="E30:AE37" si="100">F$5</f>
         <v>-</v>
       </c>
       <c r="G30" t="str">
@@ -4461,7 +4484,7 @@
         <v>29</v>
       </c>
       <c r="B34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -4588,15 +4611,13 @@
         <v>0</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="F35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
+        <v>64</v>
+      </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <v>1</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="100"/>
@@ -4606,8 +4627,9 @@
         <f t="shared" si="100"/>
         <v>-</v>
       </c>
-      <c r="I35" t="b">
-        <v>1</v>
+      <c r="I35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="100"/>
@@ -4710,112 +4732,234 @@
         <v>0</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="M36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="N36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Z36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AB36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B37" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="F36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="G36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="H36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="I36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="J36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="K36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="L36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="M36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="N36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="O36" t="b">
-        <v>1</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="T36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="U36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="V36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="W36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="X36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Y36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Z36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="AA36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="AB36">
-        <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="AC36">
-        <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="AD36">
-        <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="AE36">
+      <c r="E37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="I37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="O37" t="b">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AE37">
         <f t="shared" si="100"/>
         <v>0</v>
       </c>
@@ -4823,16 +4967,16 @@
   </sheetData>
   <autoFilter ref="D4:AE4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="7" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="24" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="26" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="8" priority="28" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="27" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="7" priority="29" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="28" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="6" priority="30" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4843,7 +4987,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="29" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
+          <x14:cfRule type="containsText" priority="31" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,B1)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
@@ -4857,10 +5001,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B37:C1048576 B1:C33 B34:B36</xm:sqref>
+          <xm:sqref>B38:C1048576 B34:B37 B1:C33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,C34)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
@@ -4877,7 +5021,24 @@
           <xm:sqref>C34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{DDDE047A-6A94-4B19-BC19-507EF1A1F811}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{DDDE047A-6A94-4B19-BC19-507EF1A1F811}">
+            <xm:f>NOT(ISERROR(SEARCH(TRUE,C37)))</xm:f>
+            <xm:f>TRUE</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C37</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{A0A976DA-27E6-4B6E-9D9F-24E8BBBA62F3}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,C36)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
@@ -4894,7 +5055,7 @@
           <xm:sqref>C36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{A0A976DA-27E6-4B6E-9D9F-24E8BBBA62F3}">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{1B445044-CC40-4A49-93E2-E84C4E8D18AA}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,C35)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>

</xml_diff>

<commit_message>
change excel reader engine. fix sire require for bbt
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B054CFD6-74FA-4330-A18D-C7631E14A228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A94A1AE-1E5F-4580-9FC8-E77761610C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -973,7 +973,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
+      <selection pane="bottomRight" activeCell="C37" sqref="B37:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4726,7 +4726,7 @@
         <v>31</v>
       </c>
       <c r="B36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -4848,7 +4848,7 @@
         <v>32</v>
       </c>
       <c r="B37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -5001,7 +5001,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B38:C1048576 B34:B37 B1:C33</xm:sqref>
+          <xm:sqref>B38:C1048576 B1:C33 B34:B36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="7" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
@@ -5022,7 +5022,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="5" operator="containsText" id="{DDDE047A-6A94-4B19-BC19-507EF1A1F811}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,C37)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(TRUE,B37)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -5035,7 +5035,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C37</xm:sqref>
+          <xm:sqref>B37:C37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="3" operator="containsText" id="{A0A976DA-27E6-4B6E-9D9F-24E8BBBA62F3}">

</xml_diff>

<commit_message>
fix prog2dams and prog2off constraint to work with t axis
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A94A1AE-1E5F-4580-9FC8-E77761610C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CFA3F7-E089-4F54-8FAD-0207BB70D07E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="66">
   <si>
     <t>sam</t>
   </si>
@@ -434,6 +434,9 @@
   </si>
   <si>
     <t>BBT inc</t>
+  </si>
+  <si>
+    <t>TOL 1 only</t>
   </si>
   <si>
     <t>TOL 2 only</t>
@@ -554,37 +557,7 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -967,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:AE37"/>
+  <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="C37" sqref="B37:C37"/>
@@ -1404,7 +1377,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6">
-        <f t="shared" ref="A6:A37" si="0">ROW(A6)-5</f>
+        <f t="shared" ref="A6:A38" si="0">ROW(A6)-5</f>
         <v>1</v>
       </c>
       <c r="B6" t="b">
@@ -4013,7 +3986,7 @@
         <v>-</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ref="E30:AE37" si="100">F$5</f>
+        <f t="shared" ref="E30:AE38" si="100">F$5</f>
         <v>-</v>
       </c>
       <c r="G30" t="str">
@@ -4487,7 +4460,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>58</v>
@@ -4608,16 +4581,16 @@
         <v>0</v>
       </c>
       <c r="C35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="100"/>
@@ -4726,21 +4699,19 @@
         <v>31</v>
       </c>
       <c r="B36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="F36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
+        <v>65</v>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="100"/>
@@ -4750,8 +4721,9 @@
         <f t="shared" si="100"/>
         <v>-</v>
       </c>
-      <c r="I36" t="b">
-        <v>1</v>
+      <c r="I36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="100"/>
@@ -4848,118 +4820,240 @@
         <v>32</v>
       </c>
       <c r="B37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="H37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="M37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AB37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AC37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AD37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AE37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B38" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="F37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="G37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="H37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="I37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="J37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="K37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="L37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="M37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="N37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="O37" t="b">
-        <v>1</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="T37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="U37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="V37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="W37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="X37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Y37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Z37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="AA37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="AB37">
-        <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="AC37">
-        <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="AD37">
-        <f t="shared" si="100"/>
-        <v>0</v>
-      </c>
-      <c r="AE37">
+      <c r="E38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="H38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="M38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="N38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="O38" t="b">
+        <v>1</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AB38">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AC38">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AD38">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AE38">
         <f t="shared" si="100"/>
         <v>0</v>
       </c>
@@ -4967,16 +5061,16 @@
   </sheetData>
   <autoFilter ref="D4:AE4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="9" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="26" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="28" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="5" priority="30" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="29" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="4" priority="31" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="30" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="3" priority="32" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4987,7 +5081,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="31" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
+          <x14:cfRule type="containsText" priority="33" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
             <xm:f>NOT(ISERROR(SEARCH(TRUE,B1)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
@@ -5001,11 +5095,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B38:C1048576 B1:C33 B34:B36</xm:sqref>
+          <xm:sqref>B39:C1048576 B34:B36 B1:C33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,C34)))</xm:f>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
+            <xm:f>NOT(ISERROR(SEARCH(TRUE,B34)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -5018,11 +5112,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C34</xm:sqref>
+          <xm:sqref>C34:C37 B37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{DDDE047A-6A94-4B19-BC19-507EF1A1F811}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,B37)))</xm:f>
+          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{DDDE047A-6A94-4B19-BC19-507EF1A1F811}">
+            <xm:f>NOT(ISERROR(SEARCH(TRUE,B38)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -5035,41 +5129,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B37:C37</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{A0A976DA-27E6-4B6E-9D9F-24E8BBBA62F3}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,C36)))</xm:f>
-            <xm:f>TRUE</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C36</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{1B445044-CC40-4A49-93E2-E84C4E8D18AA}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,C35)))</xm:f>
-            <xm:f>TRUE</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C35</xm:sqref>
+          <xm:sqref>B38:C38</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
fix problem due to changing worker set names
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CFA3F7-E089-4F54-8FAD-0207BB70D07E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C154BC24-E2E9-4451-8290-39FAA7BEEB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="30990" yWindow="2520" windowWidth="21600" windowHeight="11055" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -943,10 +943,10 @@
   <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="B37:C37"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1258,10 +1258,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
@@ -4820,7 +4820,7 @@
         <v>32</v>
       </c>
       <c r="B37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" t="b">
         <v>1</v>
@@ -5095,11 +5095,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B39:C1048576 B34:B36 B1:C33</xm:sqref>
+          <xm:sqref>B39:C1048576 B34:B38 B1:C33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="9" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,B34)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(TRUE,C34)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -5112,11 +5112,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C34:C37 B37</xm:sqref>
+          <xm:sqref>C34:C37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="7" operator="containsText" id="{DDDE047A-6A94-4B19-BC19-507EF1A1F811}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,B38)))</xm:f>
+            <xm:f>NOT(ISERROR(SEARCH(TRUE,C38)))</xm:f>
             <xm:f>TRUE</xm:f>
             <x14:dxf>
               <font>
@@ -5129,7 +5129,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B38:C38</xm:sqref>
+          <xm:sqref>C38</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Add code to check for duplicate trials Tidy up exp.xl
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Michael\Work\AFO - local\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C154BC24-E2E9-4451-8290-39FAA7BEEB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9B1398-CA6D-4290-BE0D-C661C0174D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30990" yWindow="2520" windowWidth="21600" windowHeight="11055" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -557,7 +557,295 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFEBAC9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -943,20 +1231,20 @@
   <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C5:C6"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.54296875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -1048,7 +1336,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1125,7 +1413,7 @@
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
     </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1180,7 +1468,7 @@
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
     </row>
-    <row r="4" spans="1:31" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -1252,7 +1540,7 @@
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>ROW(A5)-5</f>
         <v>0</v>
@@ -1375,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" ref="A6:A38" si="0">ROW(A6)-5</f>
         <v>1</v>
@@ -1483,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1591,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1699,7 +1987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1807,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1915,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2023,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2131,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2239,7 +2527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2347,7 +2635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2455,7 +2743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2563,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2671,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2779,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2887,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2995,7 +3283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3103,7 +3391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3211,7 +3499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3319,7 +3607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3427,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3535,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3643,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3751,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3859,7 +4147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3967,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4088,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4209,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4330,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4451,7 +4739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4572,7 +4860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4693,7 +4981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4814,7 +5102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4936,7 +5224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -5061,78 +5349,26 @@
   </sheetData>
   <autoFilter ref="D4:AE4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="6" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="34" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="30" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="3" priority="38" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="31" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="2" priority="39" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="32" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="1" priority="40" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:C1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="33" operator="containsText" id="{58377061-9543-45FA-9122-64515576238C}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,B1)))</xm:f>
-            <xm:f>TRUE</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>B39:C1048576 B34:B38 B1:C33</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{43D706A3-6AC5-4AC8-99C5-84B291883E8D}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,C34)))</xm:f>
-            <xm:f>TRUE</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C34:C37</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="7" operator="containsText" id="{DDDE047A-6A94-4B19-BC19-507EF1A1F811}">
-            <xm:f>NOT(ISERROR(SEARCH(TRUE,C38)))</xm:f>
-            <xm:f>TRUE</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C38</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test push of exp.xlsx
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,35 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Michael\Work\AFO - local\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9B1398-CA6D-4290-BE0D-C661C0174D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B91145-9BE2-4A49-AD82-4C3FF5A0B6A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="1875" yWindow="390" windowWidth="26835" windowHeight="15360" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$AE$4</definedName>
+    <definedName name="trial_names">Sheet1!$D:$D</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -220,14 +213,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -557,315 +550,7 @@
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1231,20 +916,20 @@
   <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.5546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -1336,7 +1021,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1098,7 @@
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
     </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1153,7 @@
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
     </row>
-    <row r="4" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -1540,13 +1225,13 @@
       <c r="AC4" s="8"/>
       <c r="AD4" s="8"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>ROW(A5)-5</f>
         <v>0</v>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1663,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ref="A6:A38" si="0">ROW(A6)-5</f>
         <v>1</v>
@@ -1771,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1879,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1987,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2095,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2203,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2311,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2419,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2527,7 +2212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2635,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2743,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2851,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2959,7 +2644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3067,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3175,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3283,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3391,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3499,7 +3184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3607,7 +3292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3715,7 +3400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3823,7 +3508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3931,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4039,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4147,7 +3832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4255,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4376,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4497,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4618,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4739,7 +4424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4860,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4981,7 +4666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -5102,13 +4787,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" t="b">
         <v>1</v>
@@ -5224,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -5233,7 +4918,7 @@
         <v>0</v>
       </c>
       <c r="C38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>62</v>
@@ -5349,21 +5034,21 @@
   </sheetData>
   <autoFilter ref="D4:AE4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="cellIs" dxfId="4" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="35" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="38" operator="containsText" text="sam">
+    <cfRule type="containsText" dxfId="3" priority="39" operator="containsText" text="sam">
       <formula>NOT(ISERROR(SEARCH("sam",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="39" operator="containsText" text="sap">
+    <cfRule type="containsText" dxfId="2" priority="40" operator="containsText" text="sap">
       <formula>NOT(ISERROR(SEARCH("sap",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="40" operator="containsText" text="saa">
+    <cfRule type="containsText" dxfId="1" priority="41" operator="containsText" text="saa">
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add equaiton system SAV
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Michael\Work\AFO - local\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9B1398-CA6D-4290-BE0D-C661C0174D5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBD78BE-6D04-48B6-A471-AA8290E821E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$AE$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$AI$4</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="70">
   <si>
     <t>sam</t>
   </si>
@@ -440,13 +440,25 @@
   </si>
   <si>
     <t>TOL 2 only</t>
+  </si>
+  <si>
+    <t>eqn_used_g0_q1p7</t>
+  </si>
+  <si>
+    <t>eqn_used_g3_q1p7</t>
+  </si>
+  <si>
+    <t>eqn_used_g2_q1p7</t>
+  </si>
+  <si>
+    <t>eqn_used_g1_q1p7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +483,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -523,7 +541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -552,320 +570,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" textRotation="90"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFEBAC9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1228,23 +941,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:AE38"/>
+  <dimension ref="A1:AI38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="17.5546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -1288,16 +1001,16 @@
         <v>43</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>0</v>
@@ -1324,19 +1037,31 @@
         <v>0</v>
       </c>
       <c r="AB1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1362,58 +1087,70 @@
         <v>46</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="U2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="V2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="AA2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
+      <c r="AB2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
     </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1428,18 +1165,10 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
       <c r="T3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1464,11 +1193,23 @@
       <c r="AA3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
+      <c r="AB3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
     </row>
-    <row r="4" spans="1:31" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -1500,47 +1241,51 @@
         <v>60</v>
       </c>
       <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7" t="s">
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="V4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="W4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="X4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7" t="s">
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="AB4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="AC4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AD4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5">
         <f>ROW(A5)-5</f>
         <v>0</v>
@@ -1598,21 +1343,21 @@
         <f t="array" ref="O5">_xlfn.IFS(OR(O1="sam",O1="sai"),1,O1="sav","-",OR(O1="sap",O1="saa"),0)</f>
         <v>-</v>
       </c>
-      <c r="P5" s="9" cm="1">
+      <c r="P5" s="9" t="str" cm="1">
         <f t="array" ref="P5">_xlfn.IFS(OR(P1="sam",P1="sai"),1,P1="sav","-",OR(P1="sap",P1="saa"),0)</f>
-        <v>1</v>
-      </c>
-      <c r="Q5" s="9" cm="1">
+        <v>-</v>
+      </c>
+      <c r="Q5" s="9" t="str" cm="1">
         <f t="array" ref="Q5">_xlfn.IFS(OR(Q1="sam",Q1="sai"),1,Q1="sav","-",OR(Q1="sap",Q1="saa"),0)</f>
-        <v>1</v>
-      </c>
-      <c r="R5" s="9" cm="1">
+        <v>-</v>
+      </c>
+      <c r="R5" s="9" t="str" cm="1">
         <f t="array" ref="R5">_xlfn.IFS(OR(R1="sam",R1="sai"),1,R1="sav","-",OR(R1="sap",R1="saa"),0)</f>
-        <v>1</v>
-      </c>
-      <c r="S5" s="9" cm="1">
+        <v>-</v>
+      </c>
+      <c r="S5" s="9" t="str" cm="1">
         <f t="array" ref="S5">_xlfn.IFS(OR(S1="sam",S1="sai"),1,S1="sav","-",OR(S1="sap",S1="saa"),0)</f>
-        <v>1</v>
+        <v>-</v>
       </c>
       <c r="T5" s="9" cm="1">
         <f t="array" ref="T5">_xlfn.IFS(OR(T1="sam",T1="sai"),1,T1="sav","-",OR(T1="sap",T1="saa"),0)</f>
@@ -1648,22 +1393,38 @@
       </c>
       <c r="AB5" s="9" cm="1">
         <f t="array" ref="AB5">_xlfn.IFS(OR(AB1="sam",AB1="sai"),1,AB1="sav","-",OR(AB1="sap",AB1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC5" s="9" cm="1">
         <f t="array" ref="AC5">_xlfn.IFS(OR(AC1="sam",AC1="sai"),1,AC1="sav","-",OR(AC1="sap",AC1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5" s="9" cm="1">
         <f t="array" ref="AD5">_xlfn.IFS(OR(AD1="sam",AD1="sai"),1,AD1="sav","-",OR(AD1="sap",AD1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE5" s="9" cm="1">
         <f t="array" ref="AE5">_xlfn.IFS(OR(AE1="sam",AE1="sai"),1,AE1="sav","-",OR(AE1="sap",AE1="saa"),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF5" s="9" cm="1">
+        <f t="array" ref="AF5">_xlfn.IFS(OR(AF1="sam",AF1="sai"),1,AF1="sav","-",OR(AF1="sap",AF1="saa"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG5" s="9" cm="1">
+        <f t="array" ref="AG5">_xlfn.IFS(OR(AG1="sam",AG1="sai"),1,AG1="sav","-",OR(AG1="sap",AG1="saa"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="9" cm="1">
+        <f t="array" ref="AH5">_xlfn.IFS(OR(AH1="sam",AH1="sai"),1,AH1="sav","-",OR(AH1="sap",AH1="saa"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="9" cm="1">
+        <f t="array" ref="AI5">_xlfn.IFS(OR(AI1="sam",AI1="sai"),1,AI1="sav","-",OR(AI1="sap",AI1="saa"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" ref="A6:A38" si="0">ROW(A6)-5</f>
         <v>1</v>
@@ -1678,7 +1439,7 @@
         <v>11</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" ref="E6:O6" si="1">E5</f>
+        <f t="shared" ref="E6:S6" si="1">E5</f>
         <v>-</v>
       </c>
       <c r="F6" t="str">
@@ -1721,21 +1482,25 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="P6">
+      <c r="P6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="Q6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="R6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="T6">
         <v>0.9</v>
       </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
       <c r="U6">
         <v>1</v>
       </c>
@@ -1767,11 +1532,23 @@
         <v>1</v>
       </c>
       <c r="AE6">
-        <f>AE5</f>
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
+        <f>AI5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1810,40 +1587,44 @@
         <v>-</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" ref="K7" si="8">K6</f>
+        <f t="shared" ref="K7:O7" si="8">K6</f>
         <v>-</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" ref="L7:N7" si="9">L6</f>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="M7" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" ref="P7:R7" si="9">P6</f>
+        <v>-</v>
+      </c>
+      <c r="Q7" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="N7" t="str">
+      <c r="R7" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="O7" t="str">
-        <f t="shared" ref="O7" si="10">O6</f>
-        <v>-</v>
-      </c>
-      <c r="P7">
+      <c r="S7" t="str">
+        <f t="shared" ref="S7" si="10">S6</f>
+        <v>-</v>
+      </c>
+      <c r="T7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7">
-        <v>1</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
       <c r="U7">
         <v>1</v>
       </c>
@@ -1875,11 +1656,23 @@
         <v>1</v>
       </c>
       <c r="AE7">
-        <f t="shared" ref="AE7:AE29" si="11">AE6</f>
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" ref="AI7:AI29" si="11">AI6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1918,43 +1711,47 @@
         <v>-</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" ref="K8" si="13">K7</f>
+        <f t="shared" ref="K8:O8" si="13">K7</f>
         <v>-</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" ref="L8:N8" si="14">L7</f>
+        <f t="shared" si="13"/>
         <v>-</v>
       </c>
       <c r="M8" t="str">
+        <f t="shared" si="13"/>
+        <v>-</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="13"/>
+        <v>-</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="13"/>
+        <v>-</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" ref="P8:R8" si="14">P7</f>
+        <v>-</v>
+      </c>
+      <c r="Q8" t="str">
         <f t="shared" si="14"/>
         <v>-</v>
       </c>
-      <c r="N8" t="str">
+      <c r="R8" t="str">
         <f t="shared" si="14"/>
         <v>-</v>
       </c>
-      <c r="O8" t="str">
-        <f t="shared" ref="O8" si="15">O7</f>
-        <v>-</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
+      <c r="S8" t="str">
+        <f t="shared" ref="S8" si="15">S7</f>
+        <v>-</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
         <v>0.9</v>
       </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
-        <v>1</v>
-      </c>
       <c r="V8">
         <v>1</v>
       </c>
@@ -1983,11 +1780,23 @@
         <v>1</v>
       </c>
       <c r="AE8">
+        <v>1</v>
+      </c>
+      <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2026,43 +1835,47 @@
         <v>-</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" ref="K9" si="17">K8</f>
+        <f t="shared" ref="K9:O9" si="17">K8</f>
         <v>-</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" ref="L9:N9" si="18">L8</f>
+        <f t="shared" si="17"/>
         <v>-</v>
       </c>
       <c r="M9" t="str">
+        <f t="shared" si="17"/>
+        <v>-</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="17"/>
+        <v>-</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="17"/>
+        <v>-</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" ref="P9:R9" si="18">P8</f>
+        <v>-</v>
+      </c>
+      <c r="Q9" t="str">
         <f t="shared" si="18"/>
         <v>-</v>
       </c>
-      <c r="N9" t="str">
+      <c r="R9" t="str">
         <f t="shared" si="18"/>
         <v>-</v>
       </c>
-      <c r="O9" t="str">
-        <f t="shared" ref="O9" si="19">O8</f>
-        <v>-</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
+      <c r="S9" t="str">
+        <f t="shared" ref="S9" si="19">S8</f>
+        <v>-</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="U9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
-        <v>1</v>
-      </c>
       <c r="V9">
         <v>1</v>
       </c>
@@ -2091,11 +1904,23 @@
         <v>1</v>
       </c>
       <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AF9">
+        <v>1</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2134,46 +1959,50 @@
         <v>-</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" ref="K10" si="21">K9</f>
+        <f t="shared" ref="K10:O10" si="21">K9</f>
         <v>-</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" ref="L10:N10" si="22">L9</f>
+        <f t="shared" si="21"/>
         <v>-</v>
       </c>
       <c r="M10" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" ref="P10:R10" si="22">P9</f>
+        <v>-</v>
+      </c>
+      <c r="Q10" t="str">
         <f t="shared" si="22"/>
         <v>-</v>
       </c>
-      <c r="N10" t="str">
+      <c r="R10" t="str">
         <f t="shared" si="22"/>
         <v>-</v>
       </c>
-      <c r="O10" t="str">
-        <f t="shared" ref="O10" si="23">O9</f>
-        <v>-</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10">
+      <c r="S10" t="str">
+        <f t="shared" ref="S10" si="23">S9</f>
+        <v>-</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
         <v>0.9</v>
       </c>
-      <c r="S10">
-        <v>1</v>
-      </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
-      <c r="U10">
-        <v>1</v>
-      </c>
-      <c r="V10">
-        <v>1</v>
-      </c>
       <c r="W10">
         <v>1</v>
       </c>
@@ -2199,11 +2028,23 @@
         <v>1</v>
       </c>
       <c r="AE10">
+        <v>1</v>
+      </c>
+      <c r="AF10">
+        <v>1</v>
+      </c>
+      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2242,46 +2083,50 @@
         <v>-</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" ref="K11" si="25">K10</f>
+        <f t="shared" ref="K11:O11" si="25">K10</f>
         <v>-</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" ref="L11:N11" si="26">L10</f>
+        <f t="shared" si="25"/>
         <v>-</v>
       </c>
       <c r="M11" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" ref="P11:R11" si="26">P10</f>
+        <v>-</v>
+      </c>
+      <c r="Q11" t="str">
         <f t="shared" si="26"/>
         <v>-</v>
       </c>
-      <c r="N11" t="str">
+      <c r="R11" t="str">
         <f t="shared" si="26"/>
         <v>-</v>
       </c>
-      <c r="O11" t="str">
-        <f t="shared" ref="O11" si="27">O10</f>
-        <v>-</v>
-      </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-      <c r="R11">
+      <c r="S11" t="str">
+        <f t="shared" ref="S11" si="27">S10</f>
+        <v>-</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S11">
-        <v>1</v>
-      </c>
-      <c r="T11">
-        <v>1</v>
-      </c>
-      <c r="U11">
-        <v>1</v>
-      </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
       <c r="W11">
         <v>1</v>
       </c>
@@ -2307,11 +2152,23 @@
         <v>1</v>
       </c>
       <c r="AE11">
+        <v>1</v>
+      </c>
+      <c r="AF11">
+        <v>1</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AI11">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2350,49 +2207,53 @@
         <v>-</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" ref="K12" si="29">K11</f>
+        <f t="shared" ref="K12:O12" si="29">K11</f>
         <v>-</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" ref="L12:N12" si="30">L11</f>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="M12" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" ref="P12:R12" si="30">P11</f>
+        <v>-</v>
+      </c>
+      <c r="Q12" t="str">
         <f t="shared" si="30"/>
         <v>-</v>
       </c>
-      <c r="N12" t="str">
+      <c r="R12" t="str">
         <f t="shared" si="30"/>
         <v>-</v>
       </c>
-      <c r="O12" t="str">
-        <f t="shared" ref="O12" si="31">O11</f>
-        <v>-</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-      <c r="S12">
+      <c r="S12" t="str">
+        <f t="shared" ref="S12" si="31">S11</f>
+        <v>-</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
         <v>0.9</v>
       </c>
-      <c r="T12">
-        <v>1</v>
-      </c>
-      <c r="U12">
-        <v>1</v>
-      </c>
-      <c r="V12">
-        <v>1</v>
-      </c>
-      <c r="W12">
-        <v>1</v>
-      </c>
       <c r="X12">
         <v>1</v>
       </c>
@@ -2415,11 +2276,23 @@
         <v>1</v>
       </c>
       <c r="AE12">
+        <v>1</v>
+      </c>
+      <c r="AF12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>1</v>
+      </c>
+      <c r="AH12">
+        <v>1</v>
+      </c>
+      <c r="AI12">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2458,49 +2331,53 @@
         <v>-</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" ref="K13" si="33">K12</f>
+        <f t="shared" ref="K13:O13" si="33">K12</f>
         <v>-</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" ref="L13:N13" si="34">L12</f>
+        <f t="shared" si="33"/>
         <v>-</v>
       </c>
       <c r="M13" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" ref="P13:R13" si="34">P12</f>
+        <v>-</v>
+      </c>
+      <c r="Q13" t="str">
         <f t="shared" si="34"/>
         <v>-</v>
       </c>
-      <c r="N13" t="str">
+      <c r="R13" t="str">
         <f t="shared" si="34"/>
         <v>-</v>
       </c>
-      <c r="O13" t="str">
-        <f t="shared" ref="O13" si="35">O12</f>
-        <v>-</v>
-      </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-      <c r="S13">
+      <c r="S13" t="str">
+        <f t="shared" ref="S13" si="35">S12</f>
+        <v>-</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="T13">
-        <v>1</v>
-      </c>
-      <c r="U13">
-        <v>1</v>
-      </c>
-      <c r="V13">
-        <v>1</v>
-      </c>
-      <c r="W13">
-        <v>1</v>
-      </c>
       <c r="X13">
         <v>1</v>
       </c>
@@ -2523,11 +2400,23 @@
         <v>1</v>
       </c>
       <c r="AE13">
+        <v>1</v>
+      </c>
+      <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AG13">
+        <v>1</v>
+      </c>
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AI13">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2566,52 +2455,56 @@
         <v>-</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" ref="K14" si="37">K13</f>
+        <f t="shared" ref="K14:O14" si="37">K13</f>
         <v>-</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" ref="L14:N14" si="38">L13</f>
+        <f t="shared" si="37"/>
         <v>-</v>
       </c>
       <c r="M14" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" ref="P14:R14" si="38">P13</f>
+        <v>-</v>
+      </c>
+      <c r="Q14" t="str">
         <f t="shared" si="38"/>
         <v>-</v>
       </c>
-      <c r="N14" t="str">
+      <c r="R14" t="str">
         <f t="shared" si="38"/>
         <v>-</v>
       </c>
-      <c r="O14" t="str">
-        <f t="shared" ref="O14" si="39">O13</f>
-        <v>-</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-      <c r="S14">
-        <v>1</v>
+      <c r="S14" t="str">
+        <f t="shared" ref="S14" si="39">S13</f>
+        <v>-</v>
       </c>
       <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
         <v>0.9</v>
       </c>
-      <c r="U14">
-        <v>1</v>
-      </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
-      <c r="W14">
-        <v>1</v>
-      </c>
-      <c r="X14">
-        <v>1</v>
-      </c>
       <c r="Y14">
         <v>1</v>
       </c>
@@ -2631,11 +2524,23 @@
         <v>1</v>
       </c>
       <c r="AE14">
+        <v>1</v>
+      </c>
+      <c r="AF14">
+        <v>1</v>
+      </c>
+      <c r="AG14">
+        <v>1</v>
+      </c>
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AI14">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2674,52 +2579,56 @@
         <v>-</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" ref="K15" si="41">K14</f>
+        <f t="shared" ref="K15:O15" si="41">K14</f>
         <v>-</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" ref="L15:N15" si="42">L14</f>
+        <f t="shared" si="41"/>
         <v>-</v>
       </c>
       <c r="M15" t="str">
+        <f t="shared" si="41"/>
+        <v>-</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="41"/>
+        <v>-</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="41"/>
+        <v>-</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" ref="P15:R15" si="42">P14</f>
+        <v>-</v>
+      </c>
+      <c r="Q15" t="str">
         <f t="shared" si="42"/>
         <v>-</v>
       </c>
-      <c r="N15" t="str">
+      <c r="R15" t="str">
         <f t="shared" si="42"/>
         <v>-</v>
       </c>
-      <c r="O15" t="str">
-        <f t="shared" ref="O15" si="43">O14</f>
-        <v>-</v>
-      </c>
-      <c r="P15">
-        <v>1</v>
-      </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15">
-        <v>1</v>
+      <c r="S15" t="str">
+        <f t="shared" ref="S15" si="43">S14</f>
+        <v>-</v>
       </c>
       <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="U15">
-        <v>1</v>
-      </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
-      <c r="W15">
-        <v>1</v>
-      </c>
-      <c r="X15">
-        <v>1</v>
-      </c>
       <c r="Y15">
         <v>1</v>
       </c>
@@ -2739,11 +2648,23 @@
         <v>1</v>
       </c>
       <c r="AE15">
+        <v>1</v>
+      </c>
+      <c r="AF15">
+        <v>1</v>
+      </c>
+      <c r="AG15">
+        <v>1</v>
+      </c>
+      <c r="AH15">
+        <v>1</v>
+      </c>
+      <c r="AI15">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2782,55 +2703,59 @@
         <v>-</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" ref="K16" si="45">K15</f>
+        <f t="shared" ref="K16:O16" si="45">K15</f>
         <v>-</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" ref="L16:N16" si="46">L15</f>
+        <f t="shared" si="45"/>
         <v>-</v>
       </c>
       <c r="M16" t="str">
+        <f t="shared" si="45"/>
+        <v>-</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" si="45"/>
+        <v>-</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="45"/>
+        <v>-</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" ref="P16:R16" si="46">P15</f>
+        <v>-</v>
+      </c>
+      <c r="Q16" t="str">
         <f t="shared" si="46"/>
         <v>-</v>
       </c>
-      <c r="N16" t="str">
+      <c r="R16" t="str">
         <f t="shared" si="46"/>
         <v>-</v>
       </c>
-      <c r="O16" t="str">
-        <f t="shared" ref="O16" si="47">O15</f>
-        <v>-</v>
-      </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-      <c r="S16">
-        <v>1</v>
+      <c r="S16" t="str">
+        <f t="shared" ref="S16" si="47">S15</f>
+        <v>-</v>
       </c>
       <c r="T16">
         <v>1</v>
       </c>
       <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
         <v>0.9</v>
       </c>
-      <c r="V16">
-        <v>1</v>
-      </c>
-      <c r="W16">
-        <v>1</v>
-      </c>
-      <c r="X16">
-        <v>1</v>
-      </c>
-      <c r="Y16">
-        <v>1</v>
-      </c>
       <c r="Z16">
         <v>1</v>
       </c>
@@ -2847,11 +2772,23 @@
         <v>1</v>
       </c>
       <c r="AE16">
+        <v>1</v>
+      </c>
+      <c r="AF16">
+        <v>1</v>
+      </c>
+      <c r="AG16">
+        <v>1</v>
+      </c>
+      <c r="AH16">
+        <v>1</v>
+      </c>
+      <c r="AI16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2890,55 +2827,59 @@
         <v>-</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" ref="K17" si="49">K16</f>
+        <f t="shared" ref="K17:O17" si="49">K16</f>
         <v>-</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" ref="L17:N17" si="50">L16</f>
+        <f t="shared" si="49"/>
         <v>-</v>
       </c>
       <c r="M17" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="49"/>
+        <v>-</v>
+      </c>
+      <c r="P17" t="str">
+        <f t="shared" ref="P17:R17" si="50">P16</f>
+        <v>-</v>
+      </c>
+      <c r="Q17" t="str">
         <f t="shared" si="50"/>
         <v>-</v>
       </c>
-      <c r="N17" t="str">
+      <c r="R17" t="str">
         <f t="shared" si="50"/>
         <v>-</v>
       </c>
-      <c r="O17" t="str">
-        <f t="shared" ref="O17" si="51">O16</f>
-        <v>-</v>
-      </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
-      <c r="S17">
-        <v>1</v>
+      <c r="S17" t="str">
+        <f t="shared" ref="S17" si="51">S16</f>
+        <v>-</v>
       </c>
       <c r="T17">
         <v>1</v>
       </c>
       <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>1</v>
+      </c>
+      <c r="Y17">
         <v>1.1000000000000001</v>
       </c>
-      <c r="V17">
-        <v>1</v>
-      </c>
-      <c r="W17">
-        <v>1</v>
-      </c>
-      <c r="X17">
-        <v>1</v>
-      </c>
-      <c r="Y17">
-        <v>1</v>
-      </c>
       <c r="Z17">
         <v>1</v>
       </c>
@@ -2955,11 +2896,23 @@
         <v>1</v>
       </c>
       <c r="AE17">
+        <v>1</v>
+      </c>
+      <c r="AF17">
+        <v>1</v>
+      </c>
+      <c r="AG17">
+        <v>1</v>
+      </c>
+      <c r="AH17">
+        <v>1</v>
+      </c>
+      <c r="AI17">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2998,36 +2951,40 @@
         <v>-</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" ref="K18" si="53">K17</f>
+        <f t="shared" ref="K18:O18" si="53">K17</f>
         <v>-</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" ref="L18:N18" si="54">L17</f>
+        <f t="shared" si="53"/>
         <v>-</v>
       </c>
       <c r="M18" t="str">
+        <f t="shared" si="53"/>
+        <v>-</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" si="53"/>
+        <v>-</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="53"/>
+        <v>-</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" ref="P18:R18" si="54">P17</f>
+        <v>-</v>
+      </c>
+      <c r="Q18" t="str">
         <f t="shared" si="54"/>
         <v>-</v>
       </c>
-      <c r="N18" t="str">
+      <c r="R18" t="str">
         <f t="shared" si="54"/>
         <v>-</v>
       </c>
-      <c r="O18" t="str">
-        <f t="shared" ref="O18" si="55">O17</f>
-        <v>-</v>
-      </c>
-      <c r="P18">
-        <v>1</v>
-      </c>
-      <c r="Q18">
-        <v>1</v>
-      </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-      <c r="S18">
-        <v>1</v>
+      <c r="S18" t="str">
+        <f t="shared" ref="S18" si="55">S17</f>
+        <v>-</v>
       </c>
       <c r="T18">
         <v>1</v>
@@ -3036,20 +2993,20 @@
         <v>1</v>
       </c>
       <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
         <v>0.9</v>
       </c>
-      <c r="W18">
-        <v>1</v>
-      </c>
-      <c r="X18">
-        <v>1</v>
-      </c>
-      <c r="Y18">
-        <v>1</v>
-      </c>
-      <c r="Z18">
-        <v>1</v>
-      </c>
       <c r="AA18">
         <v>1</v>
       </c>
@@ -3063,11 +3020,23 @@
         <v>1</v>
       </c>
       <c r="AE18">
+        <v>1</v>
+      </c>
+      <c r="AF18">
+        <v>1</v>
+      </c>
+      <c r="AG18">
+        <v>1</v>
+      </c>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+      <c r="AI18">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3106,36 +3075,40 @@
         <v>-</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" ref="K19" si="57">K18</f>
+        <f t="shared" ref="K19:O19" si="57">K18</f>
         <v>-</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" ref="L19:N19" si="58">L18</f>
+        <f t="shared" si="57"/>
         <v>-</v>
       </c>
       <c r="M19" t="str">
+        <f t="shared" si="57"/>
+        <v>-</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" si="57"/>
+        <v>-</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="57"/>
+        <v>-</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" ref="P19:R19" si="58">P18</f>
+        <v>-</v>
+      </c>
+      <c r="Q19" t="str">
         <f t="shared" si="58"/>
         <v>-</v>
       </c>
-      <c r="N19" t="str">
+      <c r="R19" t="str">
         <f t="shared" si="58"/>
         <v>-</v>
       </c>
-      <c r="O19" t="str">
-        <f t="shared" ref="O19" si="59">O18</f>
-        <v>-</v>
-      </c>
-      <c r="P19">
-        <v>1</v>
-      </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
+      <c r="S19" t="str">
+        <f t="shared" ref="S19" si="59">S18</f>
+        <v>-</v>
       </c>
       <c r="T19">
         <v>1</v>
@@ -3144,20 +3117,20 @@
         <v>1</v>
       </c>
       <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="W19">
-        <v>1</v>
-      </c>
-      <c r="X19">
-        <v>1</v>
-      </c>
-      <c r="Y19">
-        <v>1</v>
-      </c>
-      <c r="Z19">
-        <v>1</v>
-      </c>
       <c r="AA19">
         <v>1</v>
       </c>
@@ -3171,11 +3144,23 @@
         <v>1</v>
       </c>
       <c r="AE19">
+        <v>1</v>
+      </c>
+      <c r="AF19">
+        <v>1</v>
+      </c>
+      <c r="AG19">
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <v>1</v>
+      </c>
+      <c r="AI19">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3214,36 +3199,40 @@
         <v>-</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" ref="K20" si="61">K19</f>
+        <f t="shared" ref="K20:O20" si="61">K19</f>
         <v>-</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" ref="L20:N20" si="62">L19</f>
+        <f t="shared" si="61"/>
         <v>-</v>
       </c>
       <c r="M20" t="str">
+        <f t="shared" si="61"/>
+        <v>-</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" si="61"/>
+        <v>-</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="61"/>
+        <v>-</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" ref="P20:R20" si="62">P19</f>
+        <v>-</v>
+      </c>
+      <c r="Q20" t="str">
         <f t="shared" si="62"/>
         <v>-</v>
       </c>
-      <c r="N20" t="str">
+      <c r="R20" t="str">
         <f t="shared" si="62"/>
         <v>-</v>
       </c>
-      <c r="O20" t="str">
-        <f t="shared" ref="O20" si="63">O19</f>
-        <v>-</v>
-      </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-      <c r="R20">
-        <v>1</v>
-      </c>
-      <c r="S20">
-        <v>1</v>
+      <c r="S20" t="str">
+        <f t="shared" ref="S20" si="63">S19</f>
+        <v>-</v>
       </c>
       <c r="T20">
         <v>1</v>
@@ -3255,20 +3244,20 @@
         <v>1</v>
       </c>
       <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
         <v>0.9</v>
       </c>
-      <c r="X20">
-        <v>1</v>
-      </c>
-      <c r="Y20">
-        <v>1</v>
-      </c>
-      <c r="Z20">
-        <v>1</v>
-      </c>
-      <c r="AA20">
-        <v>1</v>
-      </c>
       <c r="AB20">
         <v>1</v>
       </c>
@@ -3279,11 +3268,23 @@
         <v>1</v>
       </c>
       <c r="AE20">
+        <v>1</v>
+      </c>
+      <c r="AF20">
+        <v>1</v>
+      </c>
+      <c r="AG20">
+        <v>1</v>
+      </c>
+      <c r="AH20">
+        <v>1</v>
+      </c>
+      <c r="AI20">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3322,36 +3323,40 @@
         <v>-</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" ref="K21" si="65">K20</f>
+        <f t="shared" ref="K21:O21" si="65">K20</f>
         <v>-</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" ref="L21:N21" si="66">L20</f>
+        <f t="shared" si="65"/>
         <v>-</v>
       </c>
       <c r="M21" t="str">
+        <f t="shared" si="65"/>
+        <v>-</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" si="65"/>
+        <v>-</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="65"/>
+        <v>-</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" ref="P21:R21" si="66">P20</f>
+        <v>-</v>
+      </c>
+      <c r="Q21" t="str">
         <f t="shared" si="66"/>
         <v>-</v>
       </c>
-      <c r="N21" t="str">
+      <c r="R21" t="str">
         <f t="shared" si="66"/>
         <v>-</v>
       </c>
-      <c r="O21" t="str">
-        <f t="shared" ref="O21" si="67">O20</f>
-        <v>-</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
+      <c r="S21" t="str">
+        <f t="shared" ref="S21" si="67">S20</f>
+        <v>-</v>
       </c>
       <c r="T21">
         <v>1</v>
@@ -3363,20 +3368,20 @@
         <v>1</v>
       </c>
       <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
         <v>1.1000000000000001</v>
       </c>
-      <c r="X21">
-        <v>1</v>
-      </c>
-      <c r="Y21">
-        <v>1</v>
-      </c>
-      <c r="Z21">
-        <v>1</v>
-      </c>
-      <c r="AA21">
-        <v>1</v>
-      </c>
       <c r="AB21">
         <v>1</v>
       </c>
@@ -3387,11 +3392,23 @@
         <v>1</v>
       </c>
       <c r="AE21">
+        <v>1</v>
+      </c>
+      <c r="AF21">
+        <v>1</v>
+      </c>
+      <c r="AG21">
+        <v>1</v>
+      </c>
+      <c r="AH21">
+        <v>1</v>
+      </c>
+      <c r="AI21">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3430,36 +3447,40 @@
         <v>-</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" ref="K22" si="69">K21</f>
+        <f t="shared" ref="K22:O22" si="69">K21</f>
         <v>-</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" ref="L22:N22" si="70">L21</f>
+        <f t="shared" si="69"/>
         <v>-</v>
       </c>
       <c r="M22" t="str">
+        <f t="shared" si="69"/>
+        <v>-</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" si="69"/>
+        <v>-</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="69"/>
+        <v>-</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" ref="P22:R22" si="70">P21</f>
+        <v>-</v>
+      </c>
+      <c r="Q22" t="str">
         <f t="shared" si="70"/>
         <v>-</v>
       </c>
-      <c r="N22" t="str">
+      <c r="R22" t="str">
         <f t="shared" si="70"/>
         <v>-</v>
       </c>
-      <c r="O22" t="str">
-        <f t="shared" ref="O22" si="71">O21</f>
-        <v>-</v>
-      </c>
-      <c r="P22">
-        <v>1</v>
-      </c>
-      <c r="Q22">
-        <v>1</v>
-      </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-      <c r="S22">
-        <v>1</v>
+      <c r="S22" t="str">
+        <f t="shared" ref="S22" si="71">S21</f>
+        <v>-</v>
       </c>
       <c r="T22">
         <v>1</v>
@@ -3474,20 +3495,20 @@
         <v>1</v>
       </c>
       <c r="X22">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
         <v>0.9</v>
       </c>
-      <c r="Y22">
-        <v>1</v>
-      </c>
-      <c r="Z22">
-        <v>1</v>
-      </c>
-      <c r="AA22">
-        <v>1</v>
-      </c>
-      <c r="AB22">
-        <v>1</v>
-      </c>
       <c r="AC22">
         <v>1</v>
       </c>
@@ -3495,11 +3516,23 @@
         <v>1</v>
       </c>
       <c r="AE22">
+        <v>1</v>
+      </c>
+      <c r="AF22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>1</v>
+      </c>
+      <c r="AH22">
+        <v>1</v>
+      </c>
+      <c r="AI22">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3538,36 +3571,40 @@
         <v>-</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" ref="K23" si="73">K22</f>
+        <f t="shared" ref="K23:O23" si="73">K22</f>
         <v>-</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" ref="L23:N23" si="74">L22</f>
+        <f t="shared" si="73"/>
         <v>-</v>
       </c>
       <c r="M23" t="str">
+        <f t="shared" si="73"/>
+        <v>-</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" si="73"/>
+        <v>-</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="73"/>
+        <v>-</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" ref="P23:R23" si="74">P22</f>
+        <v>-</v>
+      </c>
+      <c r="Q23" t="str">
         <f t="shared" si="74"/>
         <v>-</v>
       </c>
-      <c r="N23" t="str">
+      <c r="R23" t="str">
         <f t="shared" si="74"/>
         <v>-</v>
       </c>
-      <c r="O23" t="str">
-        <f t="shared" ref="O23" si="75">O22</f>
-        <v>-</v>
-      </c>
-      <c r="P23">
-        <v>1</v>
-      </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-      <c r="S23">
-        <v>1</v>
+      <c r="S23" t="str">
+        <f t="shared" ref="S23" si="75">S22</f>
+        <v>-</v>
       </c>
       <c r="T23">
         <v>1</v>
@@ -3582,20 +3619,20 @@
         <v>1</v>
       </c>
       <c r="X23">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+      <c r="AA23">
+        <v>1</v>
+      </c>
+      <c r="AB23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Y23">
-        <v>1</v>
-      </c>
-      <c r="Z23">
-        <v>1</v>
-      </c>
-      <c r="AA23">
-        <v>1</v>
-      </c>
-      <c r="AB23">
-        <v>1</v>
-      </c>
       <c r="AC23">
         <v>1</v>
       </c>
@@ -3603,11 +3640,23 @@
         <v>1</v>
       </c>
       <c r="AE23">
+        <v>1</v>
+      </c>
+      <c r="AF23">
+        <v>1</v>
+      </c>
+      <c r="AG23">
+        <v>1</v>
+      </c>
+      <c r="AH23">
+        <v>1</v>
+      </c>
+      <c r="AI23">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3646,36 +3695,40 @@
         <v>-</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" ref="K24" si="77">K23</f>
+        <f t="shared" ref="K24:O24" si="77">K23</f>
         <v>-</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" ref="L24:N24" si="78">L23</f>
+        <f t="shared" si="77"/>
         <v>-</v>
       </c>
       <c r="M24" t="str">
+        <f t="shared" si="77"/>
+        <v>-</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" si="77"/>
+        <v>-</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="77"/>
+        <v>-</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" ref="P24:R24" si="78">P23</f>
+        <v>-</v>
+      </c>
+      <c r="Q24" t="str">
         <f t="shared" si="78"/>
         <v>-</v>
       </c>
-      <c r="N24" t="str">
+      <c r="R24" t="str">
         <f t="shared" si="78"/>
         <v>-</v>
       </c>
-      <c r="O24" t="str">
-        <f t="shared" ref="O24" si="79">O23</f>
-        <v>-</v>
-      </c>
-      <c r="P24">
-        <v>1</v>
-      </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="R24">
-        <v>1</v>
-      </c>
-      <c r="S24">
-        <v>1</v>
+      <c r="S24" t="str">
+        <f t="shared" ref="S24" si="79">S23</f>
+        <v>-</v>
       </c>
       <c r="T24">
         <v>1</v>
@@ -3693,29 +3746,41 @@
         <v>1</v>
       </c>
       <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+      <c r="AA24">
+        <v>1</v>
+      </c>
+      <c r="AB24">
+        <v>1</v>
+      </c>
+      <c r="AC24">
         <v>0.9</v>
       </c>
-      <c r="Z24">
-        <v>1</v>
-      </c>
-      <c r="AA24">
-        <v>1</v>
-      </c>
-      <c r="AB24">
-        <v>1</v>
-      </c>
-      <c r="AC24">
-        <v>1</v>
-      </c>
       <c r="AD24">
         <v>1</v>
       </c>
       <c r="AE24">
+        <v>1</v>
+      </c>
+      <c r="AF24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>1</v>
+      </c>
+      <c r="AH24">
+        <v>1</v>
+      </c>
+      <c r="AI24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3754,36 +3819,40 @@
         <v>-</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" ref="K25" si="81">K24</f>
+        <f t="shared" ref="K25:O25" si="81">K24</f>
         <v>-</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" ref="L25:N25" si="82">L24</f>
+        <f t="shared" si="81"/>
         <v>-</v>
       </c>
       <c r="M25" t="str">
+        <f t="shared" si="81"/>
+        <v>-</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="81"/>
+        <v>-</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="81"/>
+        <v>-</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" ref="P25:R25" si="82">P24</f>
+        <v>-</v>
+      </c>
+      <c r="Q25" t="str">
         <f t="shared" si="82"/>
         <v>-</v>
       </c>
-      <c r="N25" t="str">
+      <c r="R25" t="str">
         <f t="shared" si="82"/>
         <v>-</v>
       </c>
-      <c r="O25" t="str">
-        <f t="shared" ref="O25" si="83">O24</f>
-        <v>-</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="R25">
-        <v>1</v>
-      </c>
-      <c r="S25">
-        <v>1</v>
+      <c r="S25" t="str">
+        <f t="shared" ref="S25" si="83">S24</f>
+        <v>-</v>
       </c>
       <c r="T25">
         <v>1</v>
@@ -3801,29 +3870,41 @@
         <v>1</v>
       </c>
       <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+      <c r="AA25">
+        <v>1</v>
+      </c>
+      <c r="AB25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Z25">
-        <v>1</v>
-      </c>
-      <c r="AA25">
-        <v>1</v>
-      </c>
-      <c r="AB25">
-        <v>1</v>
-      </c>
-      <c r="AC25">
-        <v>1</v>
-      </c>
       <c r="AD25">
         <v>1</v>
       </c>
       <c r="AE25">
+        <v>1</v>
+      </c>
+      <c r="AF25">
+        <v>1</v>
+      </c>
+      <c r="AG25">
+        <v>1</v>
+      </c>
+      <c r="AH25">
+        <v>1</v>
+      </c>
+      <c r="AI25">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3862,36 +3943,40 @@
         <v>-</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" ref="K26" si="85">K25</f>
+        <f t="shared" ref="K26:O26" si="85">K25</f>
         <v>-</v>
       </c>
       <c r="L26" t="str">
-        <f t="shared" ref="L26:N26" si="86">L25</f>
+        <f t="shared" si="85"/>
         <v>-</v>
       </c>
       <c r="M26" t="str">
+        <f t="shared" si="85"/>
+        <v>-</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" si="85"/>
+        <v>-</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="85"/>
+        <v>-</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" ref="P26:R26" si="86">P25</f>
+        <v>-</v>
+      </c>
+      <c r="Q26" t="str">
         <f t="shared" si="86"/>
         <v>-</v>
       </c>
-      <c r="N26" t="str">
+      <c r="R26" t="str">
         <f t="shared" si="86"/>
         <v>-</v>
       </c>
-      <c r="O26" t="str">
-        <f t="shared" ref="O26" si="87">O25</f>
-        <v>-</v>
-      </c>
-      <c r="P26">
-        <v>1</v>
-      </c>
-      <c r="Q26">
-        <v>1</v>
-      </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-      <c r="S26">
-        <v>1</v>
+      <c r="S26" t="str">
+        <f t="shared" ref="S26" si="87">S25</f>
+        <v>-</v>
       </c>
       <c r="T26">
         <v>1</v>
@@ -3912,26 +3997,38 @@
         <v>1</v>
       </c>
       <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+      <c r="AB26">
+        <v>1</v>
+      </c>
+      <c r="AC26">
+        <v>1</v>
+      </c>
+      <c r="AD26">
         <v>0.9</v>
       </c>
-      <c r="AA26">
-        <v>1</v>
-      </c>
-      <c r="AB26">
-        <v>1</v>
-      </c>
-      <c r="AC26">
-        <v>1</v>
-      </c>
-      <c r="AD26">
-        <v>1</v>
-      </c>
       <c r="AE26">
+        <v>1</v>
+      </c>
+      <c r="AF26">
+        <v>1</v>
+      </c>
+      <c r="AG26">
+        <v>1</v>
+      </c>
+      <c r="AH26">
+        <v>1</v>
+      </c>
+      <c r="AI26">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3970,36 +4067,40 @@
         <v>-</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" ref="K27" si="89">K26</f>
+        <f t="shared" ref="K27:O27" si="89">K26</f>
         <v>-</v>
       </c>
       <c r="L27" t="str">
-        <f t="shared" ref="L27:N27" si="90">L26</f>
+        <f t="shared" si="89"/>
         <v>-</v>
       </c>
       <c r="M27" t="str">
+        <f t="shared" si="89"/>
+        <v>-</v>
+      </c>
+      <c r="N27" t="str">
+        <f t="shared" si="89"/>
+        <v>-</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="89"/>
+        <v>-</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" ref="P27:R27" si="90">P26</f>
+        <v>-</v>
+      </c>
+      <c r="Q27" t="str">
         <f t="shared" si="90"/>
         <v>-</v>
       </c>
-      <c r="N27" t="str">
+      <c r="R27" t="str">
         <f t="shared" si="90"/>
         <v>-</v>
       </c>
-      <c r="O27" t="str">
-        <f t="shared" ref="O27" si="91">O26</f>
-        <v>-</v>
-      </c>
-      <c r="P27">
-        <v>1</v>
-      </c>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-      <c r="R27">
-        <v>1</v>
-      </c>
-      <c r="S27">
-        <v>1</v>
+      <c r="S27" t="str">
+        <f t="shared" ref="S27" si="91">S26</f>
+        <v>-</v>
       </c>
       <c r="T27">
         <v>1</v>
@@ -4020,26 +4121,38 @@
         <v>1</v>
       </c>
       <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AB27">
+        <v>1</v>
+      </c>
+      <c r="AC27">
+        <v>1</v>
+      </c>
+      <c r="AD27">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AA27">
-        <v>1</v>
-      </c>
-      <c r="AB27">
-        <v>1</v>
-      </c>
-      <c r="AC27">
-        <v>1</v>
-      </c>
-      <c r="AD27">
-        <v>1</v>
-      </c>
       <c r="AE27">
+        <v>1</v>
+      </c>
+      <c r="AF27">
+        <v>1</v>
+      </c>
+      <c r="AG27">
+        <v>1</v>
+      </c>
+      <c r="AH27">
+        <v>1</v>
+      </c>
+      <c r="AI27">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4078,36 +4191,40 @@
         <v>-</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" ref="K28" si="93">K27</f>
+        <f t="shared" ref="K28:O28" si="93">K27</f>
         <v>-</v>
       </c>
       <c r="L28" t="str">
-        <f t="shared" ref="L28:N28" si="94">L27</f>
+        <f t="shared" si="93"/>
         <v>-</v>
       </c>
       <c r="M28" t="str">
+        <f t="shared" si="93"/>
+        <v>-</v>
+      </c>
+      <c r="N28" t="str">
+        <f t="shared" si="93"/>
+        <v>-</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="93"/>
+        <v>-</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" ref="P28:R28" si="94">P27</f>
+        <v>-</v>
+      </c>
+      <c r="Q28" t="str">
         <f t="shared" si="94"/>
         <v>-</v>
       </c>
-      <c r="N28" t="str">
+      <c r="R28" t="str">
         <f t="shared" si="94"/>
         <v>-</v>
       </c>
-      <c r="O28" t="str">
-        <f t="shared" ref="O28" si="95">O27</f>
-        <v>-</v>
-      </c>
-      <c r="P28">
-        <v>1</v>
-      </c>
-      <c r="Q28">
-        <v>1</v>
-      </c>
-      <c r="R28">
-        <v>1</v>
-      </c>
-      <c r="S28">
-        <v>1</v>
+      <c r="S28" t="str">
+        <f t="shared" ref="S28" si="95">S27</f>
+        <v>-</v>
       </c>
       <c r="T28">
         <v>1</v>
@@ -4131,23 +4248,35 @@
         <v>1</v>
       </c>
       <c r="AA28">
+        <v>1</v>
+      </c>
+      <c r="AB28">
+        <v>1</v>
+      </c>
+      <c r="AC28">
+        <v>1</v>
+      </c>
+      <c r="AD28">
+        <v>1</v>
+      </c>
+      <c r="AE28">
         <v>0.9</v>
       </c>
-      <c r="AB28">
-        <v>1</v>
-      </c>
-      <c r="AC28">
-        <v>1</v>
-      </c>
-      <c r="AD28">
-        <v>1</v>
-      </c>
-      <c r="AE28">
+      <c r="AF28">
+        <v>1</v>
+      </c>
+      <c r="AG28">
+        <v>1</v>
+      </c>
+      <c r="AH28">
+        <v>1</v>
+      </c>
+      <c r="AI28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4186,36 +4315,40 @@
         <v>-</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" ref="K29" si="97">K28</f>
+        <f t="shared" ref="K29:O29" si="97">K28</f>
         <v>-</v>
       </c>
       <c r="L29" t="str">
-        <f t="shared" ref="L29:N29" si="98">L28</f>
+        <f t="shared" si="97"/>
         <v>-</v>
       </c>
       <c r="M29" t="str">
+        <f t="shared" si="97"/>
+        <v>-</v>
+      </c>
+      <c r="N29" t="str">
+        <f t="shared" si="97"/>
+        <v>-</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="97"/>
+        <v>-</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" ref="P29:R29" si="98">P28</f>
+        <v>-</v>
+      </c>
+      <c r="Q29" t="str">
         <f t="shared" si="98"/>
         <v>-</v>
       </c>
-      <c r="N29" t="str">
+      <c r="R29" t="str">
         <f t="shared" si="98"/>
         <v>-</v>
       </c>
-      <c r="O29" t="str">
-        <f t="shared" ref="O29:O33" si="99">O28</f>
-        <v>-</v>
-      </c>
-      <c r="P29">
-        <v>1</v>
-      </c>
-      <c r="Q29">
-        <v>1</v>
-      </c>
-      <c r="R29">
-        <v>1</v>
-      </c>
-      <c r="S29">
-        <v>1</v>
+      <c r="S29" t="str">
+        <f t="shared" ref="S29:S33" si="99">S28</f>
+        <v>-</v>
       </c>
       <c r="T29">
         <v>1</v>
@@ -4239,23 +4372,35 @@
         <v>1</v>
       </c>
       <c r="AA29">
+        <v>1</v>
+      </c>
+      <c r="AB29">
+        <v>1</v>
+      </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
+      <c r="AD29">
+        <v>1</v>
+      </c>
+      <c r="AE29">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AB29">
-        <v>1</v>
-      </c>
-      <c r="AC29">
-        <v>1</v>
-      </c>
-      <c r="AD29">
-        <v>1</v>
-      </c>
-      <c r="AE29">
+      <c r="AF29">
+        <v>1</v>
+      </c>
+      <c r="AG29">
+        <v>1</v>
+      </c>
+      <c r="AH29">
+        <v>1</v>
+      </c>
+      <c r="AI29">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4274,7 +4419,7 @@
         <v>-</v>
       </c>
       <c r="F30" t="str">
-        <f t="shared" ref="E30:AE38" si="100">F$5</f>
+        <f t="shared" ref="E30:AI38" si="100">F$5</f>
         <v>-</v>
       </c>
       <c r="G30" t="str">
@@ -4298,35 +4443,35 @@
         <v>-</v>
       </c>
       <c r="L30" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="M30">
+        <f t="shared" ref="L30:O30" si="101">L29</f>
+        <v>-</v>
+      </c>
+      <c r="M30" t="str">
+        <f t="shared" si="101"/>
+        <v>-</v>
+      </c>
+      <c r="N30" t="str">
+        <f t="shared" si="101"/>
+        <v>-</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="101"/>
+        <v>-</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="Q30">
         <v>200</v>
       </c>
-      <c r="N30" t="b">
-        <v>1</v>
-      </c>
-      <c r="O30" t="str">
+      <c r="R30" t="b">
+        <v>1</v>
+      </c>
+      <c r="S30" t="str">
         <f t="shared" si="99"/>
         <v>-</v>
       </c>
-      <c r="P30">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R30">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
       <c r="T30">
         <f t="shared" si="100"/>
         <v>1</v>
@@ -4361,22 +4506,38 @@
       </c>
       <c r="AB30">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC30">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD30">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE30">
         <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AF30">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AG30">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AH30">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AI30">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4391,7 +4552,7 @@
         <v>55</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" ref="E31:E33" si="101">E$5</f>
+        <f t="shared" ref="E31:E33" si="102">E$5</f>
         <v>-</v>
       </c>
       <c r="F31" t="str">
@@ -4419,35 +4580,35 @@
         <v>-</v>
       </c>
       <c r="L31" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="M31">
+        <f t="shared" ref="L31:O31" si="103">L30</f>
+        <v>-</v>
+      </c>
+      <c r="M31" t="str">
+        <f t="shared" si="103"/>
+        <v>-</v>
+      </c>
+      <c r="N31" t="str">
+        <f t="shared" si="103"/>
+        <v>-</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="103"/>
+        <v>-</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="Q31">
         <v>800</v>
       </c>
-      <c r="N31" t="b">
-        <v>1</v>
-      </c>
-      <c r="O31" t="str">
+      <c r="R31" t="b">
+        <v>1</v>
+      </c>
+      <c r="S31" t="str">
         <f t="shared" si="99"/>
         <v>-</v>
       </c>
-      <c r="P31">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R31">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
       <c r="T31">
         <f t="shared" si="100"/>
         <v>1</v>
@@ -4482,22 +4643,38 @@
       </c>
       <c r="AB31">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC31">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD31">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE31">
         <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AF31">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AG31">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AH31">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AI31">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4512,7 +4689,7 @@
         <v>56</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>-</v>
       </c>
       <c r="F32" t="str">
@@ -4540,35 +4717,35 @@
         <v>-</v>
       </c>
       <c r="L32" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="M32">
+        <f t="shared" ref="L32:O32" si="104">L31</f>
+        <v>-</v>
+      </c>
+      <c r="M32" t="str">
+        <f t="shared" si="104"/>
+        <v>-</v>
+      </c>
+      <c r="N32" t="str">
+        <f t="shared" si="104"/>
+        <v>-</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="104"/>
+        <v>-</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="Q32">
         <v>1200</v>
       </c>
-      <c r="N32" t="b">
-        <v>1</v>
-      </c>
-      <c r="O32" t="str">
+      <c r="R32" t="b">
+        <v>1</v>
+      </c>
+      <c r="S32" t="str">
         <f t="shared" si="99"/>
         <v>-</v>
       </c>
-      <c r="P32">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
       <c r="T32">
         <f t="shared" si="100"/>
         <v>1</v>
@@ -4603,22 +4780,38 @@
       </c>
       <c r="AB32">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC32">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD32">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE32">
         <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AF32">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AG32">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AH32">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4633,7 +4826,7 @@
         <v>57</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="101"/>
+        <f t="shared" si="102"/>
         <v>-</v>
       </c>
       <c r="F33" t="str">
@@ -4661,35 +4854,35 @@
         <v>-</v>
       </c>
       <c r="L33" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="M33">
+        <f t="shared" ref="L33:O33" si="105">L32</f>
+        <v>-</v>
+      </c>
+      <c r="M33" t="str">
+        <f t="shared" si="105"/>
+        <v>-</v>
+      </c>
+      <c r="N33" t="str">
+        <f t="shared" si="105"/>
+        <v>-</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="105"/>
+        <v>-</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="Q33">
         <v>1600</v>
       </c>
-      <c r="N33" t="b">
-        <v>1</v>
-      </c>
-      <c r="O33" t="str">
+      <c r="R33" t="b">
+        <v>1</v>
+      </c>
+      <c r="S33" t="str">
         <f t="shared" si="99"/>
         <v>-</v>
       </c>
-      <c r="P33">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R33">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
       <c r="T33">
         <f t="shared" si="100"/>
         <v>1</v>
@@ -4724,22 +4917,38 @@
       </c>
       <c r="AB33">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC33">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD33">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE33">
         <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4780,36 +4989,36 @@
         <v>-</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" ref="L34:O34" si="106">L33</f>
         <v>-</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>-</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="106"/>
         <v>-</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R34">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S34">
-        <f t="shared" si="100"/>
-        <v>1</v>
+        <f t="shared" si="106"/>
+        <v>-</v>
+      </c>
+      <c r="P34" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
       </c>
       <c r="T34">
         <f t="shared" si="100"/>
@@ -4845,22 +5054,38 @@
       </c>
       <c r="AB34">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC34">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD34">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE34">
         <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4901,36 +5126,36 @@
         <v>-</v>
       </c>
       <c r="L35" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" ref="L35:O35" si="107">L34</f>
         <v>-</v>
       </c>
       <c r="M35" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="107"/>
         <v>-</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="107"/>
         <v>-</v>
       </c>
       <c r="O35" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R35">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S35">
-        <f t="shared" si="100"/>
-        <v>1</v>
+        <f t="shared" si="107"/>
+        <v>-</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="R35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="S35" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
       </c>
       <c r="T35">
         <f t="shared" si="100"/>
@@ -4966,22 +5191,38 @@
       </c>
       <c r="AB35">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC35">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD35">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE35">
         <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AH35">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AI35">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -5022,36 +5263,36 @@
         <v>-</v>
       </c>
       <c r="L36" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" ref="L36:O36" si="108">L35</f>
         <v>-</v>
       </c>
       <c r="M36" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="108"/>
         <v>-</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="108"/>
         <v>-</v>
       </c>
       <c r="O36" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R36">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S36">
-        <f t="shared" si="100"/>
-        <v>1</v>
+        <f t="shared" si="108"/>
+        <v>-</v>
+      </c>
+      <c r="P36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="R36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="S36" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
       </c>
       <c r="T36">
         <f t="shared" si="100"/>
@@ -5087,22 +5328,38 @@
       </c>
       <c r="AB36">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC36">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD36">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE36">
         <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AF36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AG36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AH36">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AI36">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -5144,36 +5401,36 @@
         <v>-</v>
       </c>
       <c r="L37" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" ref="L37:O37" si="109">L36</f>
         <v>-</v>
       </c>
       <c r="M37" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="109"/>
         <v>-</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="109"/>
         <v>-</v>
       </c>
       <c r="O37" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R37">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S37">
-        <f t="shared" si="100"/>
-        <v>1</v>
+        <f t="shared" si="109"/>
+        <v>-</v>
+      </c>
+      <c r="P37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="R37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="S37" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
       </c>
       <c r="T37">
         <f t="shared" si="100"/>
@@ -5209,22 +5466,38 @@
       </c>
       <c r="AB37">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC37">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD37">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE37">
         <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AF37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AG37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AI37">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -5267,34 +5540,34 @@
         <v>-</v>
       </c>
       <c r="L38" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" ref="L38:O38" si="110">L37</f>
         <v>-</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" si="100"/>
+        <f t="shared" si="110"/>
         <v>-</v>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="100"/>
-        <v>-</v>
-      </c>
-      <c r="O38" t="b">
-        <v>1</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="Q38">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="R38">
-        <f t="shared" si="100"/>
-        <v>1</v>
-      </c>
-      <c r="S38">
-        <f t="shared" si="100"/>
+        <f t="shared" si="110"/>
+        <v>-</v>
+      </c>
+      <c r="O38" t="str">
+        <f t="shared" si="110"/>
+        <v>-</v>
+      </c>
+      <c r="P38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="R38" t="str">
+        <f t="shared" si="100"/>
+        <v>-</v>
+      </c>
+      <c r="S38" t="b">
         <v>1</v>
       </c>
       <c r="T38">
@@ -5331,23 +5604,40 @@
       </c>
       <c r="AB38">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC38">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD38">
         <f t="shared" si="100"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE38">
+        <f t="shared" si="100"/>
+        <v>1</v>
+      </c>
+      <c r="AF38">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AG38">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="100"/>
+        <v>0</v>
+      </c>
+      <c r="AI38">
         <f t="shared" si="100"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D4:AE4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
+  <autoFilter ref="D4:AI4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1">
     <cfRule type="cellIs" dxfId="4" priority="34" operator="equal">
       <formula>"sav"</formula>

</xml_diff>

<commit_message>
fix reports - remove trial name from lp var file Modify wean & scan report Fix axis in generator
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBD78BE-6D04-48B6-A471-AA8290E821E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B67A48-5E5A-4048-8FB0-A804F20C2CCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -947,7 +947,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
add season axis to crop
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC81D9-23CA-4D07-99BE-67FB4B31DC7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E70375-C43C-4297-9962-EB5A6C3C4C03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -942,7 +942,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B5:B6"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1262,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
exp stuff for steve. change to pkl order
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B67A48-5E5A-4048-8FB0-A804F20C2CCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B204D80C-88D4-4163-9581-35783EDF62F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -944,10 +944,10 @@
   <dimension ref="A1:AI38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B13:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1430,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -1554,7 +1554,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -1678,7 +1678,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -1802,7 +1802,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -1926,7 +1926,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2050,7 +2050,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -2174,7 +2174,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
changes for dvp and fvp so we can include more than three. Mainly dam dvp changes.
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B204D80C-88D4-4163-9581-35783EDF62F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA691C6D-636A-44B0-BDA1-7CEB1891575C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
@@ -944,10 +944,10 @@
   <dimension ref="A1:AI38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B13:B22"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1430,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="b">
         <v>0</v>
@@ -1554,7 +1554,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -1678,7 +1678,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -1802,7 +1802,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -1926,7 +1926,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -2050,7 +2050,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="b">
         <v>0</v>
@@ -2174,7 +2174,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
changes to offs sale and dvp definition stuff
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13312ED0-BFAE-4BCE-9836-703ABB648356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6CE0C4-E439-48E8-87A1-631F031DA3C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
   <si>
     <t>sam</t>
   </si>
@@ -455,6 +455,9 @@
   </si>
   <si>
     <t>steady_state</t>
+  </si>
+  <si>
+    <t>season test</t>
   </si>
 </sst>
 </file>
@@ -987,7 +990,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,19 +1490,20 @@
       <c r="C6" t="b">
         <v>0</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" ref="F6:AJ6" si="0">F5</f>
-        <v>-</v>
-      </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H6:AJ6" si="0">H5</f>
         <v>-</v>
       </c>
       <c r="I6" t="str">

</xml_diff>

<commit_message>
nothing important changed in exp
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD5F945-218B-43EF-AAEE-E12912C0DE6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E9B9EE-0787-499F-A87C-01D422CC411D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="30660" yWindow="960" windowWidth="24675" windowHeight="12840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -990,7 +990,7 @@
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="P6" sqref="P6:Q6"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1628,7 +1628,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
checking distribution is working correctly (old stuff enabled)
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E0E904-5E56-44AA-AAE8-8001CBEA70B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9AF141-814C-4428-A1C9-6B08C0919CDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -987,20 +987,20 @@
   <dimension ref="A1:AJ39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B7:B8"/>
+      <selection pane="bottomRight" activeCell="B37" sqref="B37:B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="17.5703125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>52</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1199,7 +1199,7 @@
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
     </row>
-    <row r="3" spans="1:36" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
     </row>
-    <row r="4" spans="1:36" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -1336,7 +1336,7 @@
       <c r="AH4" s="8"/>
       <c r="AI4" s="8"/>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5">
         <f>ROW(A5)-5</f>
         <v>0</v>
@@ -1479,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6">
         <f>ROW(A6)-5</f>
         <v>1</v>
@@ -1622,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" ref="A7:A39" si="1">ROW(A7)-5</f>
         <v>2</v>
@@ -1750,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1878,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2006,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2262,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2390,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -2518,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2646,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2774,7 +2774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2902,7 +2902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -3030,7 +3030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -3158,7 +3158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -3286,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -3414,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -3542,7 +3542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -3670,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -3798,7 +3798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -3926,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -4054,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -4182,7 +4182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -4310,7 +4310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -4438,7 +4438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -4566,7 +4566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -4694,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -4835,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -4976,7 +4976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -5117,7 +5117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -5258,7 +5258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -5398,7 +5398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -5538,7 +5538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -5678,7 +5678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -5687,7 +5687,7 @@
         <v>0</v>
       </c>
       <c r="C38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>63</v>
@@ -5820,7 +5820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>34</v>

</xml_diff>

<commit_message>
add report column to exp.xl
</commit_message>
<xml_diff>
--- a/exp.xlsx
+++ b/exp.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Michael\Work\AFO - local\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C0ABEF-ABDB-4C1F-97F1-5CE72F2BE5C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228EF1E6-957C-4339-B1C8-08980FD93144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92F76B5C-EE3B-4928-B619-32EB52950B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Description" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$4:$AK$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$4:$AL$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -93,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{10B3F34B-4772-43FF-8769-97F5228546B0}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{10B3F34B-4772-43FF-8769-97F5228546B0}">
       <text>
         <r>
           <rPr>
@@ -117,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{28A87732-DFBE-4E72-8AD9-CC58CDE1082B}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{28A87732-DFBE-4E72-8AD9-CC58CDE1082B}">
       <text>
         <r>
           <rPr>
@@ -141,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="1" shapeId="0" xr:uid="{3BDB7BEB-FC53-4975-ADDB-A81C02A033DC}">
+    <comment ref="E3" authorId="1" shapeId="0" xr:uid="{3BDB7BEB-FC53-4975-ADDB-A81C02A033DC}">
       <text>
         <r>
           <rPr>
@@ -166,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="1" shapeId="0" xr:uid="{7875E08E-43A6-4F76-BAD2-431E3C040A9B}">
+    <comment ref="E4" authorId="1" shapeId="0" xr:uid="{7875E08E-43A6-4F76-BAD2-431E3C040A9B}">
       <text>
         <r>
           <rPr>
@@ -192,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="1" shapeId="0" xr:uid="{86423575-3B9D-46A2-9D4D-B5C8EEE47047}">
+    <comment ref="E5" authorId="1" shapeId="0" xr:uid="{86423575-3B9D-46A2-9D4D-B5C8EEE47047}">
       <text>
         <r>
           <rPr>
@@ -246,7 +245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="75">
   <si>
     <t>sam</t>
   </si>
@@ -468,6 +467,9 @@
   </si>
   <si>
     <t>lw_inc</t>
+  </si>
+  <si>
+    <t>Report</t>
   </si>
 </sst>
 </file>
@@ -997,35 +999,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7915A7EB-445E-4E8E-983C-F21CAA7EBF41}">
-  <dimension ref="A1:AK40"/>
+  <dimension ref="A1:AL40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="9.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="53.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="53.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>42</v>
@@ -1076,7 +1075,7 @@
         <v>42</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="W1" s="6" t="s">
         <v>0</v>
@@ -1112,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="AH1" s="6" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="AI1" s="6" t="s">
         <v>41</v>
@@ -1120,25 +1119,25 @@
       <c r="AJ1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="5" t="s">
+    <row r="2" spans="1:38" s="2" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>46</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>47</v>
@@ -1147,44 +1146,44 @@
         <v>47</v>
       </c>
       <c r="K2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="X2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1198,10 +1197,10 @@
         <v>1</v>
       </c>
       <c r="AB2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="AD2" s="6" t="s">
         <v>10</v>
@@ -1215,15 +1214,17 @@
       <c r="AG2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AH2" s="6"/>
+      <c r="AH2" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="AI2" s="6"/>
       <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
     </row>
-    <row r="3" spans="1:37" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="5" t="s">
+    <row r="3" spans="1:38" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1240,9 +1241,7 @@
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6"/>
-      <c r="V3" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="V3" s="6"/>
       <c r="W3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1276,11 +1275,14 @@
       <c r="AG3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="AH3" s="6"/>
+      <c r="AH3" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="AI3" s="6"/>
       <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
     </row>
-    <row r="4" spans="1:37" s="2" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" s="2" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -1293,31 +1295,33 @@
       <c r="C4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L4" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="12"/>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
@@ -1325,43 +1329,44 @@
       <c r="S4" s="8"/>
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7" t="s">
+      <c r="V4" s="8"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="X4" s="8" t="s">
+      <c r="Y4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="Z4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="Z4" s="8" t="s">
+      <c r="AA4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AB4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7" t="s">
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AD4" s="8" t="s">
+      <c r="AE4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AF4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AG4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AG4" s="8" t="s">
+      <c r="AH4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AH4" s="8"/>
       <c r="AI4" s="8"/>
       <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5">
         <f>ROW(A5)-5</f>
         <v>0</v>
@@ -1372,12 +1377,11 @@
       <c r="C5" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="E5" s="9" t="str" cm="1">
-        <f t="array" ref="E5">_xlfn.IFS(OR(E1="sam",E1="sai"),1,E1="sav","-",OR(E1="sap",E1="saa"),0)</f>
-        <v>-</v>
       </c>
       <c r="F5" s="9" t="str" cm="1">
         <f t="array" ref="F5">_xlfn.IFS(OR(F1="sam",F1="sai"),1,F1="sav","-",OR(F1="sap",F1="saa"),0)</f>
@@ -1443,9 +1447,9 @@
         <f t="array" ref="U5">_xlfn.IFS(OR(U1="sam",U1="sai"),1,U1="sav","-",OR(U1="sap",U1="saa"),0)</f>
         <v>-</v>
       </c>
-      <c r="V5" s="9" cm="1">
+      <c r="V5" s="9" t="str" cm="1">
         <f t="array" ref="V5">_xlfn.IFS(OR(V1="sam",V1="sai"),1,V1="sav","-",OR(V1="sap",V1="saa"),0)</f>
-        <v>1</v>
+        <v>-</v>
       </c>
       <c r="W5" s="9" cm="1">
         <f t="array" ref="W5">_xlfn.IFS(OR(W1="sam",W1="sai"),1,W1="sav","-",OR(W1="sap",W1="saa"),0)</f>
@@ -1493,7 +1497,7 @@
       </c>
       <c r="AH5" s="9" cm="1">
         <f t="array" ref="AH5">_xlfn.IFS(OR(AH1="sam",AH1="sai"),1,AH1="sav","-",OR(AH1="sap",AH1="saa"),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" s="9" cm="1">
         <f t="array" ref="AI5">_xlfn.IFS(OR(AI1="sam",AI1="sai"),1,AI1="sav","-",OR(AI1="sap",AI1="saa"),0)</f>
@@ -1507,8 +1511,12 @@
         <f t="array" ref="AK5">_xlfn.IFS(OR(AK1="sam",AK1="sai"),1,AK1="sav","-",OR(AK1="sap",AK1="saa"),0)</f>
         <v>0</v>
       </c>
+      <c r="AL5" s="9" cm="1">
+        <f t="array" ref="AL5">_xlfn.IFS(OR(AL1="sam",AL1="sai"),1,AL1="sav","-",OR(AL1="sap",AL1="saa"),0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6">
         <f>ROW(A6)-5</f>
         <v>1</v>
@@ -1519,15 +1527,14 @@
       <c r="C6" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E6" t="str">
-        <f t="shared" ref="E6:AK6" si="0">E5</f>
-        <v>-</v>
-      </c>
       <c r="F6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F6:AL6" si="0">F5</f>
         <v>-</v>
       </c>
       <c r="G6" t="str">
@@ -1587,12 +1594,12 @@
         <v>-</v>
       </c>
       <c r="U6" t="str">
-        <f t="shared" ref="U6" si="1">U5</f>
-        <v>-</v>
-      </c>
-      <c r="V6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-</v>
+      </c>
+      <c r="V6" t="str">
+        <f t="shared" ref="V6" si="1">V5</f>
+        <v>-</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
@@ -1640,7 +1647,7 @@
       </c>
       <c r="AH6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6">
         <f t="shared" si="0"/>
@@ -1654,8 +1661,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="AL6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" ref="A7:A40" si="2">ROW(A7)-5</f>
         <v>2</v>
@@ -1666,15 +1677,14 @@
       <c r="C7" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" t="str">
-        <f t="shared" ref="E7:T7" si="3">E5</f>
-        <v>-</v>
-      </c>
       <c r="F7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F7:U7" si="3">F5</f>
         <v>-</v>
       </c>
       <c r="G7" t="str">
@@ -1734,15 +1744,16 @@
         <v>-</v>
       </c>
       <c r="U7" t="str">
-        <f t="shared" ref="U7" si="4">U5</f>
-        <v>-</v>
-      </c>
-      <c r="V7">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="V7" t="str">
+        <f t="shared" ref="V7" si="4">V5</f>
+        <v>-</v>
+      </c>
+      <c r="W7">
         <v>0.9</v>
       </c>
-      <c r="W7">
-        <v>1</v>
-      </c>
       <c r="X7">
         <v>1</v>
       </c>
@@ -1783,11 +1794,14 @@
         <v>1</v>
       </c>
       <c r="AK7">
-        <f>AK5</f>
+        <v>1</v>
+      </c>
+      <c r="AL7">
+        <f>AL5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -1798,43 +1812,42 @@
       <c r="C8" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="str">
-        <f t="shared" ref="E8:E30" si="5">E7</f>
-        <v>-</v>
-      </c>
       <c r="F8" t="str">
-        <f t="shared" ref="F8" si="6">F7</f>
+        <f t="shared" ref="F8:F30" si="5">F7</f>
         <v>-</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" ref="G8:G30" si="7">G7</f>
+        <f t="shared" ref="G8" si="6">G7</f>
         <v>-</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" ref="H8:H30" si="8">H7</f>
+        <f t="shared" ref="H8:H30" si="7">H7</f>
         <v>-</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" ref="I8:I30" si="9">I7</f>
+        <f t="shared" ref="I8:I30" si="8">I7</f>
         <v>-</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" ref="J8:J30" si="10">J7</f>
+        <f t="shared" ref="J8:J30" si="9">J7</f>
         <v>-</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" ref="K8" si="11">K7</f>
+        <f t="shared" ref="K8:K30" si="10">K7</f>
         <v>-</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" ref="L8:P8" si="12">L7</f>
+        <f t="shared" ref="L8" si="11">L7</f>
         <v>-</v>
       </c>
       <c r="M8" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="M8:Q8" si="12">M7</f>
         <v>-</v>
       </c>
       <c r="N8" t="str">
@@ -1850,11 +1863,11 @@
         <v>-</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" ref="Q8:S8" si="13">Q7</f>
+        <f t="shared" si="12"/>
         <v>-</v>
       </c>
       <c r="R8" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="R8:T8" si="13">R7</f>
         <v>-</v>
       </c>
       <c r="S8" t="str">
@@ -1862,19 +1875,20 @@
         <v>-</v>
       </c>
       <c r="T8" t="str">
-        <f t="shared" ref="T8:U8" si="14">T7</f>
+        <f t="shared" si="13"/>
         <v>-</v>
       </c>
       <c r="U8" t="str">
+        <f t="shared" ref="U8:V8" si="14">U7</f>
+        <v>-</v>
+      </c>
+      <c r="V8" t="str">
         <f t="shared" si="14"/>
         <v>-</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="W8">
-        <v>1</v>
-      </c>
       <c r="X8">
         <v>1</v>
       </c>
@@ -1915,11 +1929,14 @@
         <v>1</v>
       </c>
       <c r="AK8">
-        <f t="shared" ref="AK8:AK30" si="15">AK7</f>
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <f t="shared" ref="AL8:AL30" si="15">AL7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -1930,43 +1947,42 @@
       <c r="C9" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="str">
+      <c r="F9" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F9" t="str">
-        <f t="shared" ref="F9" si="16">F8</f>
-        <v>-</v>
-      </c>
       <c r="G9" t="str">
+        <f t="shared" ref="G9" si="16">G8</f>
+        <v>-</v>
+      </c>
+      <c r="H9" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K9" t="str">
-        <f t="shared" ref="K9" si="17">K8</f>
-        <v>-</v>
-      </c>
       <c r="L9" t="str">
-        <f t="shared" ref="L9:P9" si="18">L8</f>
+        <f t="shared" ref="L9" si="17">L8</f>
         <v>-</v>
       </c>
       <c r="M9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="M9:Q9" si="18">M8</f>
         <v>-</v>
       </c>
       <c r="N9" t="str">
@@ -1982,11 +1998,11 @@
         <v>-</v>
       </c>
       <c r="Q9" t="str">
-        <f t="shared" ref="Q9:S9" si="19">Q8</f>
+        <f t="shared" si="18"/>
         <v>-</v>
       </c>
       <c r="R9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="R9:T9" si="19">R8</f>
         <v>-</v>
       </c>
       <c r="S9" t="str">
@@ -1994,22 +2010,23 @@
         <v>-</v>
       </c>
       <c r="T9" t="str">
-        <f t="shared" ref="T9:U9" si="20">T8</f>
+        <f t="shared" si="19"/>
         <v>-</v>
       </c>
       <c r="U9" t="str">
+        <f t="shared" ref="U9:V9" si="20">U8</f>
+        <v>-</v>
+      </c>
+      <c r="V9" t="str">
         <f t="shared" si="20"/>
         <v>-</v>
       </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
       <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
         <v>0.9</v>
       </c>
-      <c r="X9">
-        <v>1</v>
-      </c>
       <c r="Y9">
         <v>1</v>
       </c>
@@ -2047,11 +2064,14 @@
         <v>1</v>
       </c>
       <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -2062,43 +2082,42 @@
       <c r="C10" t="b">
         <v>0</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E10" t="str">
+      <c r="F10" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F10" t="str">
-        <f t="shared" ref="F10" si="21">F9</f>
-        <v>-</v>
-      </c>
       <c r="G10" t="str">
+        <f t="shared" ref="G10" si="21">G9</f>
+        <v>-</v>
+      </c>
+      <c r="H10" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K10" t="str">
-        <f t="shared" ref="K10" si="22">K9</f>
-        <v>-</v>
-      </c>
       <c r="L10" t="str">
-        <f t="shared" ref="L10:P10" si="23">L9</f>
+        <f t="shared" ref="L10" si="22">L9</f>
         <v>-</v>
       </c>
       <c r="M10" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="M10:Q10" si="23">M9</f>
         <v>-</v>
       </c>
       <c r="N10" t="str">
@@ -2114,11 +2133,11 @@
         <v>-</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" ref="Q10:S10" si="24">Q9</f>
+        <f t="shared" si="23"/>
         <v>-</v>
       </c>
       <c r="R10" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="R10:T10" si="24">R9</f>
         <v>-</v>
       </c>
       <c r="S10" t="str">
@@ -2126,22 +2145,23 @@
         <v>-</v>
       </c>
       <c r="T10" t="str">
-        <f t="shared" ref="T10:U10" si="25">T9</f>
+        <f t="shared" si="24"/>
         <v>-</v>
       </c>
       <c r="U10" t="str">
+        <f t="shared" ref="U10:V10" si="25">U9</f>
+        <v>-</v>
+      </c>
+      <c r="V10" t="str">
         <f t="shared" si="25"/>
         <v>-</v>
       </c>
-      <c r="V10">
-        <v>1</v>
-      </c>
       <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
         <v>1.1000000000000001</v>
       </c>
-      <c r="X10">
-        <v>1</v>
-      </c>
       <c r="Y10">
         <v>1</v>
       </c>
@@ -2179,11 +2199,14 @@
         <v>1</v>
       </c>
       <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -2194,43 +2217,42 @@
       <c r="C11" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="str">
+      <c r="F11" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" ref="F11" si="26">F10</f>
-        <v>-</v>
-      </c>
       <c r="G11" t="str">
+        <f t="shared" ref="G11" si="26">G10</f>
+        <v>-</v>
+      </c>
+      <c r="H11" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J11" t="str">
+      <c r="K11" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K11" t="str">
-        <f t="shared" ref="K11" si="27">K10</f>
-        <v>-</v>
-      </c>
       <c r="L11" t="str">
-        <f t="shared" ref="L11:P11" si="28">L10</f>
+        <f t="shared" ref="L11" si="27">L10</f>
         <v>-</v>
       </c>
       <c r="M11" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="M11:Q11" si="28">M10</f>
         <v>-</v>
       </c>
       <c r="N11" t="str">
@@ -2246,11 +2268,11 @@
         <v>-</v>
       </c>
       <c r="Q11" t="str">
-        <f t="shared" ref="Q11:S11" si="29">Q10</f>
+        <f t="shared" si="28"/>
         <v>-</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="R11:T11" si="29">R10</f>
         <v>-</v>
       </c>
       <c r="S11" t="str">
@@ -2258,25 +2280,26 @@
         <v>-</v>
       </c>
       <c r="T11" t="str">
-        <f t="shared" ref="T11:U11" si="30">T10</f>
+        <f t="shared" si="29"/>
         <v>-</v>
       </c>
       <c r="U11" t="str">
+        <f t="shared" ref="U11:V11" si="30">U10</f>
+        <v>-</v>
+      </c>
+      <c r="V11" t="str">
         <f t="shared" si="30"/>
         <v>-</v>
       </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
       <c r="W11">
         <v>1</v>
       </c>
       <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
         <v>0.9</v>
       </c>
-      <c r="Y11">
-        <v>1</v>
-      </c>
       <c r="Z11">
         <v>1</v>
       </c>
@@ -2311,11 +2334,14 @@
         <v>1</v>
       </c>
       <c r="AK11">
+        <v>1</v>
+      </c>
+      <c r="AL11">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -2326,43 +2352,42 @@
       <c r="C12" t="b">
         <v>0</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="str">
+      <c r="F12" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F12" t="str">
-        <f t="shared" ref="F12" si="31">F11</f>
-        <v>-</v>
-      </c>
       <c r="G12" t="str">
+        <f t="shared" ref="G12" si="31">G11</f>
+        <v>-</v>
+      </c>
+      <c r="H12" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I12" t="str">
+      <c r="J12" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K12" t="str">
-        <f t="shared" ref="K12" si="32">K11</f>
-        <v>-</v>
-      </c>
       <c r="L12" t="str">
-        <f t="shared" ref="L12:P12" si="33">L11</f>
+        <f t="shared" ref="L12" si="32">L11</f>
         <v>-</v>
       </c>
       <c r="M12" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" ref="M12:Q12" si="33">M11</f>
         <v>-</v>
       </c>
       <c r="N12" t="str">
@@ -2378,11 +2403,11 @@
         <v>-</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" ref="Q12:S12" si="34">Q11</f>
+        <f t="shared" si="33"/>
         <v>-</v>
       </c>
       <c r="R12" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="R12:T12" si="34">R11</f>
         <v>-</v>
       </c>
       <c r="S12" t="str">
@@ -2390,25 +2415,26 @@
         <v>-</v>
       </c>
       <c r="T12" t="str">
-        <f t="shared" ref="T12:U12" si="35">T11</f>
+        <f t="shared" si="34"/>
         <v>-</v>
       </c>
       <c r="U12" t="str">
+        <f t="shared" ref="U12:V12" si="35">U11</f>
+        <v>-</v>
+      </c>
+      <c r="V12" t="str">
         <f t="shared" si="35"/>
         <v>-</v>
       </c>
-      <c r="V12">
-        <v>1</v>
-      </c>
       <c r="W12">
         <v>1</v>
       </c>
       <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Y12">
-        <v>1</v>
-      </c>
       <c r="Z12">
         <v>1</v>
       </c>
@@ -2443,11 +2469,14 @@
         <v>1</v>
       </c>
       <c r="AK12">
+        <v>1</v>
+      </c>
+      <c r="AL12">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -2458,43 +2487,42 @@
       <c r="C13" t="b">
         <v>0</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E13" t="str">
+      <c r="F13" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F13" t="str">
-        <f t="shared" ref="F13" si="36">F12</f>
-        <v>-</v>
-      </c>
       <c r="G13" t="str">
+        <f t="shared" ref="G13" si="36">G12</f>
+        <v>-</v>
+      </c>
+      <c r="H13" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J13" t="str">
+      <c r="K13" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K13" t="str">
-        <f t="shared" ref="K13" si="37">K12</f>
-        <v>-</v>
-      </c>
       <c r="L13" t="str">
-        <f t="shared" ref="L13:P13" si="38">L12</f>
+        <f t="shared" ref="L13" si="37">L12</f>
         <v>-</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="M13:Q13" si="38">M12</f>
         <v>-</v>
       </c>
       <c r="N13" t="str">
@@ -2510,11 +2538,11 @@
         <v>-</v>
       </c>
       <c r="Q13" t="str">
-        <f t="shared" ref="Q13:S13" si="39">Q12</f>
+        <f t="shared" si="38"/>
         <v>-</v>
       </c>
       <c r="R13" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" ref="R13:T13" si="39">R12</f>
         <v>-</v>
       </c>
       <c r="S13" t="str">
@@ -2522,16 +2550,17 @@
         <v>-</v>
       </c>
       <c r="T13" t="str">
-        <f t="shared" ref="T13:U13" si="40">T12</f>
+        <f t="shared" si="39"/>
         <v>-</v>
       </c>
       <c r="U13" t="str">
+        <f t="shared" ref="U13:V13" si="40">U12</f>
+        <v>-</v>
+      </c>
+      <c r="V13" t="str">
         <f t="shared" si="40"/>
         <v>-</v>
       </c>
-      <c r="V13">
-        <v>1</v>
-      </c>
       <c r="W13">
         <v>1</v>
       </c>
@@ -2539,11 +2568,11 @@
         <v>1</v>
       </c>
       <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
         <v>0.9</v>
       </c>
-      <c r="Z13">
-        <v>1</v>
-      </c>
       <c r="AA13">
         <v>1</v>
       </c>
@@ -2575,11 +2604,14 @@
         <v>1</v>
       </c>
       <c r="AK13">
+        <v>1</v>
+      </c>
+      <c r="AL13">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -2590,43 +2622,42 @@
       <c r="C14" t="b">
         <v>0</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E14" t="str">
+      <c r="F14" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F14" t="str">
-        <f t="shared" ref="F14" si="41">F13</f>
-        <v>-</v>
-      </c>
       <c r="G14" t="str">
+        <f t="shared" ref="G14" si="41">G13</f>
+        <v>-</v>
+      </c>
+      <c r="H14" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H14" t="str">
+      <c r="I14" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I14" t="str">
+      <c r="J14" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J14" t="str">
+      <c r="K14" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K14" t="str">
-        <f t="shared" ref="K14" si="42">K13</f>
-        <v>-</v>
-      </c>
       <c r="L14" t="str">
-        <f t="shared" ref="L14:P14" si="43">L13</f>
+        <f t="shared" ref="L14" si="42">L13</f>
         <v>-</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" ref="M14:Q14" si="43">M13</f>
         <v>-</v>
       </c>
       <c r="N14" t="str">
@@ -2642,11 +2673,11 @@
         <v>-</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" ref="Q14:S14" si="44">Q13</f>
+        <f t="shared" si="43"/>
         <v>-</v>
       </c>
       <c r="R14" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" ref="R14:T14" si="44">R13</f>
         <v>-</v>
       </c>
       <c r="S14" t="str">
@@ -2654,16 +2685,17 @@
         <v>-</v>
       </c>
       <c r="T14" t="str">
-        <f t="shared" ref="T14:U14" si="45">T13</f>
+        <f t="shared" si="44"/>
         <v>-</v>
       </c>
       <c r="U14" t="str">
+        <f t="shared" ref="U14:V14" si="45">U13</f>
+        <v>-</v>
+      </c>
+      <c r="V14" t="str">
         <f t="shared" si="45"/>
         <v>-</v>
       </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
       <c r="W14">
         <v>1</v>
       </c>
@@ -2671,11 +2703,11 @@
         <v>1</v>
       </c>
       <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="Z14">
-        <v>1</v>
-      </c>
       <c r="AA14">
         <v>1</v>
       </c>
@@ -2707,11 +2739,14 @@
         <v>1</v>
       </c>
       <c r="AK14">
+        <v>1</v>
+      </c>
+      <c r="AL14">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -2722,43 +2757,42 @@
       <c r="C15" t="b">
         <v>0</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E15" t="str">
+      <c r="F15" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F15" t="str">
-        <f t="shared" ref="F15" si="46">F14</f>
-        <v>-</v>
-      </c>
       <c r="G15" t="str">
+        <f t="shared" ref="G15" si="46">G14</f>
+        <v>-</v>
+      </c>
+      <c r="H15" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H15" t="str">
+      <c r="I15" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I15" t="str">
+      <c r="J15" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J15" t="str">
+      <c r="K15" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K15" t="str">
-        <f t="shared" ref="K15" si="47">K14</f>
-        <v>-</v>
-      </c>
       <c r="L15" t="str">
-        <f t="shared" ref="L15:P15" si="48">L14</f>
+        <f t="shared" ref="L15" si="47">L14</f>
         <v>-</v>
       </c>
       <c r="M15" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="M15:Q15" si="48">M14</f>
         <v>-</v>
       </c>
       <c r="N15" t="str">
@@ -2774,11 +2808,11 @@
         <v>-</v>
       </c>
       <c r="Q15" t="str">
-        <f t="shared" ref="Q15:S15" si="49">Q14</f>
+        <f t="shared" si="48"/>
         <v>-</v>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" ref="R15:T15" si="49">R14</f>
         <v>-</v>
       </c>
       <c r="S15" t="str">
@@ -2786,16 +2820,17 @@
         <v>-</v>
       </c>
       <c r="T15" t="str">
-        <f t="shared" ref="T15:U15" si="50">T14</f>
+        <f t="shared" si="49"/>
         <v>-</v>
       </c>
       <c r="U15" t="str">
+        <f t="shared" ref="U15:V15" si="50">U14</f>
+        <v>-</v>
+      </c>
+      <c r="V15" t="str">
         <f t="shared" si="50"/>
         <v>-</v>
       </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
       <c r="W15">
         <v>1</v>
       </c>
@@ -2806,11 +2841,11 @@
         <v>1</v>
       </c>
       <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
         <v>0.9</v>
       </c>
-      <c r="AA15">
-        <v>1</v>
-      </c>
       <c r="AB15">
         <v>1</v>
       </c>
@@ -2839,11 +2874,14 @@
         <v>1</v>
       </c>
       <c r="AK15">
+        <v>1</v>
+      </c>
+      <c r="AL15">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -2854,43 +2892,42 @@
       <c r="C16" t="b">
         <v>0</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="str">
+      <c r="F16" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" ref="F16" si="51">F15</f>
-        <v>-</v>
-      </c>
       <c r="G16" t="str">
+        <f t="shared" ref="G16" si="51">G15</f>
+        <v>-</v>
+      </c>
+      <c r="H16" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I16" t="str">
+      <c r="J16" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J16" t="str">
+      <c r="K16" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K16" t="str">
-        <f t="shared" ref="K16" si="52">K15</f>
-        <v>-</v>
-      </c>
       <c r="L16" t="str">
-        <f t="shared" ref="L16:P16" si="53">L15</f>
+        <f t="shared" ref="L16" si="52">L15</f>
         <v>-</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="M16:Q16" si="53">M15</f>
         <v>-</v>
       </c>
       <c r="N16" t="str">
@@ -2906,11 +2943,11 @@
         <v>-</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" ref="Q16:S16" si="54">Q15</f>
+        <f t="shared" si="53"/>
         <v>-</v>
       </c>
       <c r="R16" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" ref="R16:T16" si="54">R15</f>
         <v>-</v>
       </c>
       <c r="S16" t="str">
@@ -2918,16 +2955,17 @@
         <v>-</v>
       </c>
       <c r="T16" t="str">
-        <f t="shared" ref="T16:U16" si="55">T15</f>
+        <f t="shared" si="54"/>
         <v>-</v>
       </c>
       <c r="U16" t="str">
+        <f t="shared" ref="U16:V16" si="55">U15</f>
+        <v>-</v>
+      </c>
+      <c r="V16" t="str">
         <f t="shared" si="55"/>
         <v>-</v>
       </c>
-      <c r="V16">
-        <v>1</v>
-      </c>
       <c r="W16">
         <v>1</v>
       </c>
@@ -2938,11 +2976,11 @@
         <v>1</v>
       </c>
       <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AA16">
-        <v>1</v>
-      </c>
       <c r="AB16">
         <v>1</v>
       </c>
@@ -2971,11 +3009,14 @@
         <v>1</v>
       </c>
       <c r="AK16">
+        <v>1</v>
+      </c>
+      <c r="AL16">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -2986,43 +3027,42 @@
       <c r="C17" t="b">
         <v>0</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E17" t="str">
+      <c r="F17" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F17" t="str">
-        <f t="shared" ref="F17" si="56">F16</f>
-        <v>-</v>
-      </c>
       <c r="G17" t="str">
+        <f t="shared" ref="G17" si="56">G16</f>
+        <v>-</v>
+      </c>
+      <c r="H17" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I17" t="str">
+      <c r="J17" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J17" t="str">
+      <c r="K17" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K17" t="str">
-        <f t="shared" ref="K17" si="57">K16</f>
-        <v>-</v>
-      </c>
       <c r="L17" t="str">
-        <f t="shared" ref="L17:P17" si="58">L16</f>
+        <f t="shared" ref="L17" si="57">L16</f>
         <v>-</v>
       </c>
       <c r="M17" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" ref="M17:Q17" si="58">M16</f>
         <v>-</v>
       </c>
       <c r="N17" t="str">
@@ -3038,11 +3078,11 @@
         <v>-</v>
       </c>
       <c r="Q17" t="str">
-        <f t="shared" ref="Q17:S17" si="59">Q16</f>
+        <f t="shared" si="58"/>
         <v>-</v>
       </c>
       <c r="R17" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" ref="R17:T17" si="59">R16</f>
         <v>-</v>
       </c>
       <c r="S17" t="str">
@@ -3050,16 +3090,17 @@
         <v>-</v>
       </c>
       <c r="T17" t="str">
-        <f t="shared" ref="T17:U17" si="60">T16</f>
+        <f t="shared" si="59"/>
         <v>-</v>
       </c>
       <c r="U17" t="str">
+        <f t="shared" ref="U17:V17" si="60">U16</f>
+        <v>-</v>
+      </c>
+      <c r="V17" t="str">
         <f t="shared" si="60"/>
         <v>-</v>
       </c>
-      <c r="V17">
-        <v>1</v>
-      </c>
       <c r="W17">
         <v>1</v>
       </c>
@@ -3073,11 +3114,11 @@
         <v>1</v>
       </c>
       <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
         <v>0.9</v>
       </c>
-      <c r="AB17">
-        <v>1</v>
-      </c>
       <c r="AC17">
         <v>1</v>
       </c>
@@ -3103,11 +3144,14 @@
         <v>1</v>
       </c>
       <c r="AK17">
+        <v>1</v>
+      </c>
+      <c r="AL17">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -3118,43 +3162,42 @@
       <c r="C18" t="b">
         <v>0</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E18" t="str">
+      <c r="F18" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F18" t="str">
-        <f t="shared" ref="F18" si="61">F17</f>
-        <v>-</v>
-      </c>
       <c r="G18" t="str">
+        <f t="shared" ref="G18" si="61">G17</f>
+        <v>-</v>
+      </c>
+      <c r="H18" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H18" t="str">
+      <c r="I18" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I18" t="str">
+      <c r="J18" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J18" t="str">
+      <c r="K18" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K18" t="str">
-        <f t="shared" ref="K18" si="62">K17</f>
-        <v>-</v>
-      </c>
       <c r="L18" t="str">
-        <f t="shared" ref="L18:P18" si="63">L17</f>
+        <f t="shared" ref="L18" si="62">L17</f>
         <v>-</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" si="63"/>
+        <f t="shared" ref="M18:Q18" si="63">M17</f>
         <v>-</v>
       </c>
       <c r="N18" t="str">
@@ -3170,11 +3213,11 @@
         <v>-</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" ref="Q18:S18" si="64">Q17</f>
+        <f t="shared" si="63"/>
         <v>-</v>
       </c>
       <c r="R18" t="str">
-        <f t="shared" si="64"/>
+        <f t="shared" ref="R18:T18" si="64">R17</f>
         <v>-</v>
       </c>
       <c r="S18" t="str">
@@ -3182,16 +3225,17 @@
         <v>-</v>
       </c>
       <c r="T18" t="str">
-        <f t="shared" ref="T18:U18" si="65">T17</f>
+        <f t="shared" si="64"/>
         <v>-</v>
       </c>
       <c r="U18" t="str">
+        <f t="shared" ref="U18:V18" si="65">U17</f>
+        <v>-</v>
+      </c>
+      <c r="V18" t="str">
         <f t="shared" si="65"/>
         <v>-</v>
       </c>
-      <c r="V18">
-        <v>1</v>
-      </c>
       <c r="W18">
         <v>1</v>
       </c>
@@ -3205,11 +3249,11 @@
         <v>1</v>
       </c>
       <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AB18">
-        <v>1</v>
-      </c>
       <c r="AC18">
         <v>1</v>
       </c>
@@ -3235,11 +3279,14 @@
         <v>1</v>
       </c>
       <c r="AK18">
+        <v>1</v>
+      </c>
+      <c r="AL18">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -3250,43 +3297,42 @@
       <c r="C19" t="b">
         <v>0</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E19" t="str">
+      <c r="F19" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F19" t="str">
-        <f t="shared" ref="F19" si="66">F18</f>
-        <v>-</v>
-      </c>
       <c r="G19" t="str">
+        <f t="shared" ref="G19" si="66">G18</f>
+        <v>-</v>
+      </c>
+      <c r="H19" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H19" t="str">
+      <c r="I19" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I19" t="str">
+      <c r="J19" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J19" t="str">
+      <c r="K19" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K19" t="str">
-        <f t="shared" ref="K19" si="67">K18</f>
-        <v>-</v>
-      </c>
       <c r="L19" t="str">
-        <f t="shared" ref="L19:P19" si="68">L18</f>
+        <f t="shared" ref="L19" si="67">L18</f>
         <v>-</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" si="68"/>
+        <f t="shared" ref="M19:Q19" si="68">M18</f>
         <v>-</v>
       </c>
       <c r="N19" t="str">
@@ -3302,11 +3348,11 @@
         <v>-</v>
       </c>
       <c r="Q19" t="str">
-        <f t="shared" ref="Q19:S19" si="69">Q18</f>
+        <f t="shared" si="68"/>
         <v>-</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="69"/>
+        <f t="shared" ref="R19:T19" si="69">R18</f>
         <v>-</v>
       </c>
       <c r="S19" t="str">
@@ -3314,16 +3360,17 @@
         <v>-</v>
       </c>
       <c r="T19" t="str">
-        <f t="shared" ref="T19:U19" si="70">T18</f>
+        <f t="shared" si="69"/>
         <v>-</v>
       </c>
       <c r="U19" t="str">
+        <f t="shared" ref="U19:V19" si="70">U18</f>
+        <v>-</v>
+      </c>
+      <c r="V19" t="str">
         <f t="shared" si="70"/>
         <v>-</v>
       </c>
-      <c r="V19">
-        <v>1</v>
-      </c>
       <c r="W19">
         <v>1</v>
       </c>
@@ -3340,11 +3387,11 @@
         <v>1</v>
       </c>
       <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
         <v>0.9</v>
       </c>
-      <c r="AC19">
-        <v>1</v>
-      </c>
       <c r="AD19">
         <v>1</v>
       </c>
@@ -3367,11 +3414,14 @@
         <v>1</v>
       </c>
       <c r="AK19">
+        <v>1</v>
+      </c>
+      <c r="AL19">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -3382,43 +3432,42 @@
       <c r="C20" t="b">
         <v>0</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E20" t="str">
+      <c r="F20" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F20" t="str">
-        <f t="shared" ref="F20" si="71">F19</f>
-        <v>-</v>
-      </c>
       <c r="G20" t="str">
+        <f t="shared" ref="G20" si="71">G19</f>
+        <v>-</v>
+      </c>
+      <c r="H20" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H20" t="str">
+      <c r="I20" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I20" t="str">
+      <c r="J20" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J20" t="str">
+      <c r="K20" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K20" t="str">
-        <f t="shared" ref="K20" si="72">K19</f>
-        <v>-</v>
-      </c>
       <c r="L20" t="str">
-        <f t="shared" ref="L20:P20" si="73">L19</f>
+        <f t="shared" ref="L20" si="72">L19</f>
         <v>-</v>
       </c>
       <c r="M20" t="str">
-        <f t="shared" si="73"/>
+        <f t="shared" ref="M20:Q20" si="73">M19</f>
         <v>-</v>
       </c>
       <c r="N20" t="str">
@@ -3434,11 +3483,11 @@
         <v>-</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" ref="Q20:S20" si="74">Q19</f>
+        <f t="shared" si="73"/>
         <v>-</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="74"/>
+        <f t="shared" ref="R20:T20" si="74">R19</f>
         <v>-</v>
       </c>
       <c r="S20" t="str">
@@ -3446,16 +3495,17 @@
         <v>-</v>
       </c>
       <c r="T20" t="str">
-        <f t="shared" ref="T20:U20" si="75">T19</f>
+        <f t="shared" si="74"/>
         <v>-</v>
       </c>
       <c r="U20" t="str">
+        <f t="shared" ref="U20:V20" si="75">U19</f>
+        <v>-</v>
+      </c>
+      <c r="V20" t="str">
         <f t="shared" si="75"/>
         <v>-</v>
       </c>
-      <c r="V20">
-        <v>1</v>
-      </c>
       <c r="W20">
         <v>1</v>
       </c>
@@ -3472,11 +3522,11 @@
         <v>1</v>
       </c>
       <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AC20">
-        <v>1</v>
-      </c>
       <c r="AD20">
         <v>1</v>
       </c>
@@ -3499,11 +3549,14 @@
         <v>1</v>
       </c>
       <c r="AK20">
+        <v>1</v>
+      </c>
+      <c r="AL20">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -3514,43 +3567,42 @@
       <c r="C21" t="b">
         <v>0</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E21" t="str">
+      <c r="F21" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F21" t="str">
-        <f t="shared" ref="F21" si="76">F20</f>
-        <v>-</v>
-      </c>
       <c r="G21" t="str">
+        <f t="shared" ref="G21" si="76">G20</f>
+        <v>-</v>
+      </c>
+      <c r="H21" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H21" t="str">
+      <c r="I21" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I21" t="str">
+      <c r="J21" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J21" t="str">
+      <c r="K21" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K21" t="str">
-        <f t="shared" ref="K21" si="77">K20</f>
-        <v>-</v>
-      </c>
       <c r="L21" t="str">
-        <f t="shared" ref="L21:P21" si="78">L20</f>
+        <f t="shared" ref="L21" si="77">L20</f>
         <v>-</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" si="78"/>
+        <f t="shared" ref="M21:Q21" si="78">M20</f>
         <v>-</v>
       </c>
       <c r="N21" t="str">
@@ -3566,11 +3618,11 @@
         <v>-</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" ref="Q21:S21" si="79">Q20</f>
+        <f t="shared" si="78"/>
         <v>-</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="79"/>
+        <f t="shared" ref="R21:T21" si="79">R20</f>
         <v>-</v>
       </c>
       <c r="S21" t="str">
@@ -3578,16 +3630,17 @@
         <v>-</v>
       </c>
       <c r="T21" t="str">
-        <f t="shared" ref="T21:U21" si="80">T20</f>
+        <f t="shared" si="79"/>
         <v>-</v>
       </c>
       <c r="U21" t="str">
+        <f t="shared" ref="U21:V21" si="80">U20</f>
+        <v>-</v>
+      </c>
+      <c r="V21" t="str">
         <f t="shared" si="80"/>
         <v>-</v>
       </c>
-      <c r="V21">
-        <v>1</v>
-      </c>
       <c r="W21">
         <v>1</v>
       </c>
@@ -3607,11 +3660,11 @@
         <v>1</v>
       </c>
       <c r="AC21">
+        <v>1</v>
+      </c>
+      <c r="AD21">
         <v>0.9</v>
       </c>
-      <c r="AD21">
-        <v>1</v>
-      </c>
       <c r="AE21">
         <v>1</v>
       </c>
@@ -3631,11 +3684,14 @@
         <v>1</v>
       </c>
       <c r="AK21">
+        <v>1</v>
+      </c>
+      <c r="AL21">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -3646,43 +3702,42 @@
       <c r="C22" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E22" t="str">
+      <c r="F22" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F22" t="str">
-        <f t="shared" ref="F22" si="81">F21</f>
-        <v>-</v>
-      </c>
       <c r="G22" t="str">
+        <f t="shared" ref="G22" si="81">G21</f>
+        <v>-</v>
+      </c>
+      <c r="H22" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H22" t="str">
+      <c r="I22" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I22" t="str">
+      <c r="J22" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J22" t="str">
+      <c r="K22" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K22" t="str">
-        <f t="shared" ref="K22" si="82">K21</f>
-        <v>-</v>
-      </c>
       <c r="L22" t="str">
-        <f t="shared" ref="L22:P22" si="83">L21</f>
+        <f t="shared" ref="L22" si="82">L21</f>
         <v>-</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" si="83"/>
+        <f t="shared" ref="M22:Q22" si="83">M21</f>
         <v>-</v>
       </c>
       <c r="N22" t="str">
@@ -3698,11 +3753,11 @@
         <v>-</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" ref="Q22:S22" si="84">Q21</f>
+        <f t="shared" si="83"/>
         <v>-</v>
       </c>
       <c r="R22" t="str">
-        <f t="shared" si="84"/>
+        <f t="shared" ref="R22:T22" si="84">R21</f>
         <v>-</v>
       </c>
       <c r="S22" t="str">
@@ -3710,16 +3765,17 @@
         <v>-</v>
       </c>
       <c r="T22" t="str">
-        <f t="shared" ref="T22:U22" si="85">T21</f>
+        <f t="shared" si="84"/>
         <v>-</v>
       </c>
       <c r="U22" t="str">
+        <f t="shared" ref="U22:V22" si="85">U21</f>
+        <v>-</v>
+      </c>
+      <c r="V22" t="str">
         <f t="shared" si="85"/>
         <v>-</v>
       </c>
-      <c r="V22">
-        <v>1</v>
-      </c>
       <c r="W22">
         <v>1</v>
       </c>
@@ -3739,11 +3795,11 @@
         <v>1</v>
       </c>
       <c r="AC22">
+        <v>1</v>
+      </c>
+      <c r="AD22">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AD22">
-        <v>1</v>
-      </c>
       <c r="AE22">
         <v>1</v>
       </c>
@@ -3763,11 +3819,14 @@
         <v>1</v>
       </c>
       <c r="AK22">
+        <v>1</v>
+      </c>
+      <c r="AL22">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -3778,43 +3837,42 @@
       <c r="C23" t="b">
         <v>0</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E23" t="str">
+      <c r="F23" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F23" t="str">
-        <f t="shared" ref="F23" si="86">F22</f>
-        <v>-</v>
-      </c>
       <c r="G23" t="str">
+        <f t="shared" ref="G23" si="86">G22</f>
+        <v>-</v>
+      </c>
+      <c r="H23" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H23" t="str">
+      <c r="I23" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I23" t="str">
+      <c r="J23" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J23" t="str">
+      <c r="K23" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K23" t="str">
-        <f t="shared" ref="K23" si="87">K22</f>
-        <v>-</v>
-      </c>
       <c r="L23" t="str">
-        <f t="shared" ref="L23:P23" si="88">L22</f>
+        <f t="shared" ref="L23" si="87">L22</f>
         <v>-</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" si="88"/>
+        <f t="shared" ref="M23:Q23" si="88">M22</f>
         <v>-</v>
       </c>
       <c r="N23" t="str">
@@ -3830,11 +3888,11 @@
         <v>-</v>
       </c>
       <c r="Q23" t="str">
-        <f t="shared" ref="Q23:S23" si="89">Q22</f>
+        <f t="shared" si="88"/>
         <v>-</v>
       </c>
       <c r="R23" t="str">
-        <f t="shared" si="89"/>
+        <f t="shared" ref="R23:T23" si="89">R22</f>
         <v>-</v>
       </c>
       <c r="S23" t="str">
@@ -3842,16 +3900,17 @@
         <v>-</v>
       </c>
       <c r="T23" t="str">
-        <f t="shared" ref="T23:U23" si="90">T22</f>
+        <f t="shared" si="89"/>
         <v>-</v>
       </c>
       <c r="U23" t="str">
+        <f t="shared" ref="U23:V23" si="90">U22</f>
+        <v>-</v>
+      </c>
+      <c r="V23" t="str">
         <f t="shared" si="90"/>
         <v>-</v>
       </c>
-      <c r="V23">
-        <v>1</v>
-      </c>
       <c r="W23">
         <v>1</v>
       </c>
@@ -3874,11 +3933,11 @@
         <v>1</v>
       </c>
       <c r="AD23">
+        <v>1</v>
+      </c>
+      <c r="AE23">
         <v>0.9</v>
       </c>
-      <c r="AE23">
-        <v>1</v>
-      </c>
       <c r="AF23">
         <v>1</v>
       </c>
@@ -3895,11 +3954,14 @@
         <v>1</v>
       </c>
       <c r="AK23">
+        <v>1</v>
+      </c>
+      <c r="AL23">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -3910,43 +3972,42 @@
       <c r="C24" t="b">
         <v>0</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E24" t="str">
+      <c r="F24" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F24" t="str">
-        <f t="shared" ref="F24" si="91">F23</f>
-        <v>-</v>
-      </c>
       <c r="G24" t="str">
+        <f t="shared" ref="G24" si="91">G23</f>
+        <v>-</v>
+      </c>
+      <c r="H24" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H24" t="str">
+      <c r="I24" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I24" t="str">
+      <c r="J24" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J24" t="str">
+      <c r="K24" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K24" t="str">
-        <f t="shared" ref="K24" si="92">K23</f>
-        <v>-</v>
-      </c>
       <c r="L24" t="str">
-        <f t="shared" ref="L24:P24" si="93">L23</f>
+        <f t="shared" ref="L24" si="92">L23</f>
         <v>-</v>
       </c>
       <c r="M24" t="str">
-        <f t="shared" si="93"/>
+        <f t="shared" ref="M24:Q24" si="93">M23</f>
         <v>-</v>
       </c>
       <c r="N24" t="str">
@@ -3962,11 +4023,11 @@
         <v>-</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" ref="Q24:S24" si="94">Q23</f>
+        <f t="shared" si="93"/>
         <v>-</v>
       </c>
       <c r="R24" t="str">
-        <f t="shared" si="94"/>
+        <f t="shared" ref="R24:T24" si="94">R23</f>
         <v>-</v>
       </c>
       <c r="S24" t="str">
@@ -3974,16 +4035,17 @@
         <v>-</v>
       </c>
       <c r="T24" t="str">
-        <f t="shared" ref="T24:U24" si="95">T23</f>
+        <f t="shared" si="94"/>
         <v>-</v>
       </c>
       <c r="U24" t="str">
+        <f t="shared" ref="U24:V24" si="95">U23</f>
+        <v>-</v>
+      </c>
+      <c r="V24" t="str">
         <f t="shared" si="95"/>
         <v>-</v>
       </c>
-      <c r="V24">
-        <v>1</v>
-      </c>
       <c r="W24">
         <v>1</v>
       </c>
@@ -4006,11 +4068,11 @@
         <v>1</v>
       </c>
       <c r="AD24">
+        <v>1</v>
+      </c>
+      <c r="AE24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AE24">
-        <v>1</v>
-      </c>
       <c r="AF24">
         <v>1</v>
       </c>
@@ -4027,11 +4089,14 @@
         <v>1</v>
       </c>
       <c r="AK24">
+        <v>1</v>
+      </c>
+      <c r="AL24">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -4042,43 +4107,42 @@
       <c r="C25" t="b">
         <v>0</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E25" t="str">
+      <c r="F25" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F25" t="str">
-        <f t="shared" ref="F25" si="96">F24</f>
-        <v>-</v>
-      </c>
       <c r="G25" t="str">
+        <f t="shared" ref="G25" si="96">G24</f>
+        <v>-</v>
+      </c>
+      <c r="H25" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H25" t="str">
+      <c r="I25" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I25" t="str">
+      <c r="J25" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J25" t="str">
+      <c r="K25" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K25" t="str">
-        <f t="shared" ref="K25" si="97">K24</f>
-        <v>-</v>
-      </c>
       <c r="L25" t="str">
-        <f t="shared" ref="L25:P25" si="98">L24</f>
+        <f t="shared" ref="L25" si="97">L24</f>
         <v>-</v>
       </c>
       <c r="M25" t="str">
-        <f t="shared" si="98"/>
+        <f t="shared" ref="M25:Q25" si="98">M24</f>
         <v>-</v>
       </c>
       <c r="N25" t="str">
@@ -4094,11 +4158,11 @@
         <v>-</v>
       </c>
       <c r="Q25" t="str">
-        <f t="shared" ref="Q25:S25" si="99">Q24</f>
+        <f t="shared" si="98"/>
         <v>-</v>
       </c>
       <c r="R25" t="str">
-        <f t="shared" si="99"/>
+        <f t="shared" ref="R25:T25" si="99">R24</f>
         <v>-</v>
       </c>
       <c r="S25" t="str">
@@ -4106,16 +4170,17 @@
         <v>-</v>
       </c>
       <c r="T25" t="str">
-        <f t="shared" ref="T25:U25" si="100">T24</f>
+        <f t="shared" si="99"/>
         <v>-</v>
       </c>
       <c r="U25" t="str">
+        <f t="shared" ref="U25:V25" si="100">U24</f>
+        <v>-</v>
+      </c>
+      <c r="V25" t="str">
         <f t="shared" si="100"/>
         <v>-</v>
       </c>
-      <c r="V25">
-        <v>1</v>
-      </c>
       <c r="W25">
         <v>1</v>
       </c>
@@ -4141,11 +4206,11 @@
         <v>1</v>
       </c>
       <c r="AE25">
+        <v>1</v>
+      </c>
+      <c r="AF25">
         <v>0.9</v>
       </c>
-      <c r="AF25">
-        <v>1</v>
-      </c>
       <c r="AG25">
         <v>1</v>
       </c>
@@ -4159,11 +4224,14 @@
         <v>1</v>
       </c>
       <c r="AK25">
+        <v>1</v>
+      </c>
+      <c r="AL25">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -4174,43 +4242,42 @@
       <c r="C26" t="b">
         <v>0</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E26" t="str">
+      <c r="F26" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F26" t="str">
-        <f t="shared" ref="F26" si="101">F25</f>
-        <v>-</v>
-      </c>
       <c r="G26" t="str">
+        <f t="shared" ref="G26" si="101">G25</f>
+        <v>-</v>
+      </c>
+      <c r="H26" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H26" t="str">
+      <c r="I26" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I26" t="str">
+      <c r="J26" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J26" t="str">
+      <c r="K26" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K26" t="str">
-        <f t="shared" ref="K26" si="102">K25</f>
-        <v>-</v>
-      </c>
       <c r="L26" t="str">
-        <f t="shared" ref="L26:P26" si="103">L25</f>
+        <f t="shared" ref="L26" si="102">L25</f>
         <v>-</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" si="103"/>
+        <f t="shared" ref="M26:Q26" si="103">M25</f>
         <v>-</v>
       </c>
       <c r="N26" t="str">
@@ -4226,11 +4293,11 @@
         <v>-</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" ref="Q26:S26" si="104">Q25</f>
+        <f t="shared" si="103"/>
         <v>-</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" si="104"/>
+        <f t="shared" ref="R26:T26" si="104">R25</f>
         <v>-</v>
       </c>
       <c r="S26" t="str">
@@ -4238,16 +4305,17 @@
         <v>-</v>
       </c>
       <c r="T26" t="str">
-        <f t="shared" ref="T26:U26" si="105">T25</f>
+        <f t="shared" si="104"/>
         <v>-</v>
       </c>
       <c r="U26" t="str">
+        <f t="shared" ref="U26:V26" si="105">U25</f>
+        <v>-</v>
+      </c>
+      <c r="V26" t="str">
         <f t="shared" si="105"/>
         <v>-</v>
       </c>
-      <c r="V26">
-        <v>1</v>
-      </c>
       <c r="W26">
         <v>1</v>
       </c>
@@ -4273,11 +4341,11 @@
         <v>1</v>
       </c>
       <c r="AE26">
+        <v>1</v>
+      </c>
+      <c r="AF26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AF26">
-        <v>1</v>
-      </c>
       <c r="AG26">
         <v>1</v>
       </c>
@@ -4291,11 +4359,14 @@
         <v>1</v>
       </c>
       <c r="AK26">
+        <v>1</v>
+      </c>
+      <c r="AL26">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -4306,43 +4377,42 @@
       <c r="C27" t="b">
         <v>0</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E27" t="str">
+      <c r="F27" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F27" t="str">
-        <f t="shared" ref="F27" si="106">F26</f>
-        <v>-</v>
-      </c>
       <c r="G27" t="str">
+        <f t="shared" ref="G27" si="106">G26</f>
+        <v>-</v>
+      </c>
+      <c r="H27" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H27" t="str">
+      <c r="I27" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I27" t="str">
+      <c r="J27" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J27" t="str">
+      <c r="K27" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K27" t="str">
-        <f t="shared" ref="K27" si="107">K26</f>
-        <v>-</v>
-      </c>
       <c r="L27" t="str">
-        <f t="shared" ref="L27:P27" si="108">L26</f>
+        <f t="shared" ref="L27" si="107">L26</f>
         <v>-</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" si="108"/>
+        <f t="shared" ref="M27:Q27" si="108">M26</f>
         <v>-</v>
       </c>
       <c r="N27" t="str">
@@ -4358,11 +4428,11 @@
         <v>-</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" ref="Q27:S27" si="109">Q26</f>
+        <f t="shared" si="108"/>
         <v>-</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="109"/>
+        <f t="shared" ref="R27:T27" si="109">R26</f>
         <v>-</v>
       </c>
       <c r="S27" t="str">
@@ -4370,16 +4440,17 @@
         <v>-</v>
       </c>
       <c r="T27" t="str">
-        <f t="shared" ref="T27:U27" si="110">T26</f>
+        <f t="shared" si="109"/>
         <v>-</v>
       </c>
       <c r="U27" t="str">
+        <f t="shared" ref="U27:V27" si="110">U26</f>
+        <v>-</v>
+      </c>
+      <c r="V27" t="str">
         <f t="shared" si="110"/>
         <v>-</v>
       </c>
-      <c r="V27">
-        <v>1</v>
-      </c>
       <c r="W27">
         <v>1</v>
       </c>
@@ -4408,11 +4479,11 @@
         <v>1</v>
       </c>
       <c r="AF27">
+        <v>1</v>
+      </c>
+      <c r="AG27">
         <v>0.9</v>
       </c>
-      <c r="AG27">
-        <v>1</v>
-      </c>
       <c r="AH27">
         <v>1</v>
       </c>
@@ -4423,11 +4494,14 @@
         <v>1</v>
       </c>
       <c r="AK27">
+        <v>1</v>
+      </c>
+      <c r="AL27">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -4438,43 +4512,42 @@
       <c r="C28" t="b">
         <v>0</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E28" t="str">
+      <c r="F28" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F28" t="str">
-        <f t="shared" ref="F28" si="111">F27</f>
-        <v>-</v>
-      </c>
       <c r="G28" t="str">
+        <f t="shared" ref="G28" si="111">G27</f>
+        <v>-</v>
+      </c>
+      <c r="H28" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H28" t="str">
+      <c r="I28" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I28" t="str">
+      <c r="J28" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J28" t="str">
+      <c r="K28" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K28" t="str">
-        <f t="shared" ref="K28" si="112">K27</f>
-        <v>-</v>
-      </c>
       <c r="L28" t="str">
-        <f t="shared" ref="L28:P28" si="113">L27</f>
+        <f t="shared" ref="L28" si="112">L27</f>
         <v>-</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" si="113"/>
+        <f t="shared" ref="M28:Q28" si="113">M27</f>
         <v>-</v>
       </c>
       <c r="N28" t="str">
@@ -4490,11 +4563,11 @@
         <v>-</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" ref="Q28:S28" si="114">Q27</f>
+        <f t="shared" si="113"/>
         <v>-</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" si="114"/>
+        <f t="shared" ref="R28:T28" si="114">R27</f>
         <v>-</v>
       </c>
       <c r="S28" t="str">
@@ -4502,16 +4575,17 @@
         <v>-</v>
       </c>
       <c r="T28" t="str">
-        <f t="shared" ref="T28:U28" si="115">T27</f>
+        <f t="shared" si="114"/>
         <v>-</v>
       </c>
       <c r="U28" t="str">
+        <f t="shared" ref="U28:V28" si="115">U27</f>
+        <v>-</v>
+      </c>
+      <c r="V28" t="str">
         <f t="shared" si="115"/>
         <v>-</v>
       </c>
-      <c r="V28">
-        <v>1</v>
-      </c>
       <c r="W28">
         <v>1</v>
       </c>
@@ -4540,11 +4614,11 @@
         <v>1</v>
       </c>
       <c r="AF28">
+        <v>1</v>
+      </c>
+      <c r="AG28">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AG28">
-        <v>1</v>
-      </c>
       <c r="AH28">
         <v>1</v>
       </c>
@@ -4555,11 +4629,14 @@
         <v>1</v>
       </c>
       <c r="AK28">
+        <v>1</v>
+      </c>
+      <c r="AL28">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -4570,43 +4647,42 @@
       <c r="C29" t="b">
         <v>0</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E29" t="str">
+      <c r="F29" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F29" t="str">
-        <f t="shared" ref="F29" si="116">F28</f>
-        <v>-</v>
-      </c>
       <c r="G29" t="str">
+        <f t="shared" ref="G29" si="116">G28</f>
+        <v>-</v>
+      </c>
+      <c r="H29" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H29" t="str">
+      <c r="I29" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I29" t="str">
+      <c r="J29" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J29" t="str">
+      <c r="K29" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K29" t="str">
-        <f t="shared" ref="K29" si="117">K28</f>
-        <v>-</v>
-      </c>
       <c r="L29" t="str">
-        <f t="shared" ref="L29:P29" si="118">L28</f>
+        <f t="shared" ref="L29" si="117">L28</f>
         <v>-</v>
       </c>
       <c r="M29" t="str">
-        <f t="shared" si="118"/>
+        <f t="shared" ref="M29:Q29" si="118">M28</f>
         <v>-</v>
       </c>
       <c r="N29" t="str">
@@ -4622,11 +4698,11 @@
         <v>-</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" ref="Q29:S29" si="119">Q28</f>
+        <f t="shared" si="118"/>
         <v>-</v>
       </c>
       <c r="R29" t="str">
-        <f t="shared" si="119"/>
+        <f t="shared" ref="R29:T29" si="119">R28</f>
         <v>-</v>
       </c>
       <c r="S29" t="str">
@@ -4634,16 +4710,17 @@
         <v>-</v>
       </c>
       <c r="T29" t="str">
-        <f t="shared" ref="T29:U29" si="120">T28</f>
+        <f t="shared" si="119"/>
         <v>-</v>
       </c>
       <c r="U29" t="str">
+        <f t="shared" ref="U29:V29" si="120">U28</f>
+        <v>-</v>
+      </c>
+      <c r="V29" t="str">
         <f t="shared" si="120"/>
         <v>-</v>
       </c>
-      <c r="V29">
-        <v>1</v>
-      </c>
       <c r="W29">
         <v>1</v>
       </c>
@@ -4675,11 +4752,11 @@
         <v>1</v>
       </c>
       <c r="AG29">
+        <v>1</v>
+      </c>
+      <c r="AH29">
         <v>0.9</v>
       </c>
-      <c r="AH29">
-        <v>1</v>
-      </c>
       <c r="AI29">
         <v>1</v>
       </c>
@@ -4687,11 +4764,14 @@
         <v>1</v>
       </c>
       <c r="AK29">
+        <v>1</v>
+      </c>
+      <c r="AL29">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -4702,43 +4782,42 @@
       <c r="C30" t="b">
         <v>0</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E30" t="str">
+      <c r="F30" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F30" t="str">
-        <f t="shared" ref="F30" si="121">F29</f>
-        <v>-</v>
-      </c>
       <c r="G30" t="str">
+        <f t="shared" ref="G30" si="121">G29</f>
+        <v>-</v>
+      </c>
+      <c r="H30" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
-      <c r="H30" t="str">
+      <c r="I30" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
       </c>
-      <c r="I30" t="str">
+      <c r="J30" t="str">
         <f t="shared" si="9"/>
         <v>-</v>
       </c>
-      <c r="J30" t="str">
+      <c r="K30" t="str">
         <f t="shared" si="10"/>
         <v>-</v>
       </c>
-      <c r="K30" t="str">
-        <f t="shared" ref="K30" si="122">K29</f>
-        <v>-</v>
-      </c>
       <c r="L30" t="str">
-        <f t="shared" ref="L30:P30" si="123">L29</f>
+        <f t="shared" ref="L30" si="122">L29</f>
         <v>-</v>
       </c>
       <c r="M30" t="str">
-        <f t="shared" si="123"/>
+        <f t="shared" ref="M30:Q30" si="123">M29</f>
         <v>-</v>
       </c>
       <c r="N30" t="str">
@@ -4754,11 +4833,11 @@
         <v>-</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:S30" si="124">Q29</f>
+        <f t="shared" si="123"/>
         <v>-</v>
       </c>
       <c r="R30" t="str">
-        <f t="shared" si="124"/>
+        <f t="shared" ref="R30:T30" si="124">R29</f>
         <v>-</v>
       </c>
       <c r="S30" t="str">
@@ -4766,16 +4845,17 @@
         <v>-</v>
       </c>
       <c r="T30" t="str">
-        <f t="shared" ref="T30:U34" si="125">T29</f>
+        <f t="shared" si="124"/>
         <v>-</v>
       </c>
       <c r="U30" t="str">
+        <f t="shared" ref="U30:V34" si="125">U29</f>
+        <v>-</v>
+      </c>
+      <c r="V30" t="str">
         <f t="shared" si="125"/>
         <v>-</v>
       </c>
-      <c r="V30">
-        <v>1</v>
-      </c>
       <c r="W30">
         <v>1</v>
       </c>
@@ -4807,11 +4887,11 @@
         <v>1</v>
       </c>
       <c r="AG30">
+        <v>1</v>
+      </c>
+      <c r="AH30">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AH30">
-        <v>1</v>
-      </c>
       <c r="AI30">
         <v>1</v>
       </c>
@@ -4819,11 +4899,14 @@
         <v>1</v>
       </c>
       <c r="AK30">
+        <v>1</v>
+      </c>
+      <c r="AL30">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -4834,23 +4917,22 @@
       <c r="C31" t="b">
         <v>0</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="E31" t="str">
-        <f>E$5</f>
-        <v>-</v>
       </c>
       <c r="F31" t="str">
         <f>F$5</f>
         <v>-</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" ref="E31:AK40" si="126">G$5</f>
+        <f>G$5</f>
         <v>-</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="126"/>
+        <f t="shared" ref="F31:AL40" si="126">H$5</f>
         <v>-</v>
       </c>
       <c r="I31" t="str">
@@ -4870,11 +4952,11 @@
         <v>-</v>
       </c>
       <c r="M31" t="str">
-        <f t="shared" ref="M31:P31" si="127">M30</f>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="127"/>
+        <f t="shared" ref="N31:Q31" si="127">N30</f>
         <v>-</v>
       </c>
       <c r="O31" t="str">
@@ -4886,26 +4968,26 @@
         <v>-</v>
       </c>
       <c r="Q31" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
-      </c>
-      <c r="R31">
+        <f t="shared" si="127"/>
+        <v>-</v>
+      </c>
+      <c r="R31" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
+      </c>
+      <c r="S31">
         <v>200</v>
       </c>
-      <c r="S31" t="b">
-        <v>1</v>
-      </c>
-      <c r="T31" t="str">
-        <f t="shared" si="125"/>
-        <v>-</v>
+      <c r="T31" t="b">
+        <v>1</v>
       </c>
       <c r="U31" t="str">
         <f t="shared" si="125"/>
         <v>-</v>
       </c>
-      <c r="V31">
-        <f t="shared" si="126"/>
-        <v>1</v>
+      <c r="V31" t="str">
+        <f t="shared" si="125"/>
+        <v>-</v>
       </c>
       <c r="W31">
         <f t="shared" si="126"/>
@@ -4953,7 +5035,7 @@
       </c>
       <c r="AH31">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI31">
         <f t="shared" si="126"/>
@@ -4967,8 +5049,12 @@
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
+      <c r="AL31">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -4979,21 +5065,20 @@
       <c r="C32" t="b">
         <v>0</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E32" t="str">
-        <f t="shared" ref="E32:F34" si="128">E$5</f>
-        <v>-</v>
-      </c>
       <c r="F32" t="str">
+        <f t="shared" ref="F32:G34" si="128">F$5</f>
+        <v>-</v>
+      </c>
+      <c r="G32" t="str">
         <f t="shared" si="128"/>
         <v>-</v>
       </c>
-      <c r="G32" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
-      </c>
       <c r="H32" t="str">
         <f t="shared" si="126"/>
         <v>-</v>
@@ -5015,11 +5100,11 @@
         <v>-</v>
       </c>
       <c r="M32" t="str">
-        <f t="shared" ref="M32:P32" si="129">M31</f>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" si="129"/>
+        <f t="shared" ref="N32:Q32" si="129">N31</f>
         <v>-</v>
       </c>
       <c r="O32" t="str">
@@ -5031,26 +5116,26 @@
         <v>-</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
-      </c>
-      <c r="R32">
+        <f t="shared" si="129"/>
+        <v>-</v>
+      </c>
+      <c r="R32" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
+      </c>
+      <c r="S32">
         <v>800</v>
       </c>
-      <c r="S32" t="b">
-        <v>1</v>
-      </c>
-      <c r="T32" t="str">
-        <f t="shared" si="125"/>
-        <v>-</v>
+      <c r="T32" t="b">
+        <v>1</v>
       </c>
       <c r="U32" t="str">
         <f t="shared" si="125"/>
         <v>-</v>
       </c>
-      <c r="V32">
-        <f t="shared" si="126"/>
-        <v>1</v>
+      <c r="V32" t="str">
+        <f t="shared" si="125"/>
+        <v>-</v>
       </c>
       <c r="W32">
         <f t="shared" si="126"/>
@@ -5098,7 +5183,7 @@
       </c>
       <c r="AH32">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI32">
         <f t="shared" si="126"/>
@@ -5112,8 +5197,12 @@
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
+      <c r="AL32">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -5124,19 +5213,18 @@
       <c r="C33" t="b">
         <v>0</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="E33" t="str">
-        <f t="shared" si="128"/>
-        <v>-</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="128"/>
         <v>-</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="126"/>
+        <f t="shared" si="128"/>
         <v>-</v>
       </c>
       <c r="H33" t="str">
@@ -5160,11 +5248,11 @@
         <v>-</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" ref="M33:P33" si="130">M32</f>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="130"/>
+        <f t="shared" ref="N33:Q33" si="130">N32</f>
         <v>-</v>
       </c>
       <c r="O33" t="str">
@@ -5176,26 +5264,26 @@
         <v>-</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
-      </c>
-      <c r="R33">
+        <f t="shared" si="130"/>
+        <v>-</v>
+      </c>
+      <c r="R33" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
+      </c>
+      <c r="S33">
         <v>1200</v>
       </c>
-      <c r="S33" t="b">
-        <v>1</v>
-      </c>
-      <c r="T33" t="str">
-        <f t="shared" si="125"/>
-        <v>-</v>
+      <c r="T33" t="b">
+        <v>1</v>
       </c>
       <c r="U33" t="str">
         <f t="shared" si="125"/>
         <v>-</v>
       </c>
-      <c r="V33">
-        <f t="shared" si="126"/>
-        <v>1</v>
+      <c r="V33" t="str">
+        <f t="shared" si="125"/>
+        <v>-</v>
       </c>
       <c r="W33">
         <f t="shared" si="126"/>
@@ -5243,7 +5331,7 @@
       </c>
       <c r="AH33">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI33">
         <f t="shared" si="126"/>
@@ -5257,8 +5345,12 @@
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
+      <c r="AL33">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -5269,19 +5361,18 @@
       <c r="C34" t="b">
         <v>0</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E34" t="str">
-        <f t="shared" si="128"/>
-        <v>-</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="128"/>
         <v>-</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="126"/>
+        <f t="shared" si="128"/>
         <v>-</v>
       </c>
       <c r="H34" t="str">
@@ -5305,11 +5396,11 @@
         <v>-</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" ref="M34:P34" si="131">M33</f>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="131"/>
+        <f t="shared" ref="N34:Q34" si="131">N33</f>
         <v>-</v>
       </c>
       <c r="O34" t="str">
@@ -5321,26 +5412,26 @@
         <v>-</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
-      </c>
-      <c r="R34">
+        <f t="shared" si="131"/>
+        <v>-</v>
+      </c>
+      <c r="R34" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
+      </c>
+      <c r="S34">
         <v>1600</v>
       </c>
-      <c r="S34" t="b">
-        <v>1</v>
-      </c>
-      <c r="T34" t="str">
-        <f t="shared" si="125"/>
-        <v>-</v>
+      <c r="T34" t="b">
+        <v>1</v>
       </c>
       <c r="U34" t="str">
         <f t="shared" si="125"/>
         <v>-</v>
       </c>
-      <c r="V34">
-        <f t="shared" si="126"/>
-        <v>1</v>
+      <c r="V34" t="str">
+        <f t="shared" si="125"/>
+        <v>-</v>
       </c>
       <c r="W34">
         <f t="shared" si="126"/>
@@ -5388,7 +5479,7 @@
       </c>
       <c r="AH34">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI34">
         <f t="shared" si="126"/>
@@ -5402,8 +5493,12 @@
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
+      <c r="AL34">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -5414,21 +5509,20 @@
       <c r="C35" t="b">
         <v>1</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E35" t="b">
-        <v>1</v>
-      </c>
       <c r="F35" t="b">
         <v>1</v>
       </c>
       <c r="G35" t="b">
         <v>1</v>
       </c>
-      <c r="H35" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
+      <c r="H35" t="b">
+        <v>1</v>
       </c>
       <c r="I35" t="str">
         <f t="shared" si="126"/>
@@ -5447,11 +5541,11 @@
         <v>-</v>
       </c>
       <c r="M35" t="str">
-        <f t="shared" ref="M35:P35" si="132">M34</f>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="132"/>
+        <f t="shared" ref="N35:Q35" si="132">N34</f>
         <v>-</v>
       </c>
       <c r="O35" t="str">
@@ -5463,7 +5557,7 @@
         <v>-</v>
       </c>
       <c r="Q35" t="str">
-        <f t="shared" si="126"/>
+        <f t="shared" si="132"/>
         <v>-</v>
       </c>
       <c r="R35" t="str">
@@ -5482,9 +5576,9 @@
         <f t="shared" si="126"/>
         <v>-</v>
       </c>
-      <c r="V35">
-        <f t="shared" si="126"/>
-        <v>1</v>
+      <c r="V35" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
       </c>
       <c r="W35">
         <f t="shared" si="126"/>
@@ -5532,7 +5626,7 @@
       </c>
       <c r="AH35">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI35">
         <f t="shared" si="126"/>
@@ -5546,8 +5640,12 @@
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
+      <c r="AL35">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -5558,21 +5656,20 @@
       <c r="C36" t="b">
         <v>1</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E36" t="b">
-        <v>1</v>
-      </c>
       <c r="F36" t="b">
         <v>1</v>
       </c>
       <c r="G36" t="b">
-        <v>0</v>
-      </c>
-      <c r="H36" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
+        <v>1</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
       </c>
       <c r="I36" t="str">
         <f t="shared" si="126"/>
@@ -5591,11 +5688,11 @@
         <v>-</v>
       </c>
       <c r="M36" t="str">
-        <f t="shared" ref="M36:P36" si="133">M35</f>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="133"/>
+        <f t="shared" ref="N36:Q36" si="133">N35</f>
         <v>-</v>
       </c>
       <c r="O36" t="str">
@@ -5607,7 +5704,7 @@
         <v>-</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" si="126"/>
+        <f t="shared" si="133"/>
         <v>-</v>
       </c>
       <c r="R36" t="str">
@@ -5626,9 +5723,9 @@
         <f t="shared" si="126"/>
         <v>-</v>
       </c>
-      <c r="V36">
-        <f t="shared" si="126"/>
-        <v>1</v>
+      <c r="V36" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
       </c>
       <c r="W36">
         <f t="shared" si="126"/>
@@ -5676,7 +5773,7 @@
       </c>
       <c r="AH36">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI36">
         <f t="shared" si="126"/>
@@ -5690,8 +5787,12 @@
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
+      <c r="AL36">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -5702,21 +5803,20 @@
       <c r="C37" t="b">
         <v>1</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E37" t="b">
-        <v>0</v>
-      </c>
       <c r="F37" t="b">
         <v>0</v>
       </c>
       <c r="G37" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
       </c>
       <c r="I37" t="str">
         <f t="shared" si="126"/>
@@ -5735,11 +5835,11 @@
         <v>-</v>
       </c>
       <c r="M37" t="str">
-        <f t="shared" ref="M37:P37" si="134">M36</f>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="134"/>
+        <f t="shared" ref="N37:Q37" si="134">N36</f>
         <v>-</v>
       </c>
       <c r="O37" t="str">
@@ -5751,7 +5851,7 @@
         <v>-</v>
       </c>
       <c r="Q37" t="str">
-        <f t="shared" si="126"/>
+        <f t="shared" si="134"/>
         <v>-</v>
       </c>
       <c r="R37" t="str">
@@ -5770,9 +5870,9 @@
         <f t="shared" si="126"/>
         <v>-</v>
       </c>
-      <c r="V37">
-        <f t="shared" si="126"/>
-        <v>1</v>
+      <c r="V37" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
       </c>
       <c r="W37">
         <f t="shared" si="126"/>
@@ -5820,7 +5920,7 @@
       </c>
       <c r="AH37">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI37">
         <f t="shared" si="126"/>
@@ -5834,8 +5934,12 @@
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
+      <c r="AL37">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -5846,13 +5950,12 @@
       <c r="C38" t="b">
         <v>0</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E38" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
-      </c>
       <c r="F38" t="str">
         <f t="shared" si="126"/>
         <v>-</v>
@@ -5869,23 +5972,23 @@
         <f t="shared" si="126"/>
         <v>-</v>
       </c>
-      <c r="J38" t="b">
-        <v>1</v>
-      </c>
-      <c r="K38" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
+      <c r="J38" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="M38" t="str">
-        <f t="shared" ref="M38:P38" si="135">M37</f>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="135"/>
+        <f t="shared" ref="N38:Q38" si="135">N37</f>
         <v>-</v>
       </c>
       <c r="O38" t="str">
@@ -5897,7 +6000,7 @@
         <v>-</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" si="126"/>
+        <f t="shared" si="135"/>
         <v>-</v>
       </c>
       <c r="R38" t="str">
@@ -5916,9 +6019,9 @@
         <f t="shared" si="126"/>
         <v>-</v>
       </c>
-      <c r="V38">
-        <f t="shared" si="126"/>
-        <v>1</v>
+      <c r="V38" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
       </c>
       <c r="W38">
         <f t="shared" si="126"/>
@@ -5966,7 +6069,7 @@
       </c>
       <c r="AH38">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI38">
         <f t="shared" si="126"/>
@@ -5980,8 +6083,12 @@
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
+      <c r="AL38">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -5992,22 +6099,21 @@
       <c r="C39" t="b">
         <v>1</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E39" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
-      </c>
-      <c r="F39" t="b">
-        <v>1</v>
+      <c r="F39" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
       </c>
       <c r="G39" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="126"/>
@@ -6026,11 +6132,11 @@
         <v>-</v>
       </c>
       <c r="M39" t="str">
-        <f t="shared" ref="M39:P40" si="136">M38</f>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N39" t="str">
-        <f t="shared" si="136"/>
+        <f t="shared" ref="N39:Q40" si="136">N38</f>
         <v>-</v>
       </c>
       <c r="O39" t="str">
@@ -6042,7 +6148,7 @@
         <v>-</v>
       </c>
       <c r="Q39" t="str">
-        <f t="shared" si="126"/>
+        <f t="shared" si="136"/>
         <v>-</v>
       </c>
       <c r="R39" t="str">
@@ -6053,14 +6159,14 @@
         <f t="shared" si="126"/>
         <v>-</v>
       </c>
-      <c r="T39" t="b">
-        <v>1</v>
+      <c r="T39" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
       </c>
       <c r="U39" t="b">
         <v>1</v>
       </c>
-      <c r="V39">
-        <f t="shared" si="126"/>
+      <c r="V39" t="b">
         <v>1</v>
       </c>
       <c r="W39">
@@ -6109,7 +6215,7 @@
       </c>
       <c r="AH39">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI39">
         <f t="shared" si="126"/>
@@ -6123,8 +6229,12 @@
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
+      <c r="AL39">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -6135,22 +6245,21 @@
       <c r="C40" t="b">
         <v>1</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E40" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
-      </c>
-      <c r="F40" t="b">
-        <v>0</v>
+      <c r="F40" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
       </c>
       <c r="G40" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" t="str">
-        <f t="shared" si="126"/>
-        <v>-</v>
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
       </c>
       <c r="I40" t="str">
         <f t="shared" si="126"/>
@@ -6169,7 +6278,7 @@
         <v>-</v>
       </c>
       <c r="M40" t="str">
-        <f t="shared" si="136"/>
+        <f t="shared" si="126"/>
         <v>-</v>
       </c>
       <c r="N40" t="str">
@@ -6185,7 +6294,7 @@
         <v>-</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" si="126"/>
+        <f t="shared" si="136"/>
         <v>-</v>
       </c>
       <c r="R40" t="str">
@@ -6196,14 +6305,14 @@
         <f t="shared" si="126"/>
         <v>-</v>
       </c>
-      <c r="T40" t="b">
-        <v>1</v>
+      <c r="T40" t="str">
+        <f t="shared" si="126"/>
+        <v>-</v>
       </c>
       <c r="U40" t="b">
         <v>1</v>
       </c>
-      <c r="V40">
-        <f t="shared" si="126"/>
+      <c r="V40" t="b">
         <v>1</v>
       </c>
       <c r="W40">
@@ -6252,7 +6361,7 @@
       </c>
       <c r="AH40">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI40">
         <f t="shared" si="126"/>
@@ -6263,19 +6372,23 @@
         <v>0</v>
       </c>
       <c r="AK40">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
+      <c r="AL40">
         <f t="shared" si="126"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D4:AK4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
+  <autoFilter ref="E4:AL4" xr:uid="{74BD5C81-DA63-4249-A1B4-6F29577A4105}"/>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="B1:C1048576">
+  <conditionalFormatting sqref="B1:D1048576">
     <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:T1 V1:XFD1">
+  <conditionalFormatting sqref="A1:U1 W1:XFD1">
     <cfRule type="cellIs" dxfId="7" priority="43" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
@@ -6289,18 +6402,18 @@
       <formula>NOT(ISERROR(SEARCH("saa",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U1">
+  <conditionalFormatting sqref="V1">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"sav"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="sam">
-      <formula>NOT(ISERROR(SEARCH("sam",U1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("sam",V1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="sap">
-      <formula>NOT(ISERROR(SEARCH("sap",U1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("sap",V1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="saa">
-      <formula>NOT(ISERROR(SEARCH("saa",U1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("saa",V1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6317,35 +6430,35 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="145.109375" customWidth="1"/>
+    <col min="1" max="1" width="145.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="10"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
     </row>
   </sheetData>

</xml_diff>